<commit_message>
new updates to project
</commit_message>
<xml_diff>
--- a/Excel Files/life_table.xlsx
+++ b/Excel Files/life_table.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-440" windowWidth="25600" windowHeight="16000"/>
+    <workbookView xWindow="0" yWindow="-440" windowWidth="25600" windowHeight="16000" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="life table" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="75">
   <si>
     <t>Year</t>
   </si>
@@ -367,6 +367,15 @@
       </rPr>
       <t xml:space="preserve"> (chance of dying this year)</t>
     </r>
+  </si>
+  <si>
+    <t>Data N/A</t>
+  </si>
+  <si>
+    <t>number of females for a male</t>
+  </si>
+  <si>
+    <t>&gt; 1</t>
   </si>
 </sst>
 </file>
@@ -806,7 +815,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -2371,10 +2380,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q41"/>
+  <dimension ref="A1:R41"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="O37" sqref="O37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2387,7 +2396,7 @@
     <col min="15" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" customHeight="1">
+    <row r="1" spans="1:18" ht="30" customHeight="1">
       <c r="A1" s="10" t="s">
         <v>32</v>
       </c>
@@ -2409,7 +2418,7 @@
       <c r="P1" s="10"/>
       <c r="Q1" s="10"/>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:18">
       <c r="A2" s="10" t="s">
         <v>23</v>
       </c>
@@ -2433,7 +2442,7 @@
       <c r="P2" s="10"/>
       <c r="Q2" s="10"/>
     </row>
-    <row r="3" spans="1:17" ht="70">
+    <row r="3" spans="1:18" ht="70">
       <c r="A3" s="2" t="s">
         <v>25</v>
       </c>
@@ -2471,7 +2480,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:18">
       <c r="A4" s="2" t="s">
         <v>26</v>
       </c>
@@ -2493,20 +2502,23 @@
       <c r="M4">
         <v>1</v>
       </c>
-      <c r="N4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q4" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17">
+      <c r="N4" s="2">
+        <v>0</v>
+      </c>
+      <c r="O4" s="2">
+        <v>0</v>
+      </c>
+      <c r="P4" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>0</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
       <c r="D5" s="10" t="s">
         <v>47</v>
       </c>
@@ -2522,20 +2534,23 @@
       <c r="M5">
         <v>2</v>
       </c>
-      <c r="N5" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="P5" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q5" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17">
+      <c r="N5" s="2">
+        <v>0</v>
+      </c>
+      <c r="O5" s="2">
+        <v>0</v>
+      </c>
+      <c r="P5" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>0</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
       <c r="D6" s="10"/>
       <c r="E6">
         <v>3</v>
@@ -2547,20 +2562,23 @@
       <c r="M6">
         <v>3</v>
       </c>
-      <c r="N6" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="O6" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="P6" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q6" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17">
+      <c r="N6" s="2">
+        <v>0</v>
+      </c>
+      <c r="O6" s="2">
+        <v>0</v>
+      </c>
+      <c r="P6" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>0</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
       <c r="D7" s="10"/>
       <c r="E7">
         <v>4</v>
@@ -2585,7 +2603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="15" customHeight="1">
+    <row r="8" spans="1:18" ht="15" customHeight="1">
       <c r="D8" s="10" t="s">
         <v>50</v>
       </c>
@@ -2614,7 +2632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:18">
       <c r="D9" s="10"/>
       <c r="E9">
         <v>6</v>
@@ -2639,7 +2657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="15" customHeight="1">
+    <row r="10" spans="1:18" ht="15" customHeight="1">
       <c r="D10" s="10" t="s">
         <v>49</v>
       </c>
@@ -2668,7 +2686,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:18">
       <c r="D11" s="10"/>
       <c r="E11">
         <v>8</v>
@@ -2693,7 +2711,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:18">
       <c r="D12" s="10"/>
       <c r="E12">
         <v>9</v>
@@ -2718,7 +2736,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="15" customHeight="1">
+    <row r="13" spans="1:18" ht="15" customHeight="1">
       <c r="D13" s="10" t="s">
         <v>51</v>
       </c>
@@ -2747,7 +2765,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:18">
       <c r="D14" s="10"/>
       <c r="E14">
         <v>11</v>
@@ -2772,7 +2790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:18">
       <c r="D15" s="10"/>
       <c r="E15">
         <v>12</v>
@@ -2797,7 +2815,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:18">
       <c r="D16" s="10"/>
       <c r="E16">
         <v>13</v>
@@ -3234,7 +3252,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="4:17">
+    <row r="33" spans="1:17">
       <c r="D33" s="10"/>
       <c r="E33">
         <v>30</v>
@@ -3259,7 +3277,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="4:17" ht="56">
+    <row r="34" spans="1:17">
+      <c r="A34" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" ht="56">
+      <c r="C35" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="D35" s="10" t="s">
         <v>59</v>
       </c>
@@ -3275,7 +3301,10 @@
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="4:17">
+    <row r="36" spans="1:17">
+      <c r="C36" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="D36" s="5"/>
       <c r="E36" s="5" t="s">
         <v>60</v>
@@ -3290,7 +3319,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="4:17">
+    <row r="37" spans="1:17">
+      <c r="C37" s="2">
+        <v>1</v>
+      </c>
       <c r="E37" s="7" t="s">
         <v>56</v>
       </c>
@@ -3304,7 +3336,10 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="38" spans="4:17">
+    <row r="38" spans="1:17">
+      <c r="C38" s="2">
+        <v>2</v>
+      </c>
       <c r="E38" s="7" t="s">
         <v>57</v>
       </c>
@@ -3318,7 +3353,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="4:17">
+    <row r="39" spans="1:17">
+      <c r="C39" s="2">
+        <v>3</v>
+      </c>
       <c r="E39" s="7" t="s">
         <v>58</v>
       </c>
@@ -3332,10 +3370,10 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="40" spans="4:17">
+    <row r="40" spans="1:17">
       <c r="E40" s="7"/>
     </row>
-    <row r="41" spans="4:17">
+    <row r="41" spans="1:17">
       <c r="E41" s="7"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
continuing to work on loader
</commit_message>
<xml_diff>
--- a/Excel Files/life_table.xlsx
+++ b/Excel Files/life_table.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-440" windowWidth="25600" windowHeight="16000" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="life table" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="70">
   <si>
     <t>Year</t>
   </si>
@@ -151,21 +151,6 @@
       </rPr>
       <t xml:space="preserve"> (chance of giving birth this year)</t>
     </r>
-  </si>
-  <si>
-    <t>Females</t>
-  </si>
-  <si>
-    <t>Chance of emmigrating</t>
-  </si>
-  <si>
-    <t>Age in Years</t>
-  </si>
-  <si>
-    <t>0-30</t>
-  </si>
-  <si>
-    <t>Males</t>
   </si>
   <si>
     <t>Age Class Title</t>
@@ -469,12 +454,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -482,9 +471,6 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -511,9 +497,13 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -815,36 +805,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:15" s="2" customFormat="1" ht="108" customHeight="1">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10" t="s">
+      <c r="B1" s="9"/>
+      <c r="C1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="E1" s="10" t="s">
+      <c r="D1" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="10"/>
+      <c r="J1" s="9"/>
       <c r="K1" s="2" t="s">
         <v>3</v>
       </c>
@@ -868,11 +858,11 @@
       <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
       <c r="I2" t="s">
         <v>1</v>
       </c>
@@ -882,7 +872,7 @@
     </row>
     <row r="3" spans="1:15">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -900,7 +890,7 @@
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="J3">
         <v>1</v>
@@ -919,8 +909,8 @@
       </c>
     </row>
     <row r="4" spans="1:15">
-      <c r="A4" s="11" t="s">
-        <v>47</v>
+      <c r="A4" s="10" t="s">
+        <v>42</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -938,8 +928,8 @@
       <c r="G4" s="1">
         <v>0</v>
       </c>
-      <c r="I4" s="10" t="s">
-        <v>47</v>
+      <c r="I4" s="9" t="s">
+        <v>42</v>
       </c>
       <c r="J4">
         <v>2</v>
@@ -959,7 +949,7 @@
       </c>
     </row>
     <row r="5" spans="1:15">
-      <c r="A5" s="11"/>
+      <c r="A5" s="10"/>
       <c r="B5">
         <v>3</v>
       </c>
@@ -976,7 +966,7 @@
       <c r="G5" s="1">
         <v>0</v>
       </c>
-      <c r="I5" s="10"/>
+      <c r="I5" s="9"/>
       <c r="J5">
         <v>3</v>
       </c>
@@ -995,7 +985,7 @@
       </c>
     </row>
     <row r="6" spans="1:15">
-      <c r="A6" s="11"/>
+      <c r="A6" s="10"/>
       <c r="B6">
         <v>4</v>
       </c>
@@ -1012,7 +1002,7 @@
       <c r="G6" s="1">
         <v>0</v>
       </c>
-      <c r="I6" s="10"/>
+      <c r="I6" s="9"/>
       <c r="J6">
         <v>4</v>
       </c>
@@ -1031,8 +1021,8 @@
       </c>
     </row>
     <row r="7" spans="1:15" ht="15" customHeight="1">
-      <c r="A7" s="10" t="s">
-        <v>48</v>
+      <c r="A7" s="9" t="s">
+        <v>43</v>
       </c>
       <c r="B7">
         <v>5</v>
@@ -1051,8 +1041,8 @@
         <f xml:space="preserve"> E7*F7</f>
         <v>97.76</v>
       </c>
-      <c r="I7" s="10" t="s">
-        <v>50</v>
+      <c r="I7" s="9" t="s">
+        <v>45</v>
       </c>
       <c r="J7">
         <v>5</v>
@@ -1072,7 +1062,7 @@
       </c>
     </row>
     <row r="8" spans="1:15">
-      <c r="A8" s="10"/>
+      <c r="A8" s="9"/>
       <c r="B8">
         <v>6</v>
       </c>
@@ -1090,7 +1080,7 @@
         <f t="shared" ref="G8:G32" si="3" xml:space="preserve"> E8*F8</f>
         <v>95.8048</v>
       </c>
-      <c r="I8" s="10"/>
+      <c r="I8" s="9"/>
       <c r="J8">
         <v>6</v>
       </c>
@@ -1109,7 +1099,7 @@
       </c>
     </row>
     <row r="9" spans="1:15">
-      <c r="A9" s="10"/>
+      <c r="A9" s="9"/>
       <c r="B9">
         <v>7</v>
       </c>
@@ -1127,8 +1117,8 @@
         <f t="shared" si="3"/>
         <v>93.888704000000004</v>
       </c>
-      <c r="I9" s="10" t="s">
-        <v>49</v>
+      <c r="I9" s="9" t="s">
+        <v>44</v>
       </c>
       <c r="J9">
         <v>7</v>
@@ -1148,7 +1138,7 @@
       </c>
     </row>
     <row r="10" spans="1:15">
-      <c r="A10" s="10"/>
+      <c r="A10" s="9"/>
       <c r="B10">
         <v>8</v>
       </c>
@@ -1166,7 +1156,7 @@
         <f t="shared" si="3"/>
         <v>92.010929920000009</v>
       </c>
-      <c r="I10" s="10"/>
+      <c r="I10" s="9"/>
       <c r="J10">
         <v>8</v>
       </c>
@@ -1185,7 +1175,7 @@
       </c>
     </row>
     <row r="11" spans="1:15">
-      <c r="A11" s="10"/>
+      <c r="A11" s="9"/>
       <c r="B11">
         <v>9</v>
       </c>
@@ -1203,7 +1193,7 @@
         <f t="shared" si="3"/>
         <v>90.17071132160001</v>
       </c>
-      <c r="I11" s="10"/>
+      <c r="I11" s="9"/>
       <c r="J11">
         <v>9</v>
       </c>
@@ -1222,8 +1212,8 @@
       </c>
     </row>
     <row r="12" spans="1:15">
-      <c r="A12" s="10" t="s">
-        <v>51</v>
+      <c r="A12" s="9" t="s">
+        <v>46</v>
       </c>
       <c r="B12">
         <v>10</v>
@@ -1242,8 +1232,8 @@
         <f t="shared" si="3"/>
         <v>106.04075651420162</v>
       </c>
-      <c r="I12" s="10" t="s">
-        <v>51</v>
+      <c r="I12" s="9" t="s">
+        <v>46</v>
       </c>
       <c r="J12">
         <v>10</v>
@@ -1263,7 +1253,7 @@
       </c>
     </row>
     <row r="13" spans="1:15">
-      <c r="A13" s="10"/>
+      <c r="A13" s="9"/>
       <c r="B13">
         <v>11</v>
       </c>
@@ -1281,7 +1271,7 @@
         <f t="shared" si="3"/>
         <v>103.38973760134657</v>
       </c>
-      <c r="I13" s="10"/>
+      <c r="I13" s="9"/>
       <c r="J13">
         <v>11</v>
       </c>
@@ -1300,7 +1290,7 @@
       </c>
     </row>
     <row r="14" spans="1:15">
-      <c r="A14" s="10"/>
+      <c r="A14" s="9"/>
       <c r="B14">
         <v>12</v>
       </c>
@@ -1318,7 +1308,7 @@
         <f t="shared" si="3"/>
         <v>100.80499416131291</v>
       </c>
-      <c r="I14" s="10"/>
+      <c r="I14" s="9"/>
       <c r="J14">
         <v>12</v>
       </c>
@@ -1337,7 +1327,7 @@
       </c>
     </row>
     <row r="15" spans="1:15">
-      <c r="A15" s="10"/>
+      <c r="A15" s="9"/>
       <c r="B15">
         <v>13</v>
       </c>
@@ -1355,7 +1345,7 @@
         <f t="shared" si="3"/>
         <v>98.284869307280076</v>
       </c>
-      <c r="I15" s="10"/>
+      <c r="I15" s="9"/>
       <c r="J15">
         <v>13</v>
       </c>
@@ -1374,7 +1364,7 @@
       </c>
     </row>
     <row r="16" spans="1:15">
-      <c r="A16" s="10"/>
+      <c r="A16" s="9"/>
       <c r="B16">
         <v>14</v>
       </c>
@@ -1392,7 +1382,7 @@
         <f t="shared" si="3"/>
         <v>95.827747574598078</v>
       </c>
-      <c r="I16" s="10"/>
+      <c r="I16" s="9"/>
       <c r="J16">
         <v>14</v>
       </c>
@@ -1411,8 +1401,8 @@
       </c>
     </row>
     <row r="17" spans="1:15">
-      <c r="A17" s="10" t="s">
-        <v>52</v>
+      <c r="A17" s="9" t="s">
+        <v>47</v>
       </c>
       <c r="B17">
         <v>15</v>
@@ -1431,8 +1421,8 @@
         <f t="shared" si="3"/>
         <v>109.0040628661053</v>
       </c>
-      <c r="I17" s="10" t="s">
-        <v>52</v>
+      <c r="I17" s="9" t="s">
+        <v>47</v>
       </c>
       <c r="J17">
         <v>15</v>
@@ -1452,7 +1442,7 @@
       </c>
     </row>
     <row r="18" spans="1:15">
-      <c r="A18" s="10"/>
+      <c r="A18" s="9"/>
       <c r="B18">
         <v>16</v>
       </c>
@@ -1470,7 +1460,7 @@
         <f t="shared" si="3"/>
         <v>105.73394098012214</v>
       </c>
-      <c r="I18" s="10"/>
+      <c r="I18" s="9"/>
       <c r="J18">
         <v>16</v>
       </c>
@@ -1489,7 +1479,7 @@
       </c>
     </row>
     <row r="19" spans="1:15">
-      <c r="A19" s="10"/>
+      <c r="A19" s="9"/>
       <c r="B19">
         <v>17</v>
       </c>
@@ -1507,7 +1497,7 @@
         <f t="shared" si="3"/>
         <v>102.56192275071849</v>
       </c>
-      <c r="I19" s="10"/>
+      <c r="I19" s="9"/>
       <c r="J19">
         <v>17</v>
       </c>
@@ -1526,7 +1516,7 @@
       </c>
     </row>
     <row r="20" spans="1:15">
-      <c r="A20" s="10"/>
+      <c r="A20" s="9"/>
       <c r="B20">
         <v>18</v>
       </c>
@@ -1544,7 +1534,7 @@
         <f t="shared" si="3"/>
         <v>99.485065068196931</v>
       </c>
-      <c r="I20" s="10"/>
+      <c r="I20" s="9"/>
       <c r="J20">
         <v>18</v>
       </c>
@@ -1563,7 +1553,7 @@
       </c>
     </row>
     <row r="21" spans="1:15">
-      <c r="A21" s="10"/>
+      <c r="A21" s="9"/>
       <c r="B21">
         <v>19</v>
       </c>
@@ -1581,7 +1571,7 @@
         <f t="shared" si="3"/>
         <v>96.500513116151041</v>
       </c>
-      <c r="I21" s="10"/>
+      <c r="I21" s="9"/>
       <c r="J21">
         <v>19</v>
       </c>
@@ -1600,7 +1590,7 @@
       </c>
     </row>
     <row r="22" spans="1:15">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="9" t="s">
         <v>9</v>
       </c>
       <c r="B22">
@@ -1620,7 +1610,7 @@
         <f t="shared" si="3"/>
         <v>100.29160470285697</v>
       </c>
-      <c r="I22" s="10" t="s">
+      <c r="I22" s="9" t="s">
         <v>9</v>
       </c>
       <c r="J22">
@@ -1641,7 +1631,7 @@
       </c>
     </row>
     <row r="23" spans="1:15">
-      <c r="A23" s="10"/>
+      <c r="A23" s="9"/>
       <c r="B23">
         <v>21</v>
       </c>
@@ -1659,7 +1649,7 @@
         <f t="shared" si="3"/>
         <v>99.288688655828395</v>
       </c>
-      <c r="I23" s="10"/>
+      <c r="I23" s="9"/>
       <c r="J23">
         <v>21</v>
       </c>
@@ -1678,7 +1668,7 @@
       </c>
     </row>
     <row r="24" spans="1:15">
-      <c r="A24" s="10"/>
+      <c r="A24" s="9"/>
       <c r="B24">
         <v>22</v>
       </c>
@@ -1696,7 +1686,7 @@
         <f t="shared" si="3"/>
         <v>98.295801769270113</v>
       </c>
-      <c r="I24" s="10"/>
+      <c r="I24" s="9"/>
       <c r="J24">
         <v>22</v>
       </c>
@@ -1715,7 +1705,7 @@
       </c>
     </row>
     <row r="25" spans="1:15">
-      <c r="A25" s="10"/>
+      <c r="A25" s="9"/>
       <c r="B25">
         <v>23</v>
       </c>
@@ -1733,7 +1723,7 @@
         <f t="shared" si="3"/>
         <v>97.312843751577418</v>
       </c>
-      <c r="I25" s="10"/>
+      <c r="I25" s="9"/>
       <c r="J25">
         <v>23</v>
       </c>
@@ -1752,7 +1742,7 @@
       </c>
     </row>
     <row r="26" spans="1:15">
-      <c r="A26" s="10"/>
+      <c r="A26" s="9"/>
       <c r="B26">
         <v>24</v>
       </c>
@@ -1770,7 +1760,7 @@
         <f t="shared" si="3"/>
         <v>96.339715314061635</v>
       </c>
-      <c r="I26" s="10"/>
+      <c r="I26" s="9"/>
       <c r="J26">
         <v>24</v>
       </c>
@@ -1789,7 +1779,7 @@
       </c>
     </row>
     <row r="27" spans="1:15">
-      <c r="A27" s="10" t="s">
+      <c r="A27" s="9" t="s">
         <v>19</v>
       </c>
       <c r="B27">
@@ -1809,7 +1799,7 @@
         <f t="shared" si="3"/>
         <v>25.433684842912271</v>
       </c>
-      <c r="I27" s="10" t="s">
+      <c r="I27" s="9" t="s">
         <v>19</v>
       </c>
       <c r="J27">
@@ -1830,7 +1820,7 @@
       </c>
     </row>
     <row r="28" spans="1:15">
-      <c r="A28" s="10"/>
+      <c r="A28" s="9"/>
       <c r="B28">
         <v>26</v>
       </c>
@@ -1848,7 +1838,7 @@
         <f t="shared" si="3"/>
         <v>17.803579390038589</v>
       </c>
-      <c r="I28" s="10"/>
+      <c r="I28" s="9"/>
       <c r="J28">
         <v>26</v>
       </c>
@@ -1867,7 +1857,7 @@
       </c>
     </row>
     <row r="29" spans="1:15">
-      <c r="A29" s="10"/>
+      <c r="A29" s="9"/>
       <c r="B29">
         <v>27</v>
       </c>
@@ -1885,7 +1875,7 @@
         <f t="shared" si="3"/>
         <v>12.462505573027014</v>
       </c>
-      <c r="I29" s="10"/>
+      <c r="I29" s="9"/>
       <c r="J29">
         <v>27</v>
       </c>
@@ -1904,7 +1894,7 @@
       </c>
     </row>
     <row r="30" spans="1:15">
-      <c r="A30" s="10"/>
+      <c r="A30" s="9"/>
       <c r="B30">
         <v>28</v>
       </c>
@@ -1922,7 +1912,7 @@
         <f t="shared" si="3"/>
         <v>8.7237539011189096</v>
       </c>
-      <c r="I30" s="10"/>
+      <c r="I30" s="9"/>
       <c r="J30">
         <v>28</v>
       </c>
@@ -1941,7 +1931,7 @@
       </c>
     </row>
     <row r="31" spans="1:15">
-      <c r="A31" s="10"/>
+      <c r="A31" s="9"/>
       <c r="B31">
         <v>29</v>
       </c>
@@ -1959,7 +1949,7 @@
         <f t="shared" si="3"/>
         <v>6.1066277307832371</v>
       </c>
-      <c r="I31" s="10"/>
+      <c r="I31" s="9"/>
       <c r="J31">
         <v>29</v>
       </c>
@@ -1978,7 +1968,7 @@
       </c>
     </row>
     <row r="32" spans="1:15">
-      <c r="A32" s="10"/>
+      <c r="A32" s="9"/>
       <c r="B32">
         <v>30</v>
       </c>
@@ -1996,7 +1986,7 @@
         <f t="shared" si="3"/>
         <v>4.2746394115482662</v>
       </c>
-      <c r="I32" s="10"/>
+      <c r="I32" s="9"/>
       <c r="J32">
         <v>30</v>
       </c>
@@ -2016,10 +2006,10 @@
     </row>
     <row r="33" spans="1:15">
       <c r="A33" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B33" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="G33">
         <f xml:space="preserve"> SUM(G7:G32)</f>
@@ -2211,145 +2201,140 @@
       </c>
     </row>
     <row r="41" spans="1:15" ht="43.5" customHeight="1">
-      <c r="B41" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="C41" s="10"/>
-      <c r="D41" s="10"/>
-      <c r="E41" s="10"/>
-      <c r="J41" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="K41" s="10"/>
-      <c r="L41" s="10"/>
-      <c r="M41" s="10"/>
+      <c r="B41" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C41" s="9"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
+      <c r="J41" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="K41" s="9"/>
+      <c r="L41" s="9"/>
+      <c r="M41" s="9"/>
     </row>
     <row r="42" spans="1:15" ht="56">
       <c r="B42" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="43" spans="1:15">
       <c r="B43" t="s">
-        <v>60</v>
-      </c>
-      <c r="C43" s="8">
+        <v>55</v>
+      </c>
+      <c r="C43" s="7">
         <v>1.2</v>
       </c>
       <c r="J43" t="s">
-        <v>60</v>
-      </c>
-      <c r="K43" s="8">
+        <v>55</v>
+      </c>
+      <c r="K43" s="7">
         <v>0.85</v>
       </c>
     </row>
     <row r="44" spans="1:15">
-      <c r="B44" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="C44" s="8">
+      <c r="B44" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C44" s="7">
         <v>1.1000000000000001</v>
       </c>
-      <c r="J44" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="K44" s="8">
+      <c r="J44" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="K44" s="7">
         <v>0.9</v>
       </c>
     </row>
     <row r="45" spans="1:15">
-      <c r="B45" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="C45" s="8">
-        <v>1</v>
-      </c>
-      <c r="J45" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="K45" s="8">
+      <c r="B45" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C45" s="7">
+        <v>1</v>
+      </c>
+      <c r="J45" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="K45" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:15">
-      <c r="B46" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="C46" s="8">
+      <c r="B46" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C46" s="7">
         <v>0.9</v>
       </c>
-      <c r="J46" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="K46" s="8">
+      <c r="J46" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="K46" s="7">
         <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="48" spans="1:15" ht="45" customHeight="1">
-      <c r="B48" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="C48" s="10"/>
-      <c r="D48" s="10"/>
-      <c r="E48" s="10"/>
+      <c r="B48" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C48" s="9"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="9"/>
     </row>
     <row r="49" spans="2:3" ht="56">
       <c r="B49" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C49" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="50" spans="2:3">
       <c r="B50" t="s">
-        <v>60</v>
-      </c>
-      <c r="C50" s="8">
+        <v>55</v>
+      </c>
+      <c r="C50" s="7">
         <v>1.2</v>
       </c>
     </row>
     <row r="51" spans="2:3">
-      <c r="B51" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="C51" s="8">
+      <c r="B51" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C51" s="7">
         <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="52" spans="2:3">
-      <c r="B52" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="C52" s="8">
+      <c r="B52" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C52" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="53" spans="2:3">
-      <c r="B53" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="C53" s="8">
+      <c r="B53" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C53" s="7">
         <v>0.9</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="A22:A26"/>
-    <mergeCell ref="A27:A32"/>
-    <mergeCell ref="I27:I32"/>
-    <mergeCell ref="I17:I21"/>
-    <mergeCell ref="I22:I26"/>
+    <mergeCell ref="I12:I16"/>
     <mergeCell ref="B41:E41"/>
     <mergeCell ref="J41:M41"/>
     <mergeCell ref="B48:E48"/>
@@ -2366,7 +2351,12 @@
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="I7:I8"/>
     <mergeCell ref="I9:I11"/>
-    <mergeCell ref="I12:I16"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="A22:A26"/>
+    <mergeCell ref="A27:A32"/>
+    <mergeCell ref="I27:I32"/>
+    <mergeCell ref="I17:I21"/>
+    <mergeCell ref="I22:I26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2380,10 +2370,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R41"/>
+  <dimension ref="A1:R40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2396,1012 +2386,966 @@
     <col min="15" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="30" customHeight="1">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:18" ht="27" customHeight="1">
+      <c r="A1" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+    </row>
+    <row r="2" spans="1:18" ht="98">
+      <c r="A2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="J1" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-    </row>
-    <row r="2" spans="1:18">
-      <c r="A2" s="10" t="s">
+      <c r="G2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
+      <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
+      <c r="A4" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0</v>
+      </c>
+      <c r="I4" s="2">
+        <v>0</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
+      <c r="A5" s="9"/>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0</v>
+      </c>
+      <c r="D5" s="9"/>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
+      <c r="A6" s="9"/>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D6" s="9"/>
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="I6" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="15" customHeight="1">
+      <c r="A7" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="I7" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
+      <c r="A8" s="9"/>
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="E8">
+        <v>6</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="I8" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="15" customHeight="1">
+      <c r="A9" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9">
+        <v>7</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="I9" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
+      <c r="A10" s="9"/>
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D10" s="9"/>
+      <c r="E10">
+        <v>8</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="G10" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="I10" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
+      <c r="A11" s="9"/>
+      <c r="B11">
+        <v>9</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D11" s="9"/>
+      <c r="E11">
+        <v>9</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="G11" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="I11" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="15" customHeight="1">
+      <c r="A12" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12">
+        <v>10</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12">
+        <v>10</v>
+      </c>
+      <c r="F12" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="G12" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="H12" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="I12" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
+      <c r="A13" s="9"/>
+      <c r="B13">
+        <v>11</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D13" s="9"/>
+      <c r="E13">
+        <v>11</v>
+      </c>
+      <c r="F13" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="G13" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="H13" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="I13" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
+      <c r="A14" s="9"/>
+      <c r="B14">
+        <v>12</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D14" s="9"/>
+      <c r="E14">
+        <v>12</v>
+      </c>
+      <c r="F14" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="G14" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="H14" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="I14" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
+      <c r="A15" s="9"/>
+      <c r="B15">
+        <v>13</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D15" s="9"/>
+      <c r="E15">
+        <v>13</v>
+      </c>
+      <c r="F15" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="G15" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="H15" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="I15" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
+      <c r="A16" s="9"/>
+      <c r="B16">
+        <v>14</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D16" s="9"/>
+      <c r="E16">
+        <v>14</v>
+      </c>
+      <c r="F16" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="G16" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="H16" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="I16" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="15" customHeight="1">
+      <c r="A17" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17">
+        <v>15</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E17">
+        <v>15</v>
+      </c>
+      <c r="F17" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="G17" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="H17" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="I17" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="9"/>
+      <c r="B18">
+        <v>16</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D18" s="9"/>
+      <c r="E18">
+        <v>16</v>
+      </c>
+      <c r="F18" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="G18" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="H18" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="I18" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="9"/>
+      <c r="B19">
+        <v>17</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D19" s="9"/>
+      <c r="E19">
+        <v>17</v>
+      </c>
+      <c r="F19" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="G19" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="H19" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="I19" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="9"/>
+      <c r="B20">
+        <v>18</v>
+      </c>
+      <c r="C20" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D20" s="9"/>
+      <c r="E20">
+        <v>18</v>
+      </c>
+      <c r="F20" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="G20" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="H20" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="I20" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="9"/>
+      <c r="B21">
+        <v>19</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D21" s="9"/>
+      <c r="E21">
+        <v>19</v>
+      </c>
+      <c r="F21" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="G21" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="H21" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="I21" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22">
+        <v>20</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22">
+        <v>20</v>
+      </c>
+      <c r="F22" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="G22" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="H22" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="I22" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" s="9"/>
+      <c r="B23">
+        <v>21</v>
+      </c>
+      <c r="C23" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D23" s="9"/>
+      <c r="E23">
+        <v>21</v>
+      </c>
+      <c r="F23" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="G23" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="H23" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="I23" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" s="9"/>
+      <c r="B24">
+        <v>22</v>
+      </c>
+      <c r="C24" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D24" s="9"/>
+      <c r="E24">
+        <v>22</v>
+      </c>
+      <c r="F24" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="G24" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="H24" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="I24" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" s="9"/>
+      <c r="B25">
         <v>23</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="D2" s="10" t="s">
+      <c r="C25" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D25" s="9"/>
+      <c r="E25">
+        <v>23</v>
+      </c>
+      <c r="F25" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="G25" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="H25" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="I25" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" s="9"/>
+      <c r="B26">
+        <v>24</v>
+      </c>
+      <c r="C26" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D26" s="9"/>
+      <c r="E26">
+        <v>24</v>
+      </c>
+      <c r="F26" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="G26" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="H26" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="I26" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27">
+        <v>25</v>
+      </c>
+      <c r="C27" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E27">
+        <v>25</v>
+      </c>
+      <c r="F27" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="G27" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="H27" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="I27" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" s="9"/>
+      <c r="B28">
+        <v>26</v>
+      </c>
+      <c r="C28" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D28" s="9"/>
+      <c r="E28">
+        <v>26</v>
+      </c>
+      <c r="F28" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="G28" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="H28" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="I28" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" s="9"/>
+      <c r="B29">
         <v>27</v>
       </c>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="J2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="L2" s="10" t="s">
+      <c r="C29" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D29" s="9"/>
+      <c r="E29">
         <v>27</v>
       </c>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10"/>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="10"/>
-    </row>
-    <row r="3" spans="1:18" ht="70">
-      <c r="A3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="F29" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="G29" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="H29" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="I29" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" s="9"/>
+      <c r="B30">
         <v>28</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="C30" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D30" s="9"/>
+      <c r="E30">
+        <v>28</v>
+      </c>
+      <c r="F30" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="G30" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="H30" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="I30" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" s="9"/>
+      <c r="B31">
         <v>29</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="C31" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D31" s="9"/>
+      <c r="E31">
+        <v>29</v>
+      </c>
+      <c r="F31" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="G31" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="H31" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="I31" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" s="9"/>
+      <c r="B32">
         <v>30</v>
       </c>
-      <c r="J3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18">
-      <c r="A4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="2">
-        <v>0</v>
-      </c>
-      <c r="D4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4" s="2">
-        <v>0</v>
-      </c>
-      <c r="L4" t="s">
-        <v>46</v>
-      </c>
-      <c r="M4">
-        <v>1</v>
-      </c>
-      <c r="N4" s="2">
-        <v>0</v>
-      </c>
-      <c r="O4" s="2">
-        <v>0</v>
-      </c>
-      <c r="P4" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="2">
-        <v>0</v>
-      </c>
-      <c r="R4" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18">
-      <c r="D5" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="E5">
+      <c r="C32" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D32" s="9"/>
+      <c r="E32">
+        <v>30</v>
+      </c>
+      <c r="F32" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="G32" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="H32" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="I32" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14">
+      <c r="A33" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" ht="56">
+      <c r="C34" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E34" s="9"/>
+      <c r="F34" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L34" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="M34" s="9"/>
+      <c r="N34" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14">
+      <c r="C35" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F35" s="3">
         <v>2</v>
       </c>
-      <c r="F5" s="2">
-        <v>0</v>
-      </c>
-      <c r="L5" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="M5">
+      <c r="M35" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="N35" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14">
+      <c r="C36" s="2">
+        <v>1</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F36" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="M36" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="N36" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14">
+      <c r="C37" s="2">
         <v>2</v>
       </c>
-      <c r="N5" s="2">
-        <v>0</v>
-      </c>
-      <c r="O5" s="2">
-        <v>0</v>
-      </c>
-      <c r="P5" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="2">
-        <v>0</v>
-      </c>
-      <c r="R5" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18">
-      <c r="D6" s="10"/>
-      <c r="E6">
+      <c r="E37" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F37" s="3">
+        <v>1</v>
+      </c>
+      <c r="M37" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="N37" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14">
+      <c r="C38" s="2">
         <v>3</v>
       </c>
-      <c r="F6" s="2">
-        <v>0</v>
-      </c>
-      <c r="L6" s="10"/>
-      <c r="M6">
-        <v>3</v>
-      </c>
-      <c r="N6" s="2">
-        <v>0</v>
-      </c>
-      <c r="O6" s="2">
-        <v>0</v>
-      </c>
-      <c r="P6" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="2">
-        <v>0</v>
-      </c>
-      <c r="R6" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18">
-      <c r="D7" s="10"/>
-      <c r="E7">
-        <v>4</v>
-      </c>
-      <c r="F7" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="L7" s="10"/>
-      <c r="M7">
-        <v>4</v>
-      </c>
-      <c r="N7" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="O7" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="P7" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="Q7" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" ht="15" customHeight="1">
-      <c r="D8" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="E8">
-        <v>5</v>
-      </c>
-      <c r="F8" s="2">
-        <v>1</v>
-      </c>
-      <c r="L8" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="M8">
-        <v>5</v>
-      </c>
-      <c r="N8" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="O8" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="P8" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="Q8" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18">
-      <c r="D9" s="10"/>
-      <c r="E9">
-        <v>6</v>
-      </c>
-      <c r="F9" s="2">
-        <v>0.3</v>
-      </c>
-      <c r="L9" s="10"/>
-      <c r="M9">
-        <v>6</v>
-      </c>
-      <c r="N9" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="O9" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="P9" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="Q9" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" ht="15" customHeight="1">
-      <c r="D10" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="E10">
-        <v>7</v>
-      </c>
-      <c r="F10" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="L10" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="M10">
-        <v>7</v>
-      </c>
-      <c r="N10" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="O10" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="P10" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="Q10" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18">
-      <c r="D11" s="10"/>
-      <c r="E11">
-        <v>8</v>
-      </c>
-      <c r="F11" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="L11" s="10"/>
-      <c r="M11">
-        <v>8</v>
-      </c>
-      <c r="N11" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="O11" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="P11" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="Q11" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18">
-      <c r="D12" s="10"/>
-      <c r="E12">
-        <v>9</v>
-      </c>
-      <c r="F12" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="L12" s="10"/>
-      <c r="M12">
-        <v>9</v>
-      </c>
-      <c r="N12" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="O12" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="P12" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="Q12" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" ht="15" customHeight="1">
-      <c r="D13" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="E13">
-        <v>10</v>
-      </c>
-      <c r="F13" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="L13" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="M13">
-        <v>10</v>
-      </c>
-      <c r="N13" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="O13" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="P13" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="Q13" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18">
-      <c r="D14" s="10"/>
-      <c r="E14">
-        <v>11</v>
-      </c>
-      <c r="F14" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="L14" s="10"/>
-      <c r="M14">
-        <v>11</v>
-      </c>
-      <c r="N14" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="O14" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="P14" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="Q14" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18">
-      <c r="D15" s="10"/>
-      <c r="E15">
-        <v>12</v>
-      </c>
-      <c r="F15" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="L15" s="10"/>
-      <c r="M15">
-        <v>12</v>
-      </c>
-      <c r="N15" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="O15" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="P15" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="Q15" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18">
-      <c r="D16" s="10"/>
-      <c r="E16">
-        <v>13</v>
-      </c>
-      <c r="F16" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="L16" s="10"/>
-      <c r="M16">
-        <v>13</v>
-      </c>
-      <c r="N16" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="O16" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="P16" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="Q16" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="4:17">
-      <c r="D17" s="10"/>
-      <c r="E17">
-        <v>14</v>
-      </c>
-      <c r="F17" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="L17" s="10"/>
-      <c r="M17">
-        <v>14</v>
-      </c>
-      <c r="N17" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="O17" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="P17" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="Q17" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="4:17" ht="15" customHeight="1">
-      <c r="D18" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="E18">
-        <v>15</v>
-      </c>
-      <c r="F18" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="L18" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="M18">
-        <v>15</v>
-      </c>
-      <c r="N18" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="O18" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="P18" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="Q18" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="4:17">
-      <c r="D19" s="10"/>
-      <c r="E19">
-        <v>16</v>
-      </c>
-      <c r="F19" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="L19" s="10"/>
-      <c r="M19">
-        <v>16</v>
-      </c>
-      <c r="N19" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="O19" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="P19" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="Q19" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="4:17">
-      <c r="D20" s="10"/>
-      <c r="E20">
-        <v>17</v>
-      </c>
-      <c r="F20" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="L20" s="10"/>
-      <c r="M20">
-        <v>17</v>
-      </c>
-      <c r="N20" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="O20" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="P20" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="Q20" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="4:17">
-      <c r="D21" s="10"/>
-      <c r="E21">
-        <v>18</v>
-      </c>
-      <c r="F21" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="L21" s="10"/>
-      <c r="M21">
-        <v>18</v>
-      </c>
-      <c r="N21" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="O21" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="P21" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="Q21" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="4:17">
-      <c r="D22" s="10"/>
-      <c r="E22">
-        <v>19</v>
-      </c>
-      <c r="F22" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="L22" s="10"/>
-      <c r="M22">
-        <v>19</v>
-      </c>
-      <c r="N22" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="O22" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="P22" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="Q22" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="4:17">
-      <c r="D23" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E23">
-        <v>20</v>
-      </c>
-      <c r="F23" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="L23" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="M23">
-        <v>20</v>
-      </c>
-      <c r="N23" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="O23" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="P23" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="Q23" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="4:17">
-      <c r="D24" s="10"/>
-      <c r="E24">
-        <v>21</v>
-      </c>
-      <c r="F24" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="L24" s="10"/>
-      <c r="M24">
-        <v>21</v>
-      </c>
-      <c r="N24" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="O24" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="P24" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="Q24" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="4:17">
-      <c r="D25" s="10"/>
-      <c r="E25">
-        <v>22</v>
-      </c>
-      <c r="F25" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="L25" s="10"/>
-      <c r="M25">
-        <v>22</v>
-      </c>
-      <c r="N25" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="O25" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="P25" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="Q25" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="4:17">
-      <c r="D26" s="10"/>
-      <c r="E26">
-        <v>23</v>
-      </c>
-      <c r="F26" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="L26" s="10"/>
-      <c r="M26">
-        <v>23</v>
-      </c>
-      <c r="N26" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="O26" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="P26" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="Q26" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="4:17">
-      <c r="D27" s="10"/>
-      <c r="E27">
-        <v>24</v>
-      </c>
-      <c r="F27" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="L27" s="10"/>
-      <c r="M27">
-        <v>24</v>
-      </c>
-      <c r="N27" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="O27" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="P27" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="Q27" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="4:17">
-      <c r="D28" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="E28">
-        <v>25</v>
-      </c>
-      <c r="F28" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="L28" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="M28">
-        <v>25</v>
-      </c>
-      <c r="N28" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="O28" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="P28" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="Q28" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="4:17">
-      <c r="D29" s="10"/>
-      <c r="E29">
-        <v>26</v>
-      </c>
-      <c r="F29" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="L29" s="10"/>
-      <c r="M29">
-        <v>26</v>
-      </c>
-      <c r="N29" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="O29" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="P29" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="Q29" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="4:17">
-      <c r="D30" s="10"/>
-      <c r="E30">
-        <v>27</v>
-      </c>
-      <c r="F30" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="L30" s="10"/>
-      <c r="M30">
-        <v>27</v>
-      </c>
-      <c r="N30" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="O30" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="P30" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="Q30" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="4:17">
-      <c r="D31" s="10"/>
-      <c r="E31">
-        <v>28</v>
-      </c>
-      <c r="F31" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="L31" s="10"/>
-      <c r="M31">
-        <v>28</v>
-      </c>
-      <c r="N31" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="O31" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="P31" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="Q31" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="4:17">
-      <c r="D32" s="10"/>
-      <c r="E32">
-        <v>29</v>
-      </c>
-      <c r="F32" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="L32" s="10"/>
-      <c r="M32">
-        <v>29</v>
-      </c>
-      <c r="N32" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="O32" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="P32" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="Q32" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17">
-      <c r="D33" s="10"/>
-      <c r="E33">
-        <v>30</v>
-      </c>
-      <c r="F33" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="L33" s="10"/>
-      <c r="M33">
-        <v>30</v>
-      </c>
-      <c r="N33" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="O33" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="P33" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="Q33" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17">
-      <c r="A34" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17" ht="56">
-      <c r="C35" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D35" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="E35" s="10"/>
-      <c r="F35" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="L35" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="M35" s="10"/>
-      <c r="N35" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17">
-      <c r="C36" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="F36" s="3">
-        <v>2</v>
-      </c>
-      <c r="M36" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="N36" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17">
-      <c r="C37" s="2">
-        <v>1</v>
-      </c>
-      <c r="E37" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F37" s="3">
+      <c r="E38" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F38" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="M38" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="N38" s="3">
         <v>1.5</v>
       </c>
-      <c r="M37" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="N37" s="3">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17">
-      <c r="C38" s="2">
-        <v>2</v>
-      </c>
-      <c r="E38" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="F38" s="3">
-        <v>1</v>
-      </c>
-      <c r="M38" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="N38" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17">
-      <c r="C39" s="2">
-        <v>3</v>
-      </c>
-      <c r="E39" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="F39" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="M39" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="N39" s="3">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17">
-      <c r="E40" s="7"/>
-    </row>
-    <row r="41" spans="1:17">
-      <c r="E41" s="7"/>
+    </row>
+    <row r="39" spans="1:14">
+      <c r="E39" s="6"/>
+    </row>
+    <row r="40" spans="1:14">
+      <c r="E40" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="21">
-    <mergeCell ref="L2:Q2"/>
-    <mergeCell ref="J1:Q1"/>
-    <mergeCell ref="D23:D27"/>
-    <mergeCell ref="D28:D33"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="L5:L7"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="L10:L12"/>
-    <mergeCell ref="L13:L17"/>
-    <mergeCell ref="L18:L22"/>
-    <mergeCell ref="L23:L27"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="D13:D17"/>
-    <mergeCell ref="D18:D22"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="L35:M35"/>
-    <mergeCell ref="L28:L33"/>
+  <mergeCells count="18">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:I1"/>
+    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="L34:M34"/>
+    <mergeCell ref="D27:D32"/>
+    <mergeCell ref="A22:A26"/>
+    <mergeCell ref="A27:A32"/>
+    <mergeCell ref="D4:D6"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="D12:D16"/>
+    <mergeCell ref="D17:D21"/>
+    <mergeCell ref="D22:D26"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3429,38 +3373,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="49.5" customHeight="1">
-      <c r="A1" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
+      <c r="A1" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="78" customHeight="1">
       <c r="A3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="F3" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="60" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E4" s="2">
         <v>0</v>
@@ -3471,9 +3415,9 @@
     </row>
     <row r="5" spans="1:7" ht="28">
       <c r="A5" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C5" s="6"/>
+        <v>35</v>
+      </c>
+      <c r="C5" s="5"/>
       <c r="E5" s="2">
         <v>1</v>
       </c>
@@ -3525,23 +3469,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="14"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="13"/>
     </row>
     <row r="2" spans="1:5" ht="56">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="28">

</xml_diff>

<commit_message>
dispersal table module of loader complete
</commit_message>
<xml_diff>
--- a/Excel Files/life_table.xlsx
+++ b/Excel Files/life_table.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="70">
   <si>
     <t>Year</t>
   </si>
@@ -454,8 +454,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -497,13 +499,15 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2373,7 +2377,7 @@
   <dimension ref="A1:R40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="D1" sqref="D1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2398,10 +2402,8 @@
       <c r="E1" s="9"/>
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-    </row>
-    <row r="2" spans="1:18" ht="98">
+    </row>
+    <row r="2" spans="1:18" ht="112">
       <c r="A2" s="2" t="s">
         <v>23</v>
       </c>
@@ -2412,21 +2414,15 @@
         <v>25</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I2" s="2" t="s">
         <v>31</v>
       </c>
       <c r="J2" s="2" t="s">
@@ -2443,22 +2439,16 @@
       <c r="C3" s="2">
         <v>0</v>
       </c>
-      <c r="D3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
+      <c r="D3" s="2">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0</v>
       </c>
       <c r="F3" s="2">
         <v>0</v>
       </c>
       <c r="G3" s="2">
-        <v>0</v>
-      </c>
-      <c r="H3" s="2">
-        <v>0</v>
-      </c>
-      <c r="I3" s="2">
         <v>0</v>
       </c>
       <c r="R3" s="2" t="s">
@@ -2475,22 +2465,16 @@
       <c r="C4" s="2">
         <v>0</v>
       </c>
-      <c r="D4" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="E4">
-        <v>2</v>
+      <c r="D4" s="2">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0</v>
       </c>
       <c r="F4" s="2">
         <v>0</v>
       </c>
       <c r="G4" s="2">
-        <v>0</v>
-      </c>
-      <c r="H4" s="2">
-        <v>0</v>
-      </c>
-      <c r="I4" s="2">
         <v>0</v>
       </c>
       <c r="R4" s="2" t="s">
@@ -2505,20 +2489,16 @@
       <c r="C5" s="2">
         <v>0</v>
       </c>
-      <c r="D5" s="9"/>
-      <c r="E5">
-        <v>3</v>
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0</v>
       </c>
       <c r="F5" s="2">
         <v>0</v>
       </c>
       <c r="G5" s="2">
-        <v>0</v>
-      </c>
-      <c r="H5" s="2">
-        <v>0</v>
-      </c>
-      <c r="I5" s="2">
         <v>0</v>
       </c>
       <c r="R5" s="2" t="s">
@@ -2533,20 +2513,16 @@
       <c r="C6" s="2">
         <v>0.2</v>
       </c>
-      <c r="D6" s="9"/>
-      <c r="E6">
-        <v>4</v>
+      <c r="D6" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.5</v>
       </c>
       <c r="F6" s="2">
         <v>0.5</v>
       </c>
       <c r="G6" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="H6" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="I6" s="2">
         <v>1</v>
       </c>
     </row>
@@ -2560,22 +2536,16 @@
       <c r="C7" s="2">
         <v>1</v>
       </c>
-      <c r="D7" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="E7">
-        <v>5</v>
+      <c r="D7" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.5</v>
       </c>
       <c r="F7" s="2">
         <v>0.5</v>
       </c>
       <c r="G7" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="H7" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="I7" s="2">
         <v>1</v>
       </c>
     </row>
@@ -2587,20 +2557,16 @@
       <c r="C8" s="2">
         <v>0.3</v>
       </c>
-      <c r="D8" s="9"/>
-      <c r="E8">
-        <v>6</v>
+      <c r="D8" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.5</v>
       </c>
       <c r="F8" s="2">
         <v>0.5</v>
       </c>
       <c r="G8" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="H8" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="I8" s="2">
         <v>1</v>
       </c>
     </row>
@@ -2614,22 +2580,16 @@
       <c r="C9" s="2">
         <v>0.2</v>
       </c>
-      <c r="D9" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="E9">
-        <v>7</v>
+      <c r="D9" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.4</v>
       </c>
       <c r="F9" s="2">
         <v>0.66</v>
       </c>
       <c r="G9" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="H9" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="I9" s="2">
         <v>1</v>
       </c>
     </row>
@@ -2641,20 +2601,16 @@
       <c r="C10" s="2">
         <v>0.2</v>
       </c>
-      <c r="D10" s="9"/>
-      <c r="E10">
-        <v>8</v>
+      <c r="D10" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.4</v>
       </c>
       <c r="F10" s="2">
         <v>0.66</v>
       </c>
       <c r="G10" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="H10" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="I10" s="2">
         <v>1</v>
       </c>
     </row>
@@ -2666,20 +2622,16 @@
       <c r="C11" s="2">
         <v>0.2</v>
       </c>
-      <c r="D11" s="9"/>
-      <c r="E11">
-        <v>9</v>
+      <c r="D11" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0.4</v>
       </c>
       <c r="F11" s="2">
         <v>0.66</v>
       </c>
       <c r="G11" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="H11" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="I11" s="2">
         <v>1</v>
       </c>
     </row>
@@ -2693,22 +2645,16 @@
       <c r="C12" s="2">
         <v>0.2</v>
       </c>
-      <c r="D12" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="E12">
-        <v>10</v>
+      <c r="D12" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0.4</v>
       </c>
       <c r="F12" s="2">
         <v>0.66</v>
       </c>
       <c r="G12" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="H12" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="I12" s="2">
         <v>1</v>
       </c>
     </row>
@@ -2720,20 +2666,16 @@
       <c r="C13" s="2">
         <v>0.2</v>
       </c>
-      <c r="D13" s="9"/>
-      <c r="E13">
-        <v>11</v>
+      <c r="D13" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0.4</v>
       </c>
       <c r="F13" s="2">
         <v>0.66</v>
       </c>
       <c r="G13" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="H13" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="I13" s="2">
         <v>1</v>
       </c>
     </row>
@@ -2745,20 +2687,16 @@
       <c r="C14" s="2">
         <v>0.2</v>
       </c>
-      <c r="D14" s="9"/>
-      <c r="E14">
-        <v>12</v>
+      <c r="D14" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.4</v>
       </c>
       <c r="F14" s="2">
         <v>0.66</v>
       </c>
       <c r="G14" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="H14" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="I14" s="2">
         <v>1</v>
       </c>
     </row>
@@ -2770,20 +2708,16 @@
       <c r="C15" s="2">
         <v>0.2</v>
       </c>
-      <c r="D15" s="9"/>
-      <c r="E15">
-        <v>13</v>
+      <c r="D15" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.4</v>
       </c>
       <c r="F15" s="2">
         <v>0.66</v>
       </c>
       <c r="G15" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="H15" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="I15" s="2">
         <v>1</v>
       </c>
     </row>
@@ -2795,24 +2729,20 @@
       <c r="C16" s="2">
         <v>0.2</v>
       </c>
-      <c r="D16" s="9"/>
-      <c r="E16">
-        <v>14</v>
+      <c r="D16" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0.4</v>
       </c>
       <c r="F16" s="2">
         <v>0.66</v>
       </c>
       <c r="G16" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="H16" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="I16" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="15" customHeight="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15" customHeight="1">
       <c r="A17" s="9" t="s">
         <v>47</v>
       </c>
@@ -2822,26 +2752,20 @@
       <c r="C17" s="2">
         <v>0.2</v>
       </c>
-      <c r="D17" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="E17">
-        <v>15</v>
+      <c r="D17" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0.4</v>
       </c>
       <c r="F17" s="2">
         <v>0.66</v>
       </c>
       <c r="G17" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="H17" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="I17" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" s="9"/>
       <c r="B18">
         <v>16</v>
@@ -2849,24 +2773,20 @@
       <c r="C18" s="2">
         <v>0.2</v>
       </c>
-      <c r="D18" s="9"/>
-      <c r="E18">
-        <v>16</v>
+      <c r="D18" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.4</v>
       </c>
       <c r="F18" s="2">
         <v>0.66</v>
       </c>
       <c r="G18" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="H18" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="I18" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" s="9"/>
       <c r="B19">
         <v>17</v>
@@ -2874,24 +2794,20 @@
       <c r="C19" s="2">
         <v>0.2</v>
       </c>
-      <c r="D19" s="9"/>
-      <c r="E19">
-        <v>17</v>
+      <c r="D19" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0.4</v>
       </c>
       <c r="F19" s="2">
         <v>0.66</v>
       </c>
       <c r="G19" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="H19" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="I19" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" s="9"/>
       <c r="B20">
         <v>18</v>
@@ -2899,24 +2815,20 @@
       <c r="C20" s="2">
         <v>0.2</v>
       </c>
-      <c r="D20" s="9"/>
-      <c r="E20">
-        <v>18</v>
+      <c r="D20" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0.4</v>
       </c>
       <c r="F20" s="2">
         <v>0.66</v>
       </c>
       <c r="G20" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="H20" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="I20" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" s="9"/>
       <c r="B21">
         <v>19</v>
@@ -2924,24 +2836,20 @@
       <c r="C21" s="2">
         <v>0.2</v>
       </c>
-      <c r="D21" s="9"/>
-      <c r="E21">
-        <v>19</v>
+      <c r="D21" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="E21" s="2">
+        <v>0.4</v>
       </c>
       <c r="F21" s="2">
         <v>0.66</v>
       </c>
       <c r="G21" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="H21" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="I21" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" s="9" t="s">
         <v>9</v>
       </c>
@@ -2951,26 +2859,20 @@
       <c r="C22" s="2">
         <v>0.2</v>
       </c>
-      <c r="D22" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E22">
-        <v>20</v>
+      <c r="D22" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="E22" s="2">
+        <v>0.4</v>
       </c>
       <c r="F22" s="2">
         <v>0.66</v>
       </c>
       <c r="G22" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="H22" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="I22" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23" s="9"/>
       <c r="B23">
         <v>21</v>
@@ -2978,24 +2880,20 @@
       <c r="C23" s="2">
         <v>0.2</v>
       </c>
-      <c r="D23" s="9"/>
-      <c r="E23">
-        <v>21</v>
+      <c r="D23" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="E23" s="2">
+        <v>0.4</v>
       </c>
       <c r="F23" s="2">
         <v>0.66</v>
       </c>
       <c r="G23" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="H23" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="I23" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24" s="9"/>
       <c r="B24">
         <v>22</v>
@@ -3003,24 +2901,20 @@
       <c r="C24" s="2">
         <v>0.2</v>
       </c>
-      <c r="D24" s="9"/>
-      <c r="E24">
-        <v>22</v>
+      <c r="D24" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="E24" s="2">
+        <v>0.4</v>
       </c>
       <c r="F24" s="2">
         <v>0.66</v>
       </c>
       <c r="G24" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="H24" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="I24" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25" s="9"/>
       <c r="B25">
         <v>23</v>
@@ -3028,24 +2922,20 @@
       <c r="C25" s="2">
         <v>0.2</v>
       </c>
-      <c r="D25" s="9"/>
-      <c r="E25">
-        <v>23</v>
+      <c r="D25" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="E25" s="2">
+        <v>0.4</v>
       </c>
       <c r="F25" s="2">
         <v>0.66</v>
       </c>
       <c r="G25" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="H25" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="I25" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
       <c r="A26" s="9"/>
       <c r="B26">
         <v>24</v>
@@ -3053,24 +2943,20 @@
       <c r="C26" s="2">
         <v>0.2</v>
       </c>
-      <c r="D26" s="9"/>
-      <c r="E26">
-        <v>24</v>
+      <c r="D26" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="E26" s="2">
+        <v>0.4</v>
       </c>
       <c r="F26" s="2">
         <v>0.66</v>
       </c>
       <c r="G26" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="H26" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="I26" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
       <c r="A27" s="9" t="s">
         <v>19</v>
       </c>
@@ -3080,26 +2966,20 @@
       <c r="C27" s="2">
         <v>0.2</v>
       </c>
-      <c r="D27" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E27">
-        <v>25</v>
+      <c r="D27" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="E27" s="2">
+        <v>0.4</v>
       </c>
       <c r="F27" s="2">
         <v>0.66</v>
       </c>
       <c r="G27" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="H27" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="I27" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
       <c r="A28" s="9"/>
       <c r="B28">
         <v>26</v>
@@ -3107,24 +2987,20 @@
       <c r="C28" s="2">
         <v>0.2</v>
       </c>
-      <c r="D28" s="9"/>
-      <c r="E28">
-        <v>26</v>
+      <c r="D28" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="E28" s="2">
+        <v>0.4</v>
       </c>
       <c r="F28" s="2">
         <v>0.66</v>
       </c>
       <c r="G28" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="H28" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="I28" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
       <c r="A29" s="9"/>
       <c r="B29">
         <v>27</v>
@@ -3132,24 +3008,20 @@
       <c r="C29" s="2">
         <v>0.2</v>
       </c>
-      <c r="D29" s="9"/>
-      <c r="E29">
-        <v>27</v>
+      <c r="D29" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="E29" s="2">
+        <v>0.4</v>
       </c>
       <c r="F29" s="2">
         <v>0.66</v>
       </c>
       <c r="G29" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="H29" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="I29" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
       <c r="A30" s="9"/>
       <c r="B30">
         <v>28</v>
@@ -3157,24 +3029,20 @@
       <c r="C30" s="2">
         <v>0.2</v>
       </c>
-      <c r="D30" s="9"/>
-      <c r="E30">
-        <v>28</v>
+      <c r="D30" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="E30" s="2">
+        <v>0.4</v>
       </c>
       <c r="F30" s="2">
         <v>0.66</v>
       </c>
       <c r="G30" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="H30" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="I30" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
       <c r="A31" s="9"/>
       <c r="B31">
         <v>29</v>
@@ -3182,24 +3050,20 @@
       <c r="C31" s="2">
         <v>0.2</v>
       </c>
-      <c r="D31" s="9"/>
-      <c r="E31">
-        <v>29</v>
+      <c r="D31" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="E31" s="2">
+        <v>0.4</v>
       </c>
       <c r="F31" s="2">
         <v>0.66</v>
       </c>
       <c r="G31" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="H31" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="I31" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
       <c r="A32" s="9"/>
       <c r="B32">
         <v>30</v>
@@ -3207,20 +3071,16 @@
       <c r="C32" s="2">
         <v>0.2</v>
       </c>
-      <c r="D32" s="9"/>
-      <c r="E32">
-        <v>30</v>
+      <c r="D32" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="E32" s="2">
+        <v>0.4</v>
       </c>
       <c r="F32" s="2">
         <v>0.66</v>
       </c>
       <c r="G32" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="H32" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="I32" s="2">
         <v>1</v>
       </c>
     </row>
@@ -3324,22 +3184,15 @@
       <c r="E40" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="11">
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:I1"/>
+    <mergeCell ref="D1:G1"/>
     <mergeCell ref="A12:A16"/>
     <mergeCell ref="A17:A21"/>
     <mergeCell ref="D34:E34"/>
     <mergeCell ref="L34:M34"/>
-    <mergeCell ref="D27:D32"/>
     <mergeCell ref="A22:A26"/>
     <mergeCell ref="A27:A32"/>
-    <mergeCell ref="D4:D6"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="D12:D16"/>
-    <mergeCell ref="D17:D21"/>
-    <mergeCell ref="D22:D26"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="A9:A11"/>

</xml_diff>

<commit_message>
fixed the module for loading seeds
</commit_message>
<xml_diff>
--- a/Excel Files/life_table.xlsx
+++ b/Excel Files/life_table.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="life table" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="80">
   <si>
     <t>Year</t>
   </si>
@@ -367,6 +367,30 @@
   </si>
   <si>
     <t>Note: This behavior is not taken from the excel file. Instead, it is coded in lifetable.py</t>
+  </si>
+  <si>
+    <t>rules for forming frendships:</t>
+  </si>
+  <si>
+    <t>1. both have to be adults (fem &gt; 5 years, male &gt; 7)</t>
+  </si>
+  <si>
+    <t>2. the two individuals can't already have a relationship, such as kin or aggressive</t>
+  </si>
+  <si>
+    <t>3. friendships have to be male-female or female-female</t>
+  </si>
+  <si>
+    <t>procedure for making new friends</t>
+  </si>
+  <si>
+    <t>1. decide if a new friend is about to be made</t>
+  </si>
+  <si>
+    <t>2. select the likely candidates for freindship</t>
+  </si>
+  <si>
+    <t>3. randomly select an individual from the pool of potential friends</t>
   </si>
 </sst>
 </file>
@@ -493,6 +517,7 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -508,7 +533,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -824,36 +848,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+    <sheetView topLeftCell="A36" workbookViewId="0">
       <selection activeCell="K43" sqref="K43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:15" s="2" customFormat="1" ht="108" customHeight="1">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="9"/>
+      <c r="J1" s="10"/>
       <c r="K1" s="2" t="s">
         <v>3</v>
       </c>
@@ -877,11 +901,11 @@
       <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
       <c r="I2" t="s">
         <v>1</v>
       </c>
@@ -928,7 +952,7 @@
       </c>
     </row>
     <row r="4" spans="1:15">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="11" t="s">
         <v>41</v>
       </c>
       <c r="B4">
@@ -947,7 +971,7 @@
       <c r="G4" s="1">
         <v>0</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="I4" s="10" t="s">
         <v>41</v>
       </c>
       <c r="J4">
@@ -968,7 +992,7 @@
       </c>
     </row>
     <row r="5" spans="1:15">
-      <c r="A5" s="10"/>
+      <c r="A5" s="11"/>
       <c r="B5">
         <v>3</v>
       </c>
@@ -985,7 +1009,7 @@
       <c r="G5" s="1">
         <v>0</v>
       </c>
-      <c r="I5" s="9"/>
+      <c r="I5" s="10"/>
       <c r="J5">
         <v>3</v>
       </c>
@@ -1004,7 +1028,7 @@
       </c>
     </row>
     <row r="6" spans="1:15">
-      <c r="A6" s="10"/>
+      <c r="A6" s="11"/>
       <c r="B6">
         <v>4</v>
       </c>
@@ -1021,7 +1045,7 @@
       <c r="G6" s="1">
         <v>0</v>
       </c>
-      <c r="I6" s="9"/>
+      <c r="I6" s="10"/>
       <c r="J6">
         <v>4</v>
       </c>
@@ -1040,7 +1064,7 @@
       </c>
     </row>
     <row r="7" spans="1:15" ht="15" customHeight="1">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="10" t="s">
         <v>42</v>
       </c>
       <c r="B7">
@@ -1060,7 +1084,7 @@
         <f xml:space="preserve"> E7*F7</f>
         <v>97.76</v>
       </c>
-      <c r="I7" s="9" t="s">
+      <c r="I7" s="10" t="s">
         <v>44</v>
       </c>
       <c r="J7">
@@ -1081,7 +1105,7 @@
       </c>
     </row>
     <row r="8" spans="1:15">
-      <c r="A8" s="9"/>
+      <c r="A8" s="10"/>
       <c r="B8">
         <v>6</v>
       </c>
@@ -1099,7 +1123,7 @@
         <f t="shared" ref="G8:G32" si="3" xml:space="preserve"> E8*F8</f>
         <v>95.8048</v>
       </c>
-      <c r="I8" s="9"/>
+      <c r="I8" s="10"/>
       <c r="J8">
         <v>6</v>
       </c>
@@ -1118,7 +1142,7 @@
       </c>
     </row>
     <row r="9" spans="1:15">
-      <c r="A9" s="9"/>
+      <c r="A9" s="10"/>
       <c r="B9">
         <v>7</v>
       </c>
@@ -1136,7 +1160,7 @@
         <f t="shared" si="3"/>
         <v>93.888704000000004</v>
       </c>
-      <c r="I9" s="9" t="s">
+      <c r="I9" s="10" t="s">
         <v>43</v>
       </c>
       <c r="J9">
@@ -1157,7 +1181,7 @@
       </c>
     </row>
     <row r="10" spans="1:15">
-      <c r="A10" s="9"/>
+      <c r="A10" s="10"/>
       <c r="B10">
         <v>8</v>
       </c>
@@ -1175,7 +1199,7 @@
         <f t="shared" si="3"/>
         <v>92.010929920000009</v>
       </c>
-      <c r="I10" s="9"/>
+      <c r="I10" s="10"/>
       <c r="J10">
         <v>8</v>
       </c>
@@ -1194,7 +1218,7 @@
       </c>
     </row>
     <row r="11" spans="1:15">
-      <c r="A11" s="9"/>
+      <c r="A11" s="10"/>
       <c r="B11">
         <v>9</v>
       </c>
@@ -1212,7 +1236,7 @@
         <f t="shared" si="3"/>
         <v>90.17071132160001</v>
       </c>
-      <c r="I11" s="9"/>
+      <c r="I11" s="10"/>
       <c r="J11">
         <v>9</v>
       </c>
@@ -1231,7 +1255,7 @@
       </c>
     </row>
     <row r="12" spans="1:15">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="10" t="s">
         <v>45</v>
       </c>
       <c r="B12">
@@ -1251,7 +1275,7 @@
         <f t="shared" si="3"/>
         <v>106.04075651420162</v>
       </c>
-      <c r="I12" s="9" t="s">
+      <c r="I12" s="10" t="s">
         <v>45</v>
       </c>
       <c r="J12">
@@ -1272,7 +1296,7 @@
       </c>
     </row>
     <row r="13" spans="1:15">
-      <c r="A13" s="9"/>
+      <c r="A13" s="10"/>
       <c r="B13">
         <v>11</v>
       </c>
@@ -1290,7 +1314,7 @@
         <f t="shared" si="3"/>
         <v>103.38973760134657</v>
       </c>
-      <c r="I13" s="9"/>
+      <c r="I13" s="10"/>
       <c r="J13">
         <v>11</v>
       </c>
@@ -1309,7 +1333,7 @@
       </c>
     </row>
     <row r="14" spans="1:15">
-      <c r="A14" s="9"/>
+      <c r="A14" s="10"/>
       <c r="B14">
         <v>12</v>
       </c>
@@ -1327,7 +1351,7 @@
         <f t="shared" si="3"/>
         <v>100.80499416131291</v>
       </c>
-      <c r="I14" s="9"/>
+      <c r="I14" s="10"/>
       <c r="J14">
         <v>12</v>
       </c>
@@ -1346,7 +1370,7 @@
       </c>
     </row>
     <row r="15" spans="1:15">
-      <c r="A15" s="9"/>
+      <c r="A15" s="10"/>
       <c r="B15">
         <v>13</v>
       </c>
@@ -1364,7 +1388,7 @@
         <f t="shared" si="3"/>
         <v>98.284869307280076</v>
       </c>
-      <c r="I15" s="9"/>
+      <c r="I15" s="10"/>
       <c r="J15">
         <v>13</v>
       </c>
@@ -1383,7 +1407,7 @@
       </c>
     </row>
     <row r="16" spans="1:15">
-      <c r="A16" s="9"/>
+      <c r="A16" s="10"/>
       <c r="B16">
         <v>14</v>
       </c>
@@ -1401,7 +1425,7 @@
         <f t="shared" si="3"/>
         <v>95.827747574598078</v>
       </c>
-      <c r="I16" s="9"/>
+      <c r="I16" s="10"/>
       <c r="J16">
         <v>14</v>
       </c>
@@ -1420,7 +1444,7 @@
       </c>
     </row>
     <row r="17" spans="1:15">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="10" t="s">
         <v>46</v>
       </c>
       <c r="B17">
@@ -1440,7 +1464,7 @@
         <f t="shared" si="3"/>
         <v>109.0040628661053</v>
       </c>
-      <c r="I17" s="9" t="s">
+      <c r="I17" s="10" t="s">
         <v>46</v>
       </c>
       <c r="J17">
@@ -1461,7 +1485,7 @@
       </c>
     </row>
     <row r="18" spans="1:15">
-      <c r="A18" s="9"/>
+      <c r="A18" s="10"/>
       <c r="B18">
         <v>16</v>
       </c>
@@ -1479,7 +1503,7 @@
         <f t="shared" si="3"/>
         <v>105.73394098012214</v>
       </c>
-      <c r="I18" s="9"/>
+      <c r="I18" s="10"/>
       <c r="J18">
         <v>16</v>
       </c>
@@ -1498,7 +1522,7 @@
       </c>
     </row>
     <row r="19" spans="1:15">
-      <c r="A19" s="9"/>
+      <c r="A19" s="10"/>
       <c r="B19">
         <v>17</v>
       </c>
@@ -1516,7 +1540,7 @@
         <f t="shared" si="3"/>
         <v>102.56192275071849</v>
       </c>
-      <c r="I19" s="9"/>
+      <c r="I19" s="10"/>
       <c r="J19">
         <v>17</v>
       </c>
@@ -1535,7 +1559,7 @@
       </c>
     </row>
     <row r="20" spans="1:15">
-      <c r="A20" s="9"/>
+      <c r="A20" s="10"/>
       <c r="B20">
         <v>18</v>
       </c>
@@ -1553,7 +1577,7 @@
         <f t="shared" si="3"/>
         <v>99.485065068196931</v>
       </c>
-      <c r="I20" s="9"/>
+      <c r="I20" s="10"/>
       <c r="J20">
         <v>18</v>
       </c>
@@ -1572,7 +1596,7 @@
       </c>
     </row>
     <row r="21" spans="1:15">
-      <c r="A21" s="9"/>
+      <c r="A21" s="10"/>
       <c r="B21">
         <v>19</v>
       </c>
@@ -1590,7 +1614,7 @@
         <f t="shared" si="3"/>
         <v>96.500513116151041</v>
       </c>
-      <c r="I21" s="9"/>
+      <c r="I21" s="10"/>
       <c r="J21">
         <v>19</v>
       </c>
@@ -1609,7 +1633,7 @@
       </c>
     </row>
     <row r="22" spans="1:15">
-      <c r="A22" s="9" t="s">
+      <c r="A22" s="10" t="s">
         <v>9</v>
       </c>
       <c r="B22">
@@ -1629,7 +1653,7 @@
         <f t="shared" si="3"/>
         <v>100.29160470285697</v>
       </c>
-      <c r="I22" s="9" t="s">
+      <c r="I22" s="10" t="s">
         <v>9</v>
       </c>
       <c r="J22">
@@ -1650,7 +1674,7 @@
       </c>
     </row>
     <row r="23" spans="1:15">
-      <c r="A23" s="9"/>
+      <c r="A23" s="10"/>
       <c r="B23">
         <v>21</v>
       </c>
@@ -1668,7 +1692,7 @@
         <f t="shared" si="3"/>
         <v>99.288688655828395</v>
       </c>
-      <c r="I23" s="9"/>
+      <c r="I23" s="10"/>
       <c r="J23">
         <v>21</v>
       </c>
@@ -1687,7 +1711,7 @@
       </c>
     </row>
     <row r="24" spans="1:15">
-      <c r="A24" s="9"/>
+      <c r="A24" s="10"/>
       <c r="B24">
         <v>22</v>
       </c>
@@ -1705,7 +1729,7 @@
         <f t="shared" si="3"/>
         <v>98.295801769270113</v>
       </c>
-      <c r="I24" s="9"/>
+      <c r="I24" s="10"/>
       <c r="J24">
         <v>22</v>
       </c>
@@ -1724,7 +1748,7 @@
       </c>
     </row>
     <row r="25" spans="1:15">
-      <c r="A25" s="9"/>
+      <c r="A25" s="10"/>
       <c r="B25">
         <v>23</v>
       </c>
@@ -1742,7 +1766,7 @@
         <f t="shared" si="3"/>
         <v>97.312843751577418</v>
       </c>
-      <c r="I25" s="9"/>
+      <c r="I25" s="10"/>
       <c r="J25">
         <v>23</v>
       </c>
@@ -1761,7 +1785,7 @@
       </c>
     </row>
     <row r="26" spans="1:15">
-      <c r="A26" s="9"/>
+      <c r="A26" s="10"/>
       <c r="B26">
         <v>24</v>
       </c>
@@ -1779,7 +1803,7 @@
         <f t="shared" si="3"/>
         <v>96.339715314061635</v>
       </c>
-      <c r="I26" s="9"/>
+      <c r="I26" s="10"/>
       <c r="J26">
         <v>24</v>
       </c>
@@ -1798,7 +1822,7 @@
       </c>
     </row>
     <row r="27" spans="1:15">
-      <c r="A27" s="9" t="s">
+      <c r="A27" s="10" t="s">
         <v>19</v>
       </c>
       <c r="B27">
@@ -1818,7 +1842,7 @@
         <f t="shared" si="3"/>
         <v>25.433684842912271</v>
       </c>
-      <c r="I27" s="9" t="s">
+      <c r="I27" s="10" t="s">
         <v>19</v>
       </c>
       <c r="J27">
@@ -1839,7 +1863,7 @@
       </c>
     </row>
     <row r="28" spans="1:15">
-      <c r="A28" s="9"/>
+      <c r="A28" s="10"/>
       <c r="B28">
         <v>26</v>
       </c>
@@ -1857,7 +1881,7 @@
         <f t="shared" si="3"/>
         <v>17.803579390038589</v>
       </c>
-      <c r="I28" s="9"/>
+      <c r="I28" s="10"/>
       <c r="J28">
         <v>26</v>
       </c>
@@ -1876,7 +1900,7 @@
       </c>
     </row>
     <row r="29" spans="1:15">
-      <c r="A29" s="9"/>
+      <c r="A29" s="10"/>
       <c r="B29">
         <v>27</v>
       </c>
@@ -1894,7 +1918,7 @@
         <f t="shared" si="3"/>
         <v>12.462505573027014</v>
       </c>
-      <c r="I29" s="9"/>
+      <c r="I29" s="10"/>
       <c r="J29">
         <v>27</v>
       </c>
@@ -1913,7 +1937,7 @@
       </c>
     </row>
     <row r="30" spans="1:15">
-      <c r="A30" s="9"/>
+      <c r="A30" s="10"/>
       <c r="B30">
         <v>28</v>
       </c>
@@ -1931,7 +1955,7 @@
         <f t="shared" si="3"/>
         <v>8.7237539011189096</v>
       </c>
-      <c r="I30" s="9"/>
+      <c r="I30" s="10"/>
       <c r="J30">
         <v>28</v>
       </c>
@@ -1950,7 +1974,7 @@
       </c>
     </row>
     <row r="31" spans="1:15">
-      <c r="A31" s="9"/>
+      <c r="A31" s="10"/>
       <c r="B31">
         <v>29</v>
       </c>
@@ -1968,7 +1992,7 @@
         <f t="shared" si="3"/>
         <v>6.1066277307832371</v>
       </c>
-      <c r="I31" s="9"/>
+      <c r="I31" s="10"/>
       <c r="J31">
         <v>29</v>
       </c>
@@ -1987,7 +2011,7 @@
       </c>
     </row>
     <row r="32" spans="1:15">
-      <c r="A32" s="9"/>
+      <c r="A32" s="10"/>
       <c r="B32">
         <v>30</v>
       </c>
@@ -2005,7 +2029,7 @@
         <f t="shared" si="3"/>
         <v>4.2746394115482662</v>
       </c>
-      <c r="I32" s="9"/>
+      <c r="I32" s="10"/>
       <c r="J32">
         <v>30</v>
       </c>
@@ -2220,18 +2244,18 @@
       </c>
     </row>
     <row r="41" spans="1:15" ht="43.5" customHeight="1">
-      <c r="B41" s="9" t="s">
+      <c r="B41" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="C41" s="9"/>
-      <c r="D41" s="9"/>
-      <c r="E41" s="9"/>
-      <c r="J41" s="9" t="s">
+      <c r="C41" s="10"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="10"/>
+      <c r="J41" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="K41" s="9"/>
-      <c r="L41" s="9"/>
-      <c r="M41" s="9"/>
+      <c r="K41" s="10"/>
+      <c r="L41" s="10"/>
+      <c r="M41" s="10"/>
     </row>
     <row r="42" spans="1:15" ht="56">
       <c r="B42" s="2" t="s">
@@ -2304,12 +2328,12 @@
       </c>
     </row>
     <row r="48" spans="1:15" ht="45" customHeight="1">
-      <c r="B48" s="9" t="s">
+      <c r="B48" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="C48" s="9"/>
-      <c r="D48" s="9"/>
-      <c r="E48" s="9"/>
+      <c r="C48" s="10"/>
+      <c r="D48" s="10"/>
+      <c r="E48" s="10"/>
     </row>
     <row r="49" spans="2:3" ht="56">
       <c r="B49" s="2" t="s">
@@ -2353,6 +2377,13 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="I9:I11"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="A22:A26"/>
+    <mergeCell ref="A27:A32"/>
+    <mergeCell ref="I27:I32"/>
+    <mergeCell ref="I17:I21"/>
+    <mergeCell ref="I22:I26"/>
     <mergeCell ref="I12:I16"/>
     <mergeCell ref="B41:E41"/>
     <mergeCell ref="J41:M41"/>
@@ -2369,13 +2400,6 @@
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="I7:I8"/>
-    <mergeCell ref="I9:I11"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="A22:A26"/>
-    <mergeCell ref="A27:A32"/>
-    <mergeCell ref="I27:I32"/>
-    <mergeCell ref="I17:I21"/>
-    <mergeCell ref="I22:I26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2406,17 +2430,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="27" customHeight="1">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
     </row>
     <row r="2" spans="1:18" ht="112">
       <c r="A2" s="2" t="s">
@@ -2471,7 +2495,7 @@
       </c>
     </row>
     <row r="4" spans="1:18">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="10" t="s">
         <v>41</v>
       </c>
       <c r="B4">
@@ -2497,7 +2521,7 @@
       </c>
     </row>
     <row r="5" spans="1:18">
-      <c r="A5" s="9"/>
+      <c r="A5" s="10"/>
       <c r="B5">
         <v>3</v>
       </c>
@@ -2521,7 +2545,7 @@
       </c>
     </row>
     <row r="6" spans="1:18">
-      <c r="A6" s="9"/>
+      <c r="A6" s="10"/>
       <c r="B6">
         <v>4</v>
       </c>
@@ -2542,7 +2566,7 @@
       </c>
     </row>
     <row r="7" spans="1:18" ht="15" customHeight="1">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="10" t="s">
         <v>44</v>
       </c>
       <c r="B7">
@@ -2565,7 +2589,7 @@
       </c>
     </row>
     <row r="8" spans="1:18">
-      <c r="A8" s="9"/>
+      <c r="A8" s="10"/>
       <c r="B8">
         <v>6</v>
       </c>
@@ -2586,7 +2610,7 @@
       </c>
     </row>
     <row r="9" spans="1:18" ht="15" customHeight="1">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="10" t="s">
         <v>43</v>
       </c>
       <c r="B9">
@@ -2609,7 +2633,7 @@
       </c>
     </row>
     <row r="10" spans="1:18">
-      <c r="A10" s="9"/>
+      <c r="A10" s="10"/>
       <c r="B10">
         <v>8</v>
       </c>
@@ -2630,7 +2654,7 @@
       </c>
     </row>
     <row r="11" spans="1:18">
-      <c r="A11" s="9"/>
+      <c r="A11" s="10"/>
       <c r="B11">
         <v>9</v>
       </c>
@@ -2651,7 +2675,7 @@
       </c>
     </row>
     <row r="12" spans="1:18" ht="15" customHeight="1">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="10" t="s">
         <v>45</v>
       </c>
       <c r="B12">
@@ -2674,7 +2698,7 @@
       </c>
     </row>
     <row r="13" spans="1:18">
-      <c r="A13" s="9"/>
+      <c r="A13" s="10"/>
       <c r="B13">
         <v>11</v>
       </c>
@@ -2695,7 +2719,7 @@
       </c>
     </row>
     <row r="14" spans="1:18">
-      <c r="A14" s="9"/>
+      <c r="A14" s="10"/>
       <c r="B14">
         <v>12</v>
       </c>
@@ -2716,7 +2740,7 @@
       </c>
     </row>
     <row r="15" spans="1:18">
-      <c r="A15" s="9"/>
+      <c r="A15" s="10"/>
       <c r="B15">
         <v>13</v>
       </c>
@@ -2737,7 +2761,7 @@
       </c>
     </row>
     <row r="16" spans="1:18">
-      <c r="A16" s="9"/>
+      <c r="A16" s="10"/>
       <c r="B16">
         <v>14</v>
       </c>
@@ -2758,7 +2782,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="15" customHeight="1">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="10" t="s">
         <v>46</v>
       </c>
       <c r="B17">
@@ -2781,7 +2805,7 @@
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="9"/>
+      <c r="A18" s="10"/>
       <c r="B18">
         <v>16</v>
       </c>
@@ -2802,7 +2826,7 @@
       </c>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="9"/>
+      <c r="A19" s="10"/>
       <c r="B19">
         <v>17</v>
       </c>
@@ -2823,7 +2847,7 @@
       </c>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="9"/>
+      <c r="A20" s="10"/>
       <c r="B20">
         <v>18</v>
       </c>
@@ -2844,7 +2868,7 @@
       </c>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="9"/>
+      <c r="A21" s="10"/>
       <c r="B21">
         <v>19</v>
       </c>
@@ -2865,7 +2889,7 @@
       </c>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="9" t="s">
+      <c r="A22" s="10" t="s">
         <v>9</v>
       </c>
       <c r="B22">
@@ -2888,7 +2912,7 @@
       </c>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="9"/>
+      <c r="A23" s="10"/>
       <c r="B23">
         <v>21</v>
       </c>
@@ -2909,7 +2933,7 @@
       </c>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="9"/>
+      <c r="A24" s="10"/>
       <c r="B24">
         <v>22</v>
       </c>
@@ -2930,7 +2954,7 @@
       </c>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="9"/>
+      <c r="A25" s="10"/>
       <c r="B25">
         <v>23</v>
       </c>
@@ -2951,7 +2975,7 @@
       </c>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="9"/>
+      <c r="A26" s="10"/>
       <c r="B26">
         <v>24</v>
       </c>
@@ -2972,7 +2996,7 @@
       </c>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="9" t="s">
+      <c r="A27" s="10" t="s">
         <v>19</v>
       </c>
       <c r="B27">
@@ -2995,7 +3019,7 @@
       </c>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="9"/>
+      <c r="A28" s="10"/>
       <c r="B28">
         <v>26</v>
       </c>
@@ -3016,7 +3040,7 @@
       </c>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="9"/>
+      <c r="A29" s="10"/>
       <c r="B29">
         <v>27</v>
       </c>
@@ -3037,7 +3061,7 @@
       </c>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="9"/>
+      <c r="A30" s="10"/>
       <c r="B30">
         <v>28</v>
       </c>
@@ -3058,7 +3082,7 @@
       </c>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="9"/>
+      <c r="A31" s="10"/>
       <c r="B31">
         <v>29</v>
       </c>
@@ -3079,7 +3103,7 @@
       </c>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="9"/>
+      <c r="A32" s="10"/>
       <c r="B32">
         <v>30</v>
       </c>
@@ -3108,17 +3132,17 @@
       <c r="C34" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D34" s="9" t="s">
+      <c r="D34" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="E34" s="9"/>
+      <c r="E34" s="10"/>
       <c r="F34" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="L34" s="9" t="s">
+      <c r="L34" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="M34" s="9"/>
+      <c r="M34" s="10"/>
       <c r="N34" s="2" t="s">
         <v>55</v>
       </c>
@@ -3200,17 +3224,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="A12:A16"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="D34:E34"/>
     <mergeCell ref="L34:M34"/>
     <mergeCell ref="A22:A26"/>
     <mergeCell ref="A27:A32"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="D34:E34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -3224,10 +3248,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -3241,15 +3265,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="49.5" customHeight="1">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="2" t="s">
@@ -3316,6 +3340,46 @@
       </c>
       <c r="F7" s="2">
         <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="28">
+      <c r="A9" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="42">
+      <c r="A10" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="28">
+      <c r="A11" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="28">
+      <c r="A14" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="28">
+      <c r="A15" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="28">
+      <c r="A16" s="2" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -3346,13 +3410,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="13"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="14"/>
     </row>
     <row r="2" spans="1:5" ht="56">
       <c r="A2" s="2" t="s">
@@ -3399,7 +3463,7 @@
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="9" t="s">
         <v>71</v>
       </c>
     </row>

</xml_diff>

<commit_message>
modified life table - all agents now die at age 30
</commit_message>
<xml_diff>
--- a/Excel Files/life_table.xlsx
+++ b/Excel Files/life_table.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540"/>
   </bookViews>
   <sheets>
     <sheet name="life table" sheetId="1" r:id="rId1"/>
@@ -499,7 +499,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -518,6 +518,9 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -846,38 +849,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O53"/>
+  <dimension ref="A1:O54"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="K43" sqref="K43"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:15" s="2" customFormat="1" ht="108" customHeight="1">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="10"/>
+      <c r="J1" s="11"/>
       <c r="K1" s="2" t="s">
         <v>3</v>
       </c>
@@ -901,11 +904,11 @@
       <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
       <c r="I2" t="s">
         <v>1</v>
       </c>
@@ -952,7 +955,7 @@
       </c>
     </row>
     <row r="4" spans="1:15">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="12" t="s">
         <v>41</v>
       </c>
       <c r="B4">
@@ -971,7 +974,7 @@
       <c r="G4" s="1">
         <v>0</v>
       </c>
-      <c r="I4" s="10" t="s">
+      <c r="I4" s="11" t="s">
         <v>41</v>
       </c>
       <c r="J4">
@@ -992,7 +995,7 @@
       </c>
     </row>
     <row r="5" spans="1:15">
-      <c r="A5" s="11"/>
+      <c r="A5" s="12"/>
       <c r="B5">
         <v>3</v>
       </c>
@@ -1009,7 +1012,7 @@
       <c r="G5" s="1">
         <v>0</v>
       </c>
-      <c r="I5" s="10"/>
+      <c r="I5" s="11"/>
       <c r="J5">
         <v>3</v>
       </c>
@@ -1020,7 +1023,7 @@
         <v>0</v>
       </c>
       <c r="N5" s="1">
-        <f t="shared" ref="N5:N32" si="1" xml:space="preserve"> N4-(N4*L4)</f>
+        <f t="shared" ref="N5:N31" si="1" xml:space="preserve"> N4-(N4*L4)</f>
         <v>557.20500000000004</v>
       </c>
       <c r="O5">
@@ -1028,7 +1031,7 @@
       </c>
     </row>
     <row r="6" spans="1:15">
-      <c r="A6" s="11"/>
+      <c r="A6" s="12"/>
       <c r="B6">
         <v>4</v>
       </c>
@@ -1045,7 +1048,7 @@
       <c r="G6" s="1">
         <v>0</v>
       </c>
-      <c r="I6" s="10"/>
+      <c r="I6" s="11"/>
       <c r="J6">
         <v>4</v>
       </c>
@@ -1064,7 +1067,7 @@
       </c>
     </row>
     <row r="7" spans="1:15" ht="15" customHeight="1">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="11" t="s">
         <v>42</v>
       </c>
       <c r="B7">
@@ -1084,7 +1087,7 @@
         <f xml:space="preserve"> E7*F7</f>
         <v>97.76</v>
       </c>
-      <c r="I7" s="10" t="s">
+      <c r="I7" s="11" t="s">
         <v>44</v>
       </c>
       <c r="J7">
@@ -1105,7 +1108,7 @@
       </c>
     </row>
     <row r="8" spans="1:15">
-      <c r="A8" s="10"/>
+      <c r="A8" s="11"/>
       <c r="B8">
         <v>6</v>
       </c>
@@ -1123,7 +1126,7 @@
         <f t="shared" ref="G8:G32" si="3" xml:space="preserve"> E8*F8</f>
         <v>95.8048</v>
       </c>
-      <c r="I8" s="10"/>
+      <c r="I8" s="11"/>
       <c r="J8">
         <v>6</v>
       </c>
@@ -1142,7 +1145,7 @@
       </c>
     </row>
     <row r="9" spans="1:15">
-      <c r="A9" s="10"/>
+      <c r="A9" s="11"/>
       <c r="B9">
         <v>7</v>
       </c>
@@ -1160,7 +1163,7 @@
         <f t="shared" si="3"/>
         <v>93.888704000000004</v>
       </c>
-      <c r="I9" s="10" t="s">
+      <c r="I9" s="11" t="s">
         <v>43</v>
       </c>
       <c r="J9">
@@ -1181,7 +1184,7 @@
       </c>
     </row>
     <row r="10" spans="1:15">
-      <c r="A10" s="10"/>
+      <c r="A10" s="11"/>
       <c r="B10">
         <v>8</v>
       </c>
@@ -1199,7 +1202,7 @@
         <f t="shared" si="3"/>
         <v>92.010929920000009</v>
       </c>
-      <c r="I10" s="10"/>
+      <c r="I10" s="11"/>
       <c r="J10">
         <v>8</v>
       </c>
@@ -1218,7 +1221,7 @@
       </c>
     </row>
     <row r="11" spans="1:15">
-      <c r="A11" s="10"/>
+      <c r="A11" s="11"/>
       <c r="B11">
         <v>9</v>
       </c>
@@ -1236,7 +1239,7 @@
         <f t="shared" si="3"/>
         <v>90.17071132160001</v>
       </c>
-      <c r="I11" s="10"/>
+      <c r="I11" s="11"/>
       <c r="J11">
         <v>9</v>
       </c>
@@ -1255,7 +1258,7 @@
       </c>
     </row>
     <row r="12" spans="1:15">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="11" t="s">
         <v>45</v>
       </c>
       <c r="B12">
@@ -1275,7 +1278,7 @@
         <f t="shared" si="3"/>
         <v>106.04075651420162</v>
       </c>
-      <c r="I12" s="10" t="s">
+      <c r="I12" s="11" t="s">
         <v>45</v>
       </c>
       <c r="J12">
@@ -1296,7 +1299,7 @@
       </c>
     </row>
     <row r="13" spans="1:15">
-      <c r="A13" s="10"/>
+      <c r="A13" s="11"/>
       <c r="B13">
         <v>11</v>
       </c>
@@ -1314,7 +1317,7 @@
         <f t="shared" si="3"/>
         <v>103.38973760134657</v>
       </c>
-      <c r="I13" s="10"/>
+      <c r="I13" s="11"/>
       <c r="J13">
         <v>11</v>
       </c>
@@ -1333,7 +1336,7 @@
       </c>
     </row>
     <row r="14" spans="1:15">
-      <c r="A14" s="10"/>
+      <c r="A14" s="11"/>
       <c r="B14">
         <v>12</v>
       </c>
@@ -1351,7 +1354,7 @@
         <f t="shared" si="3"/>
         <v>100.80499416131291</v>
       </c>
-      <c r="I14" s="10"/>
+      <c r="I14" s="11"/>
       <c r="J14">
         <v>12</v>
       </c>
@@ -1370,7 +1373,7 @@
       </c>
     </row>
     <row r="15" spans="1:15">
-      <c r="A15" s="10"/>
+      <c r="A15" s="11"/>
       <c r="B15">
         <v>13</v>
       </c>
@@ -1388,7 +1391,7 @@
         <f t="shared" si="3"/>
         <v>98.284869307280076</v>
       </c>
-      <c r="I15" s="10"/>
+      <c r="I15" s="11"/>
       <c r="J15">
         <v>13</v>
       </c>
@@ -1407,7 +1410,7 @@
       </c>
     </row>
     <row r="16" spans="1:15">
-      <c r="A16" s="10"/>
+      <c r="A16" s="11"/>
       <c r="B16">
         <v>14</v>
       </c>
@@ -1425,7 +1428,7 @@
         <f t="shared" si="3"/>
         <v>95.827747574598078</v>
       </c>
-      <c r="I16" s="10"/>
+      <c r="I16" s="11"/>
       <c r="J16">
         <v>14</v>
       </c>
@@ -1444,7 +1447,7 @@
       </c>
     </row>
     <row r="17" spans="1:15">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="11" t="s">
         <v>46</v>
       </c>
       <c r="B17">
@@ -1464,7 +1467,7 @@
         <f t="shared" si="3"/>
         <v>109.0040628661053</v>
       </c>
-      <c r="I17" s="10" t="s">
+      <c r="I17" s="11" t="s">
         <v>46</v>
       </c>
       <c r="J17">
@@ -1485,7 +1488,7 @@
       </c>
     </row>
     <row r="18" spans="1:15">
-      <c r="A18" s="10"/>
+      <c r="A18" s="11"/>
       <c r="B18">
         <v>16</v>
       </c>
@@ -1503,7 +1506,7 @@
         <f t="shared" si="3"/>
         <v>105.73394098012214</v>
       </c>
-      <c r="I18" s="10"/>
+      <c r="I18" s="11"/>
       <c r="J18">
         <v>16</v>
       </c>
@@ -1522,7 +1525,7 @@
       </c>
     </row>
     <row r="19" spans="1:15">
-      <c r="A19" s="10"/>
+      <c r="A19" s="11"/>
       <c r="B19">
         <v>17</v>
       </c>
@@ -1540,7 +1543,7 @@
         <f t="shared" si="3"/>
         <v>102.56192275071849</v>
       </c>
-      <c r="I19" s="10"/>
+      <c r="I19" s="11"/>
       <c r="J19">
         <v>17</v>
       </c>
@@ -1559,7 +1562,7 @@
       </c>
     </row>
     <row r="20" spans="1:15">
-      <c r="A20" s="10"/>
+      <c r="A20" s="11"/>
       <c r="B20">
         <v>18</v>
       </c>
@@ -1577,7 +1580,7 @@
         <f t="shared" si="3"/>
         <v>99.485065068196931</v>
       </c>
-      <c r="I20" s="10"/>
+      <c r="I20" s="11"/>
       <c r="J20">
         <v>18</v>
       </c>
@@ -1596,7 +1599,7 @@
       </c>
     </row>
     <row r="21" spans="1:15">
-      <c r="A21" s="10"/>
+      <c r="A21" s="11"/>
       <c r="B21">
         <v>19</v>
       </c>
@@ -1614,7 +1617,7 @@
         <f t="shared" si="3"/>
         <v>96.500513116151041</v>
       </c>
-      <c r="I21" s="10"/>
+      <c r="I21" s="11"/>
       <c r="J21">
         <v>19</v>
       </c>
@@ -1633,7 +1636,7 @@
       </c>
     </row>
     <row r="22" spans="1:15">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="11" t="s">
         <v>9</v>
       </c>
       <c r="B22">
@@ -1653,7 +1656,7 @@
         <f t="shared" si="3"/>
         <v>100.29160470285697</v>
       </c>
-      <c r="I22" s="10" t="s">
+      <c r="I22" s="11" t="s">
         <v>9</v>
       </c>
       <c r="J22">
@@ -1674,7 +1677,7 @@
       </c>
     </row>
     <row r="23" spans="1:15">
-      <c r="A23" s="10"/>
+      <c r="A23" s="11"/>
       <c r="B23">
         <v>21</v>
       </c>
@@ -1692,7 +1695,7 @@
         <f t="shared" si="3"/>
         <v>99.288688655828395</v>
       </c>
-      <c r="I23" s="10"/>
+      <c r="I23" s="11"/>
       <c r="J23">
         <v>21</v>
       </c>
@@ -1711,7 +1714,7 @@
       </c>
     </row>
     <row r="24" spans="1:15">
-      <c r="A24" s="10"/>
+      <c r="A24" s="11"/>
       <c r="B24">
         <v>22</v>
       </c>
@@ -1729,7 +1732,7 @@
         <f t="shared" si="3"/>
         <v>98.295801769270113</v>
       </c>
-      <c r="I24" s="10"/>
+      <c r="I24" s="11"/>
       <c r="J24">
         <v>22</v>
       </c>
@@ -1748,7 +1751,7 @@
       </c>
     </row>
     <row r="25" spans="1:15">
-      <c r="A25" s="10"/>
+      <c r="A25" s="11"/>
       <c r="B25">
         <v>23</v>
       </c>
@@ -1766,7 +1769,7 @@
         <f t="shared" si="3"/>
         <v>97.312843751577418</v>
       </c>
-      <c r="I25" s="10"/>
+      <c r="I25" s="11"/>
       <c r="J25">
         <v>23</v>
       </c>
@@ -1785,7 +1788,7 @@
       </c>
     </row>
     <row r="26" spans="1:15">
-      <c r="A26" s="10"/>
+      <c r="A26" s="11"/>
       <c r="B26">
         <v>24</v>
       </c>
@@ -1803,7 +1806,7 @@
         <f t="shared" si="3"/>
         <v>96.339715314061635</v>
       </c>
-      <c r="I26" s="10"/>
+      <c r="I26" s="11"/>
       <c r="J26">
         <v>24</v>
       </c>
@@ -1822,7 +1825,7 @@
       </c>
     </row>
     <row r="27" spans="1:15">
-      <c r="A27" s="10" t="s">
+      <c r="A27" s="11" t="s">
         <v>19</v>
       </c>
       <c r="B27">
@@ -1842,7 +1845,7 @@
         <f t="shared" si="3"/>
         <v>25.433684842912271</v>
       </c>
-      <c r="I27" s="10" t="s">
+      <c r="I27" s="11" t="s">
         <v>19</v>
       </c>
       <c r="J27">
@@ -1863,7 +1866,7 @@
       </c>
     </row>
     <row r="28" spans="1:15">
-      <c r="A28" s="10"/>
+      <c r="A28" s="11"/>
       <c r="B28">
         <v>26</v>
       </c>
@@ -1881,7 +1884,7 @@
         <f t="shared" si="3"/>
         <v>17.803579390038589</v>
       </c>
-      <c r="I28" s="10"/>
+      <c r="I28" s="11"/>
       <c r="J28">
         <v>26</v>
       </c>
@@ -1900,7 +1903,7 @@
       </c>
     </row>
     <row r="29" spans="1:15">
-      <c r="A29" s="10"/>
+      <c r="A29" s="11"/>
       <c r="B29">
         <v>27</v>
       </c>
@@ -1918,7 +1921,7 @@
         <f t="shared" si="3"/>
         <v>12.462505573027014</v>
       </c>
-      <c r="I29" s="10"/>
+      <c r="I29" s="11"/>
       <c r="J29">
         <v>27</v>
       </c>
@@ -1937,7 +1940,7 @@
       </c>
     </row>
     <row r="30" spans="1:15">
-      <c r="A30" s="10"/>
+      <c r="A30" s="11"/>
       <c r="B30">
         <v>28</v>
       </c>
@@ -1955,7 +1958,7 @@
         <f t="shared" si="3"/>
         <v>8.7237539011189096</v>
       </c>
-      <c r="I30" s="10"/>
+      <c r="I30" s="11"/>
       <c r="J30">
         <v>28</v>
       </c>
@@ -1974,7 +1977,7 @@
       </c>
     </row>
     <row r="31" spans="1:15">
-      <c r="A31" s="10"/>
+      <c r="A31" s="11"/>
       <c r="B31">
         <v>29</v>
       </c>
@@ -1992,7 +1995,7 @@
         <f t="shared" si="3"/>
         <v>6.1066277307832371</v>
       </c>
-      <c r="I31" s="10"/>
+      <c r="I31" s="11"/>
       <c r="J31">
         <v>29</v>
       </c>
@@ -2011,7 +2014,7 @@
       </c>
     </row>
     <row r="32" spans="1:15">
-      <c r="A32" s="10"/>
+      <c r="A32" s="11"/>
       <c r="B32">
         <v>30</v>
       </c>
@@ -2029,7 +2032,7 @@
         <f t="shared" si="3"/>
         <v>4.2746394115482662</v>
       </c>
-      <c r="I32" s="10"/>
+      <c r="I32" s="11"/>
       <c r="J32">
         <v>30</v>
       </c>
@@ -2040,7 +2043,7 @@
         <v>0</v>
       </c>
       <c r="N32" s="1">
-        <f t="shared" si="1"/>
+        <f xml:space="preserve"> N31-(N31*L31)</f>
         <v>11.191206979698018</v>
       </c>
       <c r="O32">
@@ -2048,346 +2051,379 @@
       </c>
     </row>
     <row r="33" spans="1:15">
-      <c r="A33" t="s">
+      <c r="A33" s="10"/>
+      <c r="B33">
+        <v>31</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33" s="1">
+        <v>0</v>
+      </c>
+      <c r="G33" s="1">
+        <v>0</v>
+      </c>
+      <c r="I33" s="10"/>
+      <c r="J33">
+        <v>31</v>
+      </c>
+      <c r="L33">
+        <v>0</v>
+      </c>
+      <c r="M33">
+        <v>0</v>
+      </c>
+      <c r="N33" s="1">
+        <v>0</v>
+      </c>
+      <c r="O33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15">
+      <c r="A34" t="s">
         <v>63</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
         <v>64</v>
       </c>
-      <c r="G33">
+      <c r="G34">
         <f xml:space="preserve"> SUM(G7:G32)</f>
         <v>2053.6022002246564</v>
       </c>
     </row>
-    <row r="35" spans="1:15">
-      <c r="B35" t="s">
-        <v>15</v>
-      </c>
-      <c r="J35" t="s">
-        <v>15</v>
-      </c>
-    </row>
     <row r="36" spans="1:15">
       <c r="B36" t="s">
+        <v>15</v>
+      </c>
+      <c r="J36" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15">
+      <c r="B37" t="s">
         <v>16</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C37" t="s">
         <v>17</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D37" t="s">
         <v>18</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E37" t="s">
         <v>9</v>
       </c>
-      <c r="F36" t="s">
+      <c r="F37" t="s">
         <v>19</v>
       </c>
-      <c r="J36" t="s">
+      <c r="J37" t="s">
         <v>16</v>
       </c>
-      <c r="K36" t="s">
+      <c r="K37" t="s">
         <v>17</v>
       </c>
-      <c r="L36" t="s">
+      <c r="L37" t="s">
         <v>18</v>
       </c>
-      <c r="M36" t="s">
+      <c r="M37" t="s">
         <v>9</v>
       </c>
-      <c r="N36" t="s">
+      <c r="N37" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="1:15">
-      <c r="B37" s="1">
+    <row r="38" spans="1:15">
+      <c r="B38" s="1">
         <f xml:space="preserve"> SUM(F7:F11)</f>
         <v>939.27029048320014</v>
       </c>
-      <c r="C37" s="1">
+      <c r="C38" s="1">
         <f xml:space="preserve"> SUM(F12:F16)</f>
         <v>840.58017526456536</v>
       </c>
-      <c r="D37" s="1">
+      <c r="D38" s="1">
         <f xml:space="preserve"> SUM(F17:F21)</f>
         <v>733.26500683041991</v>
       </c>
-      <c r="E37" s="1">
+      <c r="E38" s="1">
         <f xml:space="preserve"> SUM(F22:F26)</f>
         <v>655.37153892479273</v>
       </c>
-      <c r="F37" s="1">
+      <c r="F38" s="1">
         <f xml:space="preserve"> SUM(F27:F32)</f>
         <v>374.02395424714138</v>
       </c>
-      <c r="G37" s="1">
-        <f xml:space="preserve"> SUM(B37:F37)</f>
+      <c r="G38" s="1">
+        <f xml:space="preserve"> SUM(B38:F38)</f>
         <v>3542.5109657501193</v>
       </c>
-      <c r="J37" s="1">
+      <c r="J38" s="1">
         <f xml:space="preserve"> SUM(N9:N11)</f>
         <v>600.56913027224243</v>
       </c>
-      <c r="K37" s="1">
+      <c r="K38" s="1">
         <f xml:space="preserve"> SUM(N12:N16)</f>
         <v>806.72366821742844</v>
       </c>
-      <c r="L37" s="1">
+      <c r="L38" s="1">
         <f xml:space="preserve"> SUM(N17:N21)</f>
         <v>590.60577424751023</v>
       </c>
-      <c r="M37" s="1">
+      <c r="M38" s="1">
         <f xml:space="preserve"> SUM(N22:N26)</f>
         <v>298.1302273304463</v>
       </c>
-      <c r="N37" s="1">
+      <c r="N38" s="1">
         <f xml:space="preserve"> SUM(N27:N32)</f>
         <v>125.9994387391977</v>
       </c>
-      <c r="O37" s="1">
-        <f xml:space="preserve"> SUM(J37:N37)</f>
+      <c r="O38" s="1">
+        <f xml:space="preserve"> SUM(J38:N38)</f>
         <v>2422.0282388068249</v>
       </c>
     </row>
-    <row r="38" spans="1:15">
-      <c r="B38">
-        <f t="shared" ref="B38:G38" si="6">(B37/$G$37)</f>
+    <row r="39" spans="1:15">
+      <c r="B39">
+        <f t="shared" ref="B39:G39" si="6">(B38/$G$38)</f>
         <v>0.26514252166451985</v>
       </c>
-      <c r="C38">
+      <c r="C39">
         <f t="shared" si="6"/>
         <v>0.23728371863672532</v>
       </c>
-      <c r="D38">
+      <c r="D39">
         <f t="shared" si="6"/>
         <v>0.20699018688151119</v>
       </c>
-      <c r="E38">
+      <c r="E39">
         <f t="shared" si="6"/>
         <v>0.1850019788960679</v>
       </c>
-      <c r="F38">
+      <c r="F39">
         <f t="shared" si="6"/>
         <v>0.10558159392117579</v>
       </c>
-      <c r="G38">
+      <c r="G39">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="J38">
-        <f t="shared" ref="J38:O38" si="7">(J37/$O$37)</f>
+      <c r="J39">
+        <f t="shared" ref="J39:O39" si="7">(J38/$O$38)</f>
         <v>0.24796124200769171</v>
       </c>
-      <c r="K38">
+      <c r="K39">
         <f t="shared" si="7"/>
         <v>0.33307773018156406</v>
       </c>
-      <c r="L38">
+      <c r="L39">
         <f t="shared" si="7"/>
         <v>0.24384760044683174</v>
       </c>
-      <c r="M38">
+      <c r="M39">
         <f t="shared" si="7"/>
         <v>0.12309114425408829</v>
       </c>
-      <c r="N38">
+      <c r="N39">
         <f t="shared" si="7"/>
         <v>5.2022283109824263E-2</v>
       </c>
-      <c r="O38">
+      <c r="O39">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:15">
-      <c r="B39">
+    <row r="40" spans="1:15">
+      <c r="B40">
         <v>0.26514252166451985</v>
       </c>
-      <c r="C39">
-        <f xml:space="preserve"> C38 + B39</f>
+      <c r="C40">
+        <f xml:space="preserve"> C39 + B40</f>
         <v>0.50242624030124516</v>
       </c>
-      <c r="D39">
-        <f xml:space="preserve"> D38 + C39</f>
+      <c r="D40">
+        <f xml:space="preserve"> D39 + C40</f>
         <v>0.70941642718275633</v>
       </c>
-      <c r="E39">
-        <f xml:space="preserve"> E38 + D39</f>
+      <c r="E40">
+        <f xml:space="preserve"> E39 + D40</f>
         <v>0.89441840607882428</v>
       </c>
-      <c r="F39">
-        <f t="shared" ref="F39:G39" si="8" xml:space="preserve"> F38 + E39</f>
-        <v>1</v>
-      </c>
-      <c r="G39">
+      <c r="F40">
+        <f t="shared" ref="F40:G40" si="8" xml:space="preserve"> F39 + E40</f>
+        <v>1</v>
+      </c>
+      <c r="G40">
         <f t="shared" si="8"/>
         <v>2</v>
       </c>
-      <c r="J39">
+      <c r="J40">
         <v>0.24796099999999999</v>
       </c>
-      <c r="K39">
-        <f xml:space="preserve"> K38 + J39</f>
+      <c r="K40">
+        <f xml:space="preserve"> K39 + J40</f>
         <v>0.58103873018156404</v>
       </c>
-      <c r="L39">
-        <f xml:space="preserve"> L38 + K39</f>
+      <c r="L40">
+        <f xml:space="preserve"> L39 + K40</f>
         <v>0.82488633062839578</v>
       </c>
-      <c r="M39">
-        <f xml:space="preserve"> M38 + L39</f>
+      <c r="M40">
+        <f xml:space="preserve"> M39 + L40</f>
         <v>0.94797747488248407</v>
       </c>
-      <c r="N39">
-        <f xml:space="preserve"> N38 + M39</f>
+      <c r="N40">
+        <f xml:space="preserve"> N39 + M40</f>
         <v>0.99999975799230834</v>
       </c>
     </row>
-    <row r="41" spans="1:15" ht="43.5" customHeight="1">
-      <c r="B41" s="10" t="s">
+    <row r="42" spans="1:15" ht="43.5" customHeight="1">
+      <c r="B42" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C41" s="10"/>
-      <c r="D41" s="10"/>
-      <c r="E41" s="10"/>
-      <c r="J41" s="10" t="s">
+      <c r="C42" s="11"/>
+      <c r="D42" s="11"/>
+      <c r="E42" s="11"/>
+      <c r="J42" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="K41" s="10"/>
-      <c r="L41" s="10"/>
-      <c r="M41" s="10"/>
-    </row>
-    <row r="42" spans="1:15" ht="56">
-      <c r="B42" s="2" t="s">
+      <c r="K42" s="11"/>
+      <c r="L42" s="11"/>
+      <c r="M42" s="11"/>
+    </row>
+    <row r="43" spans="1:15" ht="56">
+      <c r="B43" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C43" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="J42" s="2" t="s">
+      <c r="J43" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="K42" s="2" t="s">
+      <c r="K43" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="43" spans="1:15">
-      <c r="B43" t="s">
+    <row r="44" spans="1:15">
+      <c r="B44" t="s">
         <v>54</v>
       </c>
-      <c r="C43" s="7">
+      <c r="C44" s="7">
         <v>1.2</v>
       </c>
-      <c r="J43" t="s">
+      <c r="J44" t="s">
         <v>54</v>
       </c>
-      <c r="K43" s="7">
+      <c r="K44" s="7">
         <v>0.8</v>
-      </c>
-    </row>
-    <row r="44" spans="1:15">
-      <c r="B44" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C44" s="7">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="J44" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="K44" s="7">
-        <v>0.9</v>
       </c>
     </row>
     <row r="45" spans="1:15">
       <c r="B45" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C45" s="7">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="J45" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K45" s="7">
-        <v>1</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="46" spans="1:15">
       <c r="B46" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C46" s="7">
+        <v>1</v>
+      </c>
+      <c r="J46" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="K46" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15">
+      <c r="B47" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C46" s="7">
+      <c r="C47" s="7">
         <v>0.9</v>
       </c>
-      <c r="J46" s="8" t="s">
+      <c r="J47" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="K46" s="7">
+      <c r="K47" s="7">
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="48" spans="1:15" ht="45" customHeight="1">
-      <c r="B48" s="10" t="s">
+    <row r="49" spans="2:5" ht="45" customHeight="1">
+      <c r="B49" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="C48" s="10"/>
-      <c r="D48" s="10"/>
-      <c r="E48" s="10"/>
-    </row>
-    <row r="49" spans="2:3" ht="56">
-      <c r="B49" s="2" t="s">
+      <c r="C49" s="11"/>
+      <c r="D49" s="11"/>
+      <c r="E49" s="11"/>
+    </row>
+    <row r="50" spans="2:5" ht="56">
+      <c r="B50" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="C50" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="50" spans="2:3">
-      <c r="B50" t="s">
+    <row r="51" spans="2:5">
+      <c r="B51" t="s">
         <v>54</v>
       </c>
-      <c r="C50" s="7">
+      <c r="C51" s="7">
         <v>1.2</v>
       </c>
     </row>
-    <row r="51" spans="2:3">
-      <c r="B51" s="8" t="s">
+    <row r="52" spans="2:5">
+      <c r="B52" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="C51" s="7">
+      <c r="C52" s="7">
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="52" spans="2:3">
-      <c r="B52" s="8" t="s">
+    <row r="53" spans="2:5">
+      <c r="B53" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C52" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="2:3">
-      <c r="B53" s="8" t="s">
+      <c r="C53" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5">
+      <c r="B54" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C53" s="7">
+      <c r="C54" s="7">
         <v>0.9</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="I9:I11"/>
+    <mergeCell ref="I12:I16"/>
     <mergeCell ref="A17:A21"/>
     <mergeCell ref="A22:A26"/>
     <mergeCell ref="A27:A32"/>
     <mergeCell ref="I27:I32"/>
     <mergeCell ref="I17:I21"/>
     <mergeCell ref="I22:I26"/>
-    <mergeCell ref="I12:I16"/>
-    <mergeCell ref="B41:E41"/>
-    <mergeCell ref="J41:M41"/>
-    <mergeCell ref="B48:E48"/>
+    <mergeCell ref="B42:E42"/>
+    <mergeCell ref="J42:M42"/>
+    <mergeCell ref="B49:E49"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="I1:J1"/>
@@ -2400,6 +2436,7 @@
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="I7:I8"/>
+    <mergeCell ref="I9:I11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2430,17 +2467,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="27" customHeight="1">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
     </row>
     <row r="2" spans="1:18" ht="112">
       <c r="A2" s="2" t="s">
@@ -2495,7 +2532,7 @@
       </c>
     </row>
     <row r="4" spans="1:18">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="11" t="s">
         <v>41</v>
       </c>
       <c r="B4">
@@ -2521,7 +2558,7 @@
       </c>
     </row>
     <row r="5" spans="1:18">
-      <c r="A5" s="10"/>
+      <c r="A5" s="11"/>
       <c r="B5">
         <v>3</v>
       </c>
@@ -2545,7 +2582,7 @@
       </c>
     </row>
     <row r="6" spans="1:18">
-      <c r="A6" s="10"/>
+      <c r="A6" s="11"/>
       <c r="B6">
         <v>4</v>
       </c>
@@ -2566,7 +2603,7 @@
       </c>
     </row>
     <row r="7" spans="1:18" ht="15" customHeight="1">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="11" t="s">
         <v>44</v>
       </c>
       <c r="B7">
@@ -2589,7 +2626,7 @@
       </c>
     </row>
     <row r="8" spans="1:18">
-      <c r="A8" s="10"/>
+      <c r="A8" s="11"/>
       <c r="B8">
         <v>6</v>
       </c>
@@ -2610,7 +2647,7 @@
       </c>
     </row>
     <row r="9" spans="1:18" ht="15" customHeight="1">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="11" t="s">
         <v>43</v>
       </c>
       <c r="B9">
@@ -2633,7 +2670,7 @@
       </c>
     </row>
     <row r="10" spans="1:18">
-      <c r="A10" s="10"/>
+      <c r="A10" s="11"/>
       <c r="B10">
         <v>8</v>
       </c>
@@ -2654,7 +2691,7 @@
       </c>
     </row>
     <row r="11" spans="1:18">
-      <c r="A11" s="10"/>
+      <c r="A11" s="11"/>
       <c r="B11">
         <v>9</v>
       </c>
@@ -2675,7 +2712,7 @@
       </c>
     </row>
     <row r="12" spans="1:18" ht="15" customHeight="1">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="11" t="s">
         <v>45</v>
       </c>
       <c r="B12">
@@ -2698,7 +2735,7 @@
       </c>
     </row>
     <row r="13" spans="1:18">
-      <c r="A13" s="10"/>
+      <c r="A13" s="11"/>
       <c r="B13">
         <v>11</v>
       </c>
@@ -2719,7 +2756,7 @@
       </c>
     </row>
     <row r="14" spans="1:18">
-      <c r="A14" s="10"/>
+      <c r="A14" s="11"/>
       <c r="B14">
         <v>12</v>
       </c>
@@ -2740,7 +2777,7 @@
       </c>
     </row>
     <row r="15" spans="1:18">
-      <c r="A15" s="10"/>
+      <c r="A15" s="11"/>
       <c r="B15">
         <v>13</v>
       </c>
@@ -2761,7 +2798,7 @@
       </c>
     </row>
     <row r="16" spans="1:18">
-      <c r="A16" s="10"/>
+      <c r="A16" s="11"/>
       <c r="B16">
         <v>14</v>
       </c>
@@ -2782,7 +2819,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="15" customHeight="1">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="11" t="s">
         <v>46</v>
       </c>
       <c r="B17">
@@ -2805,7 +2842,7 @@
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="10"/>
+      <c r="A18" s="11"/>
       <c r="B18">
         <v>16</v>
       </c>
@@ -2826,7 +2863,7 @@
       </c>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="10"/>
+      <c r="A19" s="11"/>
       <c r="B19">
         <v>17</v>
       </c>
@@ -2847,7 +2884,7 @@
       </c>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="10"/>
+      <c r="A20" s="11"/>
       <c r="B20">
         <v>18</v>
       </c>
@@ -2868,7 +2905,7 @@
       </c>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="10"/>
+      <c r="A21" s="11"/>
       <c r="B21">
         <v>19</v>
       </c>
@@ -2889,7 +2926,7 @@
       </c>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="11" t="s">
         <v>9</v>
       </c>
       <c r="B22">
@@ -2912,7 +2949,7 @@
       </c>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="10"/>
+      <c r="A23" s="11"/>
       <c r="B23">
         <v>21</v>
       </c>
@@ -2933,7 +2970,7 @@
       </c>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="10"/>
+      <c r="A24" s="11"/>
       <c r="B24">
         <v>22</v>
       </c>
@@ -2954,7 +2991,7 @@
       </c>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="10"/>
+      <c r="A25" s="11"/>
       <c r="B25">
         <v>23</v>
       </c>
@@ -2975,7 +3012,7 @@
       </c>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="10"/>
+      <c r="A26" s="11"/>
       <c r="B26">
         <v>24</v>
       </c>
@@ -2996,7 +3033,7 @@
       </c>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="10" t="s">
+      <c r="A27" s="11" t="s">
         <v>19</v>
       </c>
       <c r="B27">
@@ -3019,7 +3056,7 @@
       </c>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="10"/>
+      <c r="A28" s="11"/>
       <c r="B28">
         <v>26</v>
       </c>
@@ -3040,7 +3077,7 @@
       </c>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="10"/>
+      <c r="A29" s="11"/>
       <c r="B29">
         <v>27</v>
       </c>
@@ -3061,7 +3098,7 @@
       </c>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="10"/>
+      <c r="A30" s="11"/>
       <c r="B30">
         <v>28</v>
       </c>
@@ -3082,7 +3119,7 @@
       </c>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="10"/>
+      <c r="A31" s="11"/>
       <c r="B31">
         <v>29</v>
       </c>
@@ -3103,7 +3140,7 @@
       </c>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="10"/>
+      <c r="A32" s="11"/>
       <c r="B32">
         <v>30</v>
       </c>
@@ -3132,17 +3169,17 @@
       <c r="C34" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D34" s="10" t="s">
+      <c r="D34" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="E34" s="10"/>
+      <c r="E34" s="11"/>
       <c r="F34" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="L34" s="10" t="s">
+      <c r="L34" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="M34" s="10"/>
+      <c r="M34" s="11"/>
       <c r="N34" s="2" t="s">
         <v>55</v>
       </c>
@@ -3250,7 +3287,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
@@ -3265,15 +3302,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="49.5" customHeight="1">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="2" t="s">
@@ -3410,13 +3447,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="14"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="15"/>
     </row>
     <row r="2" spans="1:5" ht="56">
       <c r="A2" s="2" t="s">

</xml_diff>

<commit_message>
fixed life table so that all males also die at age 30
</commit_message>
<xml_diff>
--- a/Excel Files/life_table.xlsx
+++ b/Excel Files/life_table.xlsx
@@ -484,8 +484,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -537,19 +539,21 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -849,10 +853,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O54"/>
+  <dimension ref="A1:O55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="L34" sqref="L34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2072,7 +2076,7 @@
         <v>31</v>
       </c>
       <c r="L33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M33">
         <v>0</v>
@@ -2085,330 +2089,364 @@
       </c>
     </row>
     <row r="34" spans="1:15">
-      <c r="A34" t="s">
+      <c r="A34" s="10"/>
+      <c r="B34">
+        <v>32</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34" s="1">
+        <v>0</v>
+      </c>
+      <c r="G34" s="1">
+        <v>0</v>
+      </c>
+      <c r="I34" s="10"/>
+      <c r="J34">
+        <v>32</v>
+      </c>
+      <c r="L34">
+        <v>1</v>
+      </c>
+      <c r="M34">
+        <v>0</v>
+      </c>
+      <c r="N34" s="1">
+        <v>0</v>
+      </c>
+      <c r="O34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15">
+      <c r="A35" t="s">
         <v>63</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B35" t="s">
         <v>64</v>
       </c>
-      <c r="G34">
+      <c r="G35">
         <f xml:space="preserve"> SUM(G7:G32)</f>
         <v>2053.6022002246564</v>
       </c>
     </row>
-    <row r="36" spans="1:15">
-      <c r="B36" t="s">
-        <v>15</v>
-      </c>
-      <c r="J36" t="s">
-        <v>15</v>
-      </c>
-    </row>
     <row r="37" spans="1:15">
       <c r="B37" t="s">
+        <v>15</v>
+      </c>
+      <c r="J37" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15">
+      <c r="B38" t="s">
         <v>16</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C38" t="s">
         <v>17</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D38" t="s">
         <v>18</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E38" t="s">
         <v>9</v>
       </c>
-      <c r="F37" t="s">
+      <c r="F38" t="s">
         <v>19</v>
       </c>
-      <c r="J37" t="s">
+      <c r="J38" t="s">
         <v>16</v>
       </c>
-      <c r="K37" t="s">
+      <c r="K38" t="s">
         <v>17</v>
       </c>
-      <c r="L37" t="s">
+      <c r="L38" t="s">
         <v>18</v>
       </c>
-      <c r="M37" t="s">
+      <c r="M38" t="s">
         <v>9</v>
       </c>
-      <c r="N37" t="s">
+      <c r="N38" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="38" spans="1:15">
-      <c r="B38" s="1">
+    <row r="39" spans="1:15">
+      <c r="B39" s="1">
         <f xml:space="preserve"> SUM(F7:F11)</f>
         <v>939.27029048320014</v>
       </c>
-      <c r="C38" s="1">
+      <c r="C39" s="1">
         <f xml:space="preserve"> SUM(F12:F16)</f>
         <v>840.58017526456536</v>
       </c>
-      <c r="D38" s="1">
+      <c r="D39" s="1">
         <f xml:space="preserve"> SUM(F17:F21)</f>
         <v>733.26500683041991</v>
       </c>
-      <c r="E38" s="1">
+      <c r="E39" s="1">
         <f xml:space="preserve"> SUM(F22:F26)</f>
         <v>655.37153892479273</v>
       </c>
-      <c r="F38" s="1">
+      <c r="F39" s="1">
         <f xml:space="preserve"> SUM(F27:F32)</f>
         <v>374.02395424714138</v>
       </c>
-      <c r="G38" s="1">
-        <f xml:space="preserve"> SUM(B38:F38)</f>
+      <c r="G39" s="1">
+        <f xml:space="preserve"> SUM(B39:F39)</f>
         <v>3542.5109657501193</v>
       </c>
-      <c r="J38" s="1">
+      <c r="J39" s="1">
         <f xml:space="preserve"> SUM(N9:N11)</f>
         <v>600.56913027224243</v>
       </c>
-      <c r="K38" s="1">
+      <c r="K39" s="1">
         <f xml:space="preserve"> SUM(N12:N16)</f>
         <v>806.72366821742844</v>
       </c>
-      <c r="L38" s="1">
+      <c r="L39" s="1">
         <f xml:space="preserve"> SUM(N17:N21)</f>
         <v>590.60577424751023</v>
       </c>
-      <c r="M38" s="1">
+      <c r="M39" s="1">
         <f xml:space="preserve"> SUM(N22:N26)</f>
         <v>298.1302273304463</v>
       </c>
-      <c r="N38" s="1">
+      <c r="N39" s="1">
         <f xml:space="preserve"> SUM(N27:N32)</f>
         <v>125.9994387391977</v>
       </c>
-      <c r="O38" s="1">
-        <f xml:space="preserve"> SUM(J38:N38)</f>
+      <c r="O39" s="1">
+        <f xml:space="preserve"> SUM(J39:N39)</f>
         <v>2422.0282388068249</v>
       </c>
     </row>
-    <row r="39" spans="1:15">
-      <c r="B39">
-        <f t="shared" ref="B39:G39" si="6">(B38/$G$38)</f>
+    <row r="40" spans="1:15">
+      <c r="B40">
+        <f t="shared" ref="B40:G40" si="6">(B39/$G$39)</f>
         <v>0.26514252166451985</v>
       </c>
-      <c r="C39">
+      <c r="C40">
         <f t="shared" si="6"/>
         <v>0.23728371863672532</v>
       </c>
-      <c r="D39">
+      <c r="D40">
         <f t="shared" si="6"/>
         <v>0.20699018688151119</v>
       </c>
-      <c r="E39">
+      <c r="E40">
         <f t="shared" si="6"/>
         <v>0.1850019788960679</v>
       </c>
-      <c r="F39">
+      <c r="F40">
         <f t="shared" si="6"/>
         <v>0.10558159392117579</v>
       </c>
-      <c r="G39">
+      <c r="G40">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="J39">
-        <f t="shared" ref="J39:O39" si="7">(J38/$O$38)</f>
+      <c r="J40">
+        <f t="shared" ref="J40:O40" si="7">(J39/$O$39)</f>
         <v>0.24796124200769171</v>
       </c>
-      <c r="K39">
+      <c r="K40">
         <f t="shared" si="7"/>
         <v>0.33307773018156406</v>
       </c>
-      <c r="L39">
+      <c r="L40">
         <f t="shared" si="7"/>
         <v>0.24384760044683174</v>
       </c>
-      <c r="M39">
+      <c r="M40">
         <f t="shared" si="7"/>
         <v>0.12309114425408829</v>
       </c>
-      <c r="N39">
+      <c r="N40">
         <f t="shared" si="7"/>
         <v>5.2022283109824263E-2</v>
       </c>
-      <c r="O39">
+      <c r="O40">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:15">
-      <c r="B40">
+    <row r="41" spans="1:15">
+      <c r="B41">
         <v>0.26514252166451985</v>
       </c>
-      <c r="C40">
-        <f xml:space="preserve"> C39 + B40</f>
+      <c r="C41">
+        <f xml:space="preserve"> C40 + B41</f>
         <v>0.50242624030124516</v>
       </c>
-      <c r="D40">
-        <f xml:space="preserve"> D39 + C40</f>
+      <c r="D41">
+        <f xml:space="preserve"> D40 + C41</f>
         <v>0.70941642718275633</v>
       </c>
-      <c r="E40">
-        <f xml:space="preserve"> E39 + D40</f>
+      <c r="E41">
+        <f xml:space="preserve"> E40 + D41</f>
         <v>0.89441840607882428</v>
       </c>
-      <c r="F40">
-        <f t="shared" ref="F40:G40" si="8" xml:space="preserve"> F39 + E40</f>
-        <v>1</v>
-      </c>
-      <c r="G40">
+      <c r="F41">
+        <f t="shared" ref="F41:G41" si="8" xml:space="preserve"> F40 + E41</f>
+        <v>1</v>
+      </c>
+      <c r="G41">
         <f t="shared" si="8"/>
         <v>2</v>
       </c>
-      <c r="J40">
+      <c r="J41">
         <v>0.24796099999999999</v>
       </c>
-      <c r="K40">
-        <f xml:space="preserve"> K39 + J40</f>
+      <c r="K41">
+        <f xml:space="preserve"> K40 + J41</f>
         <v>0.58103873018156404</v>
       </c>
-      <c r="L40">
-        <f xml:space="preserve"> L39 + K40</f>
+      <c r="L41">
+        <f xml:space="preserve"> L40 + K41</f>
         <v>0.82488633062839578</v>
       </c>
-      <c r="M40">
-        <f xml:space="preserve"> M39 + L40</f>
+      <c r="M41">
+        <f xml:space="preserve"> M40 + L41</f>
         <v>0.94797747488248407</v>
       </c>
-      <c r="N40">
-        <f xml:space="preserve"> N39 + M40</f>
+      <c r="N41">
+        <f xml:space="preserve"> N40 + M41</f>
         <v>0.99999975799230834</v>
       </c>
     </row>
-    <row r="42" spans="1:15" ht="43.5" customHeight="1">
-      <c r="B42" s="11" t="s">
+    <row r="43" spans="1:15" ht="43.5" customHeight="1">
+      <c r="B43" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C42" s="11"/>
-      <c r="D42" s="11"/>
-      <c r="E42" s="11"/>
-      <c r="J42" s="11" t="s">
+      <c r="C43" s="11"/>
+      <c r="D43" s="11"/>
+      <c r="E43" s="11"/>
+      <c r="J43" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="K42" s="11"/>
-      <c r="L42" s="11"/>
-      <c r="M42" s="11"/>
-    </row>
-    <row r="43" spans="1:15" ht="56">
-      <c r="B43" s="2" t="s">
+      <c r="K43" s="11"/>
+      <c r="L43" s="11"/>
+      <c r="M43" s="11"/>
+    </row>
+    <row r="44" spans="1:15" ht="56">
+      <c r="B44" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="C44" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="J43" s="2" t="s">
+      <c r="J44" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="K43" s="2" t="s">
+      <c r="K44" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="44" spans="1:15">
-      <c r="B44" t="s">
+    <row r="45" spans="1:15">
+      <c r="B45" t="s">
         <v>54</v>
       </c>
-      <c r="C44" s="7">
+      <c r="C45" s="7">
         <v>1.2</v>
       </c>
-      <c r="J44" t="s">
+      <c r="J45" t="s">
         <v>54</v>
       </c>
-      <c r="K44" s="7">
+      <c r="K45" s="7">
         <v>0.8</v>
-      </c>
-    </row>
-    <row r="45" spans="1:15">
-      <c r="B45" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C45" s="7">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="J45" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="K45" s="7">
-        <v>0.9</v>
       </c>
     </row>
     <row r="46" spans="1:15">
       <c r="B46" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C46" s="7">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="J46" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K46" s="7">
-        <v>1</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="47" spans="1:15">
       <c r="B47" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C47" s="7">
+        <v>1</v>
+      </c>
+      <c r="J47" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="K47" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15">
+      <c r="B48" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C47" s="7">
+      <c r="C48" s="7">
         <v>0.9</v>
       </c>
-      <c r="J47" s="8" t="s">
+      <c r="J48" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="K47" s="7">
+      <c r="K48" s="7">
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="49" spans="2:5" ht="45" customHeight="1">
-      <c r="B49" s="11" t="s">
+    <row r="50" spans="2:5" ht="45" customHeight="1">
+      <c r="B50" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="C49" s="11"/>
-      <c r="D49" s="11"/>
-      <c r="E49" s="11"/>
-    </row>
-    <row r="50" spans="2:5" ht="56">
-      <c r="B50" s="2" t="s">
+      <c r="C50" s="11"/>
+      <c r="D50" s="11"/>
+      <c r="E50" s="11"/>
+    </row>
+    <row r="51" spans="2:5" ht="56">
+      <c r="B51" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="C51" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="51" spans="2:5">
-      <c r="B51" t="s">
+    <row r="52" spans="2:5">
+      <c r="B52" t="s">
         <v>54</v>
       </c>
-      <c r="C51" s="7">
+      <c r="C52" s="7">
         <v>1.2</v>
-      </c>
-    </row>
-    <row r="52" spans="2:5">
-      <c r="B52" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C52" s="7">
-        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="53" spans="2:5">
       <c r="B53" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C53" s="7">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="54" spans="2:5">
       <c r="B54" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C54" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5">
+      <c r="B55" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C54" s="7">
+      <c r="C55" s="7">
         <v>0.9</v>
       </c>
     </row>
@@ -2421,9 +2459,9 @@
     <mergeCell ref="I27:I32"/>
     <mergeCell ref="I17:I21"/>
     <mergeCell ref="I22:I26"/>
-    <mergeCell ref="B42:E42"/>
-    <mergeCell ref="J42:M42"/>
-    <mergeCell ref="B49:E49"/>
+    <mergeCell ref="B43:E43"/>
+    <mergeCell ref="J43:M43"/>
+    <mergeCell ref="B50:E50"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="I1:J1"/>

</xml_diff>

<commit_message>
population not performing as expected
</commit_message>
<xml_diff>
--- a/Excel Files/life_table.xlsx
+++ b/Excel Files/life_table.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Friendships" sheetId="4" r:id="rId3"/>
     <sheet name="Dominance" sheetId="2" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001" calcOnSave="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -855,8 +855,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="L34" sqref="L34"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2452,13 +2452,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="I12:I16"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="A22:A26"/>
-    <mergeCell ref="A27:A32"/>
-    <mergeCell ref="I27:I32"/>
-    <mergeCell ref="I17:I21"/>
-    <mergeCell ref="I22:I26"/>
     <mergeCell ref="B43:E43"/>
     <mergeCell ref="J43:M43"/>
     <mergeCell ref="B50:E50"/>
@@ -2475,6 +2468,13 @@
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="I7:I8"/>
     <mergeCell ref="I9:I11"/>
+    <mergeCell ref="I12:I16"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="A22:A26"/>
+    <mergeCell ref="A27:A32"/>
+    <mergeCell ref="I27:I32"/>
+    <mergeCell ref="I17:I21"/>
+    <mergeCell ref="I22:I26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -3299,17 +3299,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="D34:E34"/>
     <mergeCell ref="L34:M34"/>
     <mergeCell ref="A22:A26"/>
     <mergeCell ref="A27:A32"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="A9:A11"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="A12:A16"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="D34:E34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
modifying sim so that agents only migrate once every 5 years
</commit_message>
<xml_diff>
--- a/Excel Files/life_table.xlsx
+++ b/Excel Files/life_table.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20610" windowHeight="11640" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="life table" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="Friendships" sheetId="4" r:id="rId3"/>
     <sheet name="Dominance" sheetId="2" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="140001" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="145621" calcOnSave="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -855,13 +855,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+    <sheetView topLeftCell="A20" workbookViewId="0">
       <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:15" s="2" customFormat="1" ht="108" customHeight="1">
+    <row r="1" spans="1:15" s="2" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>2</v>
       </c>
@@ -901,7 +901,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -920,7 +920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>40</v>
       </c>
@@ -958,7 +958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>41</v>
       </c>
@@ -998,7 +998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="12"/>
       <c r="B5">
         <v>3</v>
@@ -1034,7 +1034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="12"/>
       <c r="B6">
         <v>4</v>
@@ -1070,7 +1070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="15" customHeight="1">
+    <row r="7" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>42</v>
       </c>
@@ -1111,7 +1111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="11"/>
       <c r="B8">
         <v>6</v>
@@ -1148,7 +1148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="11"/>
       <c r="B9">
         <v>7</v>
@@ -1187,7 +1187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="11"/>
       <c r="B10">
         <v>8</v>
@@ -1224,7 +1224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="11"/>
       <c r="B11">
         <v>9</v>
@@ -1261,7 +1261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>45</v>
       </c>
@@ -1302,7 +1302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="11"/>
       <c r="B13">
         <v>11</v>
@@ -1339,7 +1339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="11"/>
       <c r="B14">
         <v>12</v>
@@ -1376,7 +1376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="11"/>
       <c r="B15">
         <v>13</v>
@@ -1413,7 +1413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="11"/>
       <c r="B16">
         <v>14</v>
@@ -1450,7 +1450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>46</v>
       </c>
@@ -1491,7 +1491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="11"/>
       <c r="B18">
         <v>16</v>
@@ -1528,7 +1528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:15">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="11"/>
       <c r="B19">
         <v>17</v>
@@ -1565,7 +1565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="11"/>
       <c r="B20">
         <v>18</v>
@@ -1602,7 +1602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:15">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="11"/>
       <c r="B21">
         <v>19</v>
@@ -1639,7 +1639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:15">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>9</v>
       </c>
@@ -1680,7 +1680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="11"/>
       <c r="B23">
         <v>21</v>
@@ -1717,7 +1717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:15">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="11"/>
       <c r="B24">
         <v>22</v>
@@ -1754,7 +1754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:15">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="11"/>
       <c r="B25">
         <v>23</v>
@@ -1791,7 +1791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:15">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="11"/>
       <c r="B26">
         <v>24</v>
@@ -1828,7 +1828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:15">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
         <v>19</v>
       </c>
@@ -1869,7 +1869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:15">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="11"/>
       <c r="B28">
         <v>26</v>
@@ -1906,7 +1906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:15">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="11"/>
       <c r="B29">
         <v>27</v>
@@ -1943,7 +1943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:15">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="11"/>
       <c r="B30">
         <v>28</v>
@@ -1980,7 +1980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:15">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="11"/>
       <c r="B31">
         <v>29</v>
@@ -2017,7 +2017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:15">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="11"/>
       <c r="B32">
         <v>30</v>
@@ -2054,7 +2054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:15">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="10"/>
       <c r="B33">
         <v>31</v>
@@ -2088,7 +2088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:15">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="10"/>
       <c r="B34">
         <v>32</v>
@@ -2122,7 +2122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:15">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>63</v>
       </c>
@@ -2134,7 +2134,7 @@
         <v>2053.6022002246564</v>
       </c>
     </row>
-    <row r="37" spans="1:15">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>15</v>
       </c>
@@ -2142,7 +2142,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:15">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>16</v>
       </c>
@@ -2174,7 +2174,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="39" spans="1:15">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B39" s="1">
         <f xml:space="preserve"> SUM(F7:F11)</f>
         <v>939.27029048320014</v>
@@ -2224,7 +2224,7 @@
         <v>2422.0282388068249</v>
       </c>
     </row>
-    <row r="40" spans="1:15">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B40">
         <f t="shared" ref="B40:G40" si="6">(B39/$G$39)</f>
         <v>0.26514252166451985</v>
@@ -2274,7 +2274,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:15">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B41">
         <v>0.26514252166451985</v>
       </c>
@@ -2318,7 +2318,7 @@
         <v>0.99999975799230834</v>
       </c>
     </row>
-    <row r="43" spans="1:15" ht="43.5" customHeight="1">
+    <row r="43" spans="1:15" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="11" t="s">
         <v>60</v>
       </c>
@@ -2332,7 +2332,7 @@
       <c r="L43" s="11"/>
       <c r="M43" s="11"/>
     </row>
-    <row r="44" spans="1:15" ht="56">
+    <row r="44" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="B44" s="2" t="s">
         <v>57</v>
       </c>
@@ -2346,7 +2346,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="45" spans="1:15">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>54</v>
       </c>
@@ -2360,7 +2360,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="46" spans="1:15">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B46" s="8" t="s">
         <v>50</v>
       </c>
@@ -2374,7 +2374,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="47" spans="1:15">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B47" s="8" t="s">
         <v>51</v>
       </c>
@@ -2388,7 +2388,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:15">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B48" s="8" t="s">
         <v>52</v>
       </c>
@@ -2402,7 +2402,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="50" spans="2:5" ht="45" customHeight="1">
+    <row r="50" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="11" t="s">
         <v>61</v>
       </c>
@@ -2410,7 +2410,7 @@
       <c r="D50" s="11"/>
       <c r="E50" s="11"/>
     </row>
-    <row r="51" spans="2:5" ht="56">
+    <row r="51" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B51" s="2" t="s">
         <v>57</v>
       </c>
@@ -2418,7 +2418,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="52" spans="2:5">
+    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>54</v>
       </c>
@@ -2426,7 +2426,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="53" spans="2:5">
+    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B53" s="8" t="s">
         <v>50</v>
       </c>
@@ -2434,7 +2434,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="54" spans="2:5">
+    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B54" s="8" t="s">
         <v>51</v>
       </c>
@@ -2442,7 +2442,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="2:5">
+    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B55" s="8" t="s">
         <v>52</v>
       </c>
@@ -2452,6 +2452,13 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="I12:I16"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="A22:A26"/>
+    <mergeCell ref="A27:A32"/>
+    <mergeCell ref="I27:I32"/>
+    <mergeCell ref="I17:I21"/>
+    <mergeCell ref="I22:I26"/>
     <mergeCell ref="B43:E43"/>
     <mergeCell ref="J43:M43"/>
     <mergeCell ref="B50:E50"/>
@@ -2468,13 +2475,6 @@
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="I7:I8"/>
     <mergeCell ref="I9:I11"/>
-    <mergeCell ref="I12:I16"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="A22:A26"/>
-    <mergeCell ref="A27:A32"/>
-    <mergeCell ref="I27:I32"/>
-    <mergeCell ref="I17:I21"/>
-    <mergeCell ref="I22:I26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2490,21 +2490,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R40"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="8.83203125" style="2"/>
-    <col min="5" max="5" width="11.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="10.83203125" style="2" customWidth="1"/>
-    <col min="9" max="13" width="8.83203125" style="2"/>
-    <col min="14" max="14" width="14.33203125" style="2" customWidth="1"/>
-    <col min="15" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="4" width="8.85546875" style="2"/>
+    <col min="5" max="5" width="11.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="10.85546875" style="2" customWidth="1"/>
+    <col min="9" max="13" width="8.85546875" style="2"/>
+    <col min="14" max="14" width="14.28515625" style="2" customWidth="1"/>
+    <col min="15" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="27" customHeight="1">
+    <row r="1" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>27</v>
       </c>
@@ -2517,7 +2517,7 @@
       <c r="F1" s="11"/>
       <c r="G1" s="11"/>
     </row>
-    <row r="2" spans="1:18" ht="112">
+    <row r="2" spans="1:18" ht="150" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>23</v>
       </c>
@@ -2543,7 +2543,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>40</v>
       </c>
@@ -2569,7 +2569,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>41</v>
       </c>
@@ -2595,7 +2595,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="11"/>
       <c r="B5">
         <v>3</v>
@@ -2619,7 +2619,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
       <c r="B6">
         <v>4</v>
@@ -2640,7 +2640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="15" customHeight="1">
+    <row r="7" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>44</v>
       </c>
@@ -2663,7 +2663,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="11"/>
       <c r="B8">
         <v>6</v>
@@ -2684,7 +2684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="15" customHeight="1">
+    <row r="9" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>43</v>
       </c>
@@ -2695,7 +2695,7 @@
         <v>0.2</v>
       </c>
       <c r="D9" s="2">
-        <v>0.66</v>
+        <v>0.75</v>
       </c>
       <c r="E9" s="2">
         <v>0.4</v>
@@ -2707,7 +2707,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="11"/>
       <c r="B10">
         <v>8</v>
@@ -2716,7 +2716,7 @@
         <v>0.2</v>
       </c>
       <c r="D10" s="2">
-        <v>0.66</v>
+        <v>0.75</v>
       </c>
       <c r="E10" s="2">
         <v>0.4</v>
@@ -2728,7 +2728,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="11"/>
       <c r="B11">
         <v>9</v>
@@ -2737,7 +2737,7 @@
         <v>0.2</v>
       </c>
       <c r="D11" s="2">
-        <v>0.66</v>
+        <v>0.75</v>
       </c>
       <c r="E11" s="2">
         <v>0.4</v>
@@ -2749,7 +2749,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="15" customHeight="1">
+    <row r="12" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>45</v>
       </c>
@@ -2760,7 +2760,7 @@
         <v>0.2</v>
       </c>
       <c r="D12" s="2">
-        <v>0.66</v>
+        <v>0.75</v>
       </c>
       <c r="E12" s="2">
         <v>0.4</v>
@@ -2772,7 +2772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="11"/>
       <c r="B13">
         <v>11</v>
@@ -2781,7 +2781,7 @@
         <v>0.2</v>
       </c>
       <c r="D13" s="2">
-        <v>0.66</v>
+        <v>0.75</v>
       </c>
       <c r="E13" s="2">
         <v>0.4</v>
@@ -2793,7 +2793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="11"/>
       <c r="B14">
         <v>12</v>
@@ -2802,7 +2802,7 @@
         <v>0.2</v>
       </c>
       <c r="D14" s="2">
-        <v>0.66</v>
+        <v>0.75</v>
       </c>
       <c r="E14" s="2">
         <v>0.4</v>
@@ -2814,7 +2814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="11"/>
       <c r="B15">
         <v>13</v>
@@ -2823,7 +2823,7 @@
         <v>0.2</v>
       </c>
       <c r="D15" s="2">
-        <v>0.66</v>
+        <v>0.75</v>
       </c>
       <c r="E15" s="2">
         <v>0.4</v>
@@ -2835,7 +2835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="11"/>
       <c r="B16">
         <v>14</v>
@@ -2844,7 +2844,7 @@
         <v>0.2</v>
       </c>
       <c r="D16" s="2">
-        <v>0.66</v>
+        <v>0.75</v>
       </c>
       <c r="E16" s="2">
         <v>0.4</v>
@@ -2856,7 +2856,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15" customHeight="1">
+    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>46</v>
       </c>
@@ -2867,7 +2867,7 @@
         <v>0.2</v>
       </c>
       <c r="D17" s="2">
-        <v>0.66</v>
+        <v>0.75</v>
       </c>
       <c r="E17" s="2">
         <v>0.4</v>
@@ -2879,7 +2879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="11"/>
       <c r="B18">
         <v>16</v>
@@ -2888,7 +2888,7 @@
         <v>0.2</v>
       </c>
       <c r="D18" s="2">
-        <v>0.66</v>
+        <v>0.75</v>
       </c>
       <c r="E18" s="2">
         <v>0.4</v>
@@ -2900,7 +2900,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="11"/>
       <c r="B19">
         <v>17</v>
@@ -2909,7 +2909,7 @@
         <v>0.2</v>
       </c>
       <c r="D19" s="2">
-        <v>0.66</v>
+        <v>0.75</v>
       </c>
       <c r="E19" s="2">
         <v>0.4</v>
@@ -2921,7 +2921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="11"/>
       <c r="B20">
         <v>18</v>
@@ -2930,7 +2930,7 @@
         <v>0.2</v>
       </c>
       <c r="D20" s="2">
-        <v>0.66</v>
+        <v>0.75</v>
       </c>
       <c r="E20" s="2">
         <v>0.4</v>
@@ -2942,7 +2942,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="11"/>
       <c r="B21">
         <v>19</v>
@@ -2951,7 +2951,7 @@
         <v>0.2</v>
       </c>
       <c r="D21" s="2">
-        <v>0.66</v>
+        <v>0.75</v>
       </c>
       <c r="E21" s="2">
         <v>0.4</v>
@@ -2963,7 +2963,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>9</v>
       </c>
@@ -2974,7 +2974,7 @@
         <v>0.2</v>
       </c>
       <c r="D22" s="2">
-        <v>0.66</v>
+        <v>0.75</v>
       </c>
       <c r="E22" s="2">
         <v>0.4</v>
@@ -2986,7 +2986,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="11"/>
       <c r="B23">
         <v>21</v>
@@ -2995,7 +2995,7 @@
         <v>0.2</v>
       </c>
       <c r="D23" s="2">
-        <v>0.66</v>
+        <v>0.75</v>
       </c>
       <c r="E23" s="2">
         <v>0.4</v>
@@ -3007,7 +3007,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="11"/>
       <c r="B24">
         <v>22</v>
@@ -3016,7 +3016,7 @@
         <v>0.2</v>
       </c>
       <c r="D24" s="2">
-        <v>0.66</v>
+        <v>0.75</v>
       </c>
       <c r="E24" s="2">
         <v>0.4</v>
@@ -3028,7 +3028,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="11"/>
       <c r="B25">
         <v>23</v>
@@ -3037,7 +3037,7 @@
         <v>0.2</v>
       </c>
       <c r="D25" s="2">
-        <v>0.66</v>
+        <v>0.75</v>
       </c>
       <c r="E25" s="2">
         <v>0.4</v>
@@ -3049,7 +3049,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="11"/>
       <c r="B26">
         <v>24</v>
@@ -3058,7 +3058,7 @@
         <v>0.2</v>
       </c>
       <c r="D26" s="2">
-        <v>0.66</v>
+        <v>0.75</v>
       </c>
       <c r="E26" s="2">
         <v>0.4</v>
@@ -3070,7 +3070,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
         <v>19</v>
       </c>
@@ -3081,7 +3081,7 @@
         <v>0.2</v>
       </c>
       <c r="D27" s="2">
-        <v>0.66</v>
+        <v>0.75</v>
       </c>
       <c r="E27" s="2">
         <v>0.4</v>
@@ -3093,7 +3093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="11"/>
       <c r="B28">
         <v>26</v>
@@ -3102,7 +3102,7 @@
         <v>0.2</v>
       </c>
       <c r="D28" s="2">
-        <v>0.66</v>
+        <v>0.75</v>
       </c>
       <c r="E28" s="2">
         <v>0.4</v>
@@ -3114,7 +3114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="11"/>
       <c r="B29">
         <v>27</v>
@@ -3123,7 +3123,7 @@
         <v>0.2</v>
       </c>
       <c r="D29" s="2">
-        <v>0.66</v>
+        <v>0.75</v>
       </c>
       <c r="E29" s="2">
         <v>0.4</v>
@@ -3135,7 +3135,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="11"/>
       <c r="B30">
         <v>28</v>
@@ -3144,7 +3144,7 @@
         <v>0.2</v>
       </c>
       <c r="D30" s="2">
-        <v>0.66</v>
+        <v>0.75</v>
       </c>
       <c r="E30" s="2">
         <v>0.4</v>
@@ -3156,7 +3156,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="11"/>
       <c r="B31">
         <v>29</v>
@@ -3165,7 +3165,7 @@
         <v>0.2</v>
       </c>
       <c r="D31" s="2">
-        <v>0.66</v>
+        <v>0.75</v>
       </c>
       <c r="E31" s="2">
         <v>0.4</v>
@@ -3177,7 +3177,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="11"/>
       <c r="B32">
         <v>30</v>
@@ -3186,7 +3186,7 @@
         <v>0.2</v>
       </c>
       <c r="D32" s="2">
-        <v>0.66</v>
+        <v>0.75</v>
       </c>
       <c r="E32" s="2">
         <v>0.4</v>
@@ -3198,12 +3198,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:14">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="56">
+    <row r="34" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="C34" s="2" t="s">
         <v>67</v>
       </c>
@@ -3222,7 +3222,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="35" spans="1:14">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C35" s="2" t="s">
         <v>68</v>
       </c>
@@ -3240,7 +3240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:14">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C36" s="2">
         <v>1</v>
       </c>
@@ -3257,7 +3257,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="37" spans="1:14">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C37" s="2">
         <v>2</v>
       </c>
@@ -3274,7 +3274,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:14">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C38" s="2">
         <v>3</v>
       </c>
@@ -3291,25 +3291,25 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="39" spans="1:14">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E39" s="6"/>
     </row>
-    <row r="40" spans="1:14">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E40" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="A12:A16"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="D34:E34"/>
     <mergeCell ref="L34:M34"/>
     <mergeCell ref="A22:A26"/>
     <mergeCell ref="A27:A32"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="D34:E34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -3329,17 +3329,17 @@
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="8.83203125" style="2"/>
-    <col min="3" max="3" width="16.83203125" style="2" customWidth="1"/>
-    <col min="4" max="5" width="8.83203125" style="2"/>
-    <col min="6" max="6" width="15.33203125" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="26.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" style="2"/>
+    <col min="3" max="3" width="16.85546875" style="2" customWidth="1"/>
+    <col min="4" max="5" width="8.85546875" style="2"/>
+    <col min="6" max="6" width="15.28515625" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="49.5" customHeight="1">
+    <row r="1" spans="1:7" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>36</v>
       </c>
@@ -3350,7 +3350,7 @@
       <c r="F1" s="11"/>
       <c r="G1" s="11"/>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>33</v>
       </c>
@@ -3358,7 +3358,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="78" customHeight="1">
+    <row r="3" spans="1:7" ht="78" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>69</v>
       </c>
@@ -3372,7 +3372,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="60" customHeight="1">
+    <row r="4" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>70</v>
       </c>
@@ -3386,7 +3386,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="42">
+    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>38</v>
       </c>
@@ -3398,7 +3398,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="28">
+    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>34</v>
       </c>
@@ -3409,7 +3409,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E7" s="2">
         <v>3</v>
       </c>
@@ -3417,42 +3417,42 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="28">
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="42">
+    <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="28">
+    <row r="11" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="28">
+    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="28">
+    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="28">
+    <row r="16" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>79</v>
       </c>
@@ -3479,12 +3479,12 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>14</v>
       </c>
@@ -3493,7 +3493,7 @@
       <c r="D1" s="14"/>
       <c r="E1" s="15"/>
     </row>
-    <row r="2" spans="1:5" ht="56">
+    <row r="2" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -3504,7 +3504,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="28">
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -3515,7 +3515,7 @@
         <v>1.1499999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="42">
+    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -3526,7 +3526,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="28">
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
@@ -3537,7 +3537,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>71</v>
       </c>

</xml_diff>

<commit_message>
fixed error with emigration adults migrate every 5th year, no coin toss applies
</commit_message>
<xml_diff>
--- a/Excel Files/life_table.xlsx
+++ b/Excel Files/life_table.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Friendships" sheetId="4" r:id="rId3"/>
     <sheet name="Dominance" sheetId="2" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" calcOnSave="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="81">
   <si>
     <t>Year</t>
   </si>
@@ -391,6 +391,9 @@
   </si>
   <si>
     <t>3. randomly select an individual from the pool of potential friends</t>
+  </si>
+  <si>
+    <t>NOTE: adult males are made to emigrate once every 5 years since their 1st emigration, so it does not matter that their probability of emigration according to this table is 1</t>
   </si>
 </sst>
 </file>
@@ -2452,6 +2455,13 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="I12:I16"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="A22:A26"/>
+    <mergeCell ref="A27:A32"/>
+    <mergeCell ref="I27:I32"/>
+    <mergeCell ref="I17:I21"/>
+    <mergeCell ref="I22:I26"/>
     <mergeCell ref="B43:E43"/>
     <mergeCell ref="J43:M43"/>
     <mergeCell ref="B50:E50"/>
@@ -2468,13 +2478,6 @@
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="I7:I8"/>
     <mergeCell ref="I9:I11"/>
-    <mergeCell ref="I12:I16"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="A22:A26"/>
-    <mergeCell ref="A27:A32"/>
-    <mergeCell ref="I27:I32"/>
-    <mergeCell ref="I17:I21"/>
-    <mergeCell ref="I22:I26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2490,8 +2493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D6:D9"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2692,7 +2695,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="2">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="D9" s="2">
         <v>0.75</v>
@@ -2713,7 +2716,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="2">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="D10" s="2">
         <v>0.75</v>
@@ -2734,7 +2737,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="2">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="D11" s="2">
         <v>0.75</v>
@@ -2757,7 +2760,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="2">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="D12" s="2">
         <v>0.75</v>
@@ -2778,7 +2781,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="2">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="D13" s="2">
         <v>0.75</v>
@@ -2799,7 +2802,7 @@
         <v>12</v>
       </c>
       <c r="C14" s="2">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="D14" s="2">
         <v>0.75</v>
@@ -2820,7 +2823,7 @@
         <v>13</v>
       </c>
       <c r="C15" s="2">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="D15" s="2">
         <v>0.75</v>
@@ -2841,7 +2844,7 @@
         <v>14</v>
       </c>
       <c r="C16" s="2">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="D16" s="2">
         <v>0.75</v>
@@ -2864,7 +2867,7 @@
         <v>15</v>
       </c>
       <c r="C17" s="2">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="D17" s="2">
         <v>0.75</v>
@@ -2885,7 +2888,7 @@
         <v>16</v>
       </c>
       <c r="C18" s="2">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="D18" s="2">
         <v>0.75</v>
@@ -2906,7 +2909,7 @@
         <v>17</v>
       </c>
       <c r="C19" s="2">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="D19" s="2">
         <v>0.75</v>
@@ -2927,7 +2930,7 @@
         <v>18</v>
       </c>
       <c r="C20" s="2">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="D20" s="2">
         <v>0.75</v>
@@ -2948,7 +2951,7 @@
         <v>19</v>
       </c>
       <c r="C21" s="2">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="D21" s="2">
         <v>0.75</v>
@@ -2971,7 +2974,7 @@
         <v>20</v>
       </c>
       <c r="C22" s="2">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="D22" s="2">
         <v>0.75</v>
@@ -2992,7 +2995,7 @@
         <v>21</v>
       </c>
       <c r="C23" s="2">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="D23" s="2">
         <v>0.75</v>
@@ -3013,7 +3016,7 @@
         <v>22</v>
       </c>
       <c r="C24" s="2">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="D24" s="2">
         <v>0.75</v>
@@ -3034,7 +3037,7 @@
         <v>23</v>
       </c>
       <c r="C25" s="2">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="D25" s="2">
         <v>0.75</v>
@@ -3055,7 +3058,7 @@
         <v>24</v>
       </c>
       <c r="C26" s="2">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="D26" s="2">
         <v>0.75</v>
@@ -3078,7 +3081,7 @@
         <v>25</v>
       </c>
       <c r="C27" s="2">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="D27" s="2">
         <v>0.75</v>
@@ -3099,7 +3102,7 @@
         <v>26</v>
       </c>
       <c r="C28" s="2">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="D28" s="2">
         <v>0.75</v>
@@ -3120,7 +3123,7 @@
         <v>27</v>
       </c>
       <c r="C29" s="2">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="D29" s="2">
         <v>0.75</v>
@@ -3141,7 +3144,7 @@
         <v>28</v>
       </c>
       <c r="C30" s="2">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="D30" s="2">
         <v>0.75</v>
@@ -3162,7 +3165,7 @@
         <v>29</v>
       </c>
       <c r="C31" s="2">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="D31" s="2">
         <v>0.75</v>
@@ -3183,7 +3186,7 @@
         <v>30</v>
       </c>
       <c r="C32" s="2">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="D32" s="2">
         <v>0.75</v>
@@ -3198,10 +3201,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:14">
+    <row r="33" spans="1:14" ht="27" customHeight="1">
       <c r="A33" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="B33" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
     </row>
     <row r="34" spans="1:14" ht="56">
       <c r="C34" s="2" t="s">
@@ -3298,18 +3310,19 @@
       <c r="E40" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="A12:A16"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="D34:E34"/>
+  <mergeCells count="12">
     <mergeCell ref="L34:M34"/>
     <mergeCell ref="A22:A26"/>
     <mergeCell ref="A27:A32"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="A9:A11"/>
+    <mergeCell ref="B33:H33"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="D34:E34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
fixed error in add_agent where in the first gen males were not added to the male set
</commit_message>
<xml_diff>
--- a/Excel Files/life_table.xlsx
+++ b/Excel Files/life_table.xlsx
@@ -2455,13 +2455,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="I12:I16"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="A22:A26"/>
-    <mergeCell ref="A27:A32"/>
-    <mergeCell ref="I27:I32"/>
-    <mergeCell ref="I17:I21"/>
-    <mergeCell ref="I22:I26"/>
     <mergeCell ref="B43:E43"/>
     <mergeCell ref="J43:M43"/>
     <mergeCell ref="B50:E50"/>
@@ -2478,6 +2471,13 @@
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="I7:I8"/>
     <mergeCell ref="I9:I11"/>
+    <mergeCell ref="I12:I16"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="A22:A26"/>
+    <mergeCell ref="A27:A32"/>
+    <mergeCell ref="I27:I32"/>
+    <mergeCell ref="I17:I21"/>
+    <mergeCell ref="I22:I26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2493,8 +2493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6:E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2660,7 +2660,7 @@
         <v>0.5</v>
       </c>
       <c r="F7" s="2">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="G7" s="2">
         <v>1</v>
@@ -2681,7 +2681,7 @@
         <v>0.5</v>
       </c>
       <c r="F8" s="2">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="G8" s="2">
         <v>1</v>
@@ -2701,10 +2701,10 @@
         <v>0.75</v>
       </c>
       <c r="E9" s="2">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="F9" s="2">
-        <v>0.66</v>
+        <v>0.75</v>
       </c>
       <c r="G9" s="2">
         <v>1</v>
@@ -2722,10 +2722,10 @@
         <v>0.75</v>
       </c>
       <c r="E10" s="2">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="F10" s="2">
-        <v>0.66</v>
+        <v>0.75</v>
       </c>
       <c r="G10" s="2">
         <v>1</v>
@@ -2743,10 +2743,10 @@
         <v>0.75</v>
       </c>
       <c r="E11" s="2">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="F11" s="2">
-        <v>0.66</v>
+        <v>0.75</v>
       </c>
       <c r="G11" s="2">
         <v>1</v>
@@ -2766,10 +2766,10 @@
         <v>0.75</v>
       </c>
       <c r="E12" s="2">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="F12" s="2">
-        <v>0.66</v>
+        <v>0.75</v>
       </c>
       <c r="G12" s="2">
         <v>1</v>
@@ -2787,10 +2787,10 @@
         <v>0.75</v>
       </c>
       <c r="E13" s="2">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="F13" s="2">
-        <v>0.66</v>
+        <v>0.75</v>
       </c>
       <c r="G13" s="2">
         <v>1</v>
@@ -2808,10 +2808,10 @@
         <v>0.75</v>
       </c>
       <c r="E14" s="2">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="F14" s="2">
-        <v>0.66</v>
+        <v>0.75</v>
       </c>
       <c r="G14" s="2">
         <v>1</v>
@@ -2829,10 +2829,10 @@
         <v>0.75</v>
       </c>
       <c r="E15" s="2">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="F15" s="2">
-        <v>0.66</v>
+        <v>0.75</v>
       </c>
       <c r="G15" s="2">
         <v>1</v>
@@ -2850,10 +2850,10 @@
         <v>0.75</v>
       </c>
       <c r="E16" s="2">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="F16" s="2">
-        <v>0.66</v>
+        <v>0.75</v>
       </c>
       <c r="G16" s="2">
         <v>1</v>
@@ -2873,10 +2873,10 @@
         <v>0.75</v>
       </c>
       <c r="E17" s="2">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="F17" s="2">
-        <v>0.66</v>
+        <v>0.75</v>
       </c>
       <c r="G17" s="2">
         <v>1</v>
@@ -2894,10 +2894,10 @@
         <v>0.75</v>
       </c>
       <c r="E18" s="2">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="F18" s="2">
-        <v>0.66</v>
+        <v>0.75</v>
       </c>
       <c r="G18" s="2">
         <v>1</v>
@@ -2915,10 +2915,10 @@
         <v>0.75</v>
       </c>
       <c r="E19" s="2">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="F19" s="2">
-        <v>0.66</v>
+        <v>0.75</v>
       </c>
       <c r="G19" s="2">
         <v>1</v>
@@ -2936,10 +2936,10 @@
         <v>0.75</v>
       </c>
       <c r="E20" s="2">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="F20" s="2">
-        <v>0.66</v>
+        <v>0.75</v>
       </c>
       <c r="G20" s="2">
         <v>1</v>
@@ -2957,10 +2957,10 @@
         <v>0.75</v>
       </c>
       <c r="E21" s="2">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="F21" s="2">
-        <v>0.66</v>
+        <v>0.75</v>
       </c>
       <c r="G21" s="2">
         <v>1</v>
@@ -2980,10 +2980,10 @@
         <v>0.75</v>
       </c>
       <c r="E22" s="2">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="F22" s="2">
-        <v>0.66</v>
+        <v>0.75</v>
       </c>
       <c r="G22" s="2">
         <v>1</v>
@@ -3001,10 +3001,10 @@
         <v>0.75</v>
       </c>
       <c r="E23" s="2">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="F23" s="2">
-        <v>0.66</v>
+        <v>0.75</v>
       </c>
       <c r="G23" s="2">
         <v>1</v>
@@ -3022,10 +3022,10 @@
         <v>0.75</v>
       </c>
       <c r="E24" s="2">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="F24" s="2">
-        <v>0.66</v>
+        <v>0.75</v>
       </c>
       <c r="G24" s="2">
         <v>1</v>
@@ -3043,10 +3043,10 @@
         <v>0.75</v>
       </c>
       <c r="E25" s="2">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="F25" s="2">
-        <v>0.66</v>
+        <v>0.75</v>
       </c>
       <c r="G25" s="2">
         <v>1</v>
@@ -3064,10 +3064,10 @@
         <v>0.75</v>
       </c>
       <c r="E26" s="2">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="F26" s="2">
-        <v>0.66</v>
+        <v>0.75</v>
       </c>
       <c r="G26" s="2">
         <v>1</v>
@@ -3087,10 +3087,10 @@
         <v>0.75</v>
       </c>
       <c r="E27" s="2">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="F27" s="2">
-        <v>0.66</v>
+        <v>0.75</v>
       </c>
       <c r="G27" s="2">
         <v>1</v>
@@ -3108,10 +3108,10 @@
         <v>0.75</v>
       </c>
       <c r="E28" s="2">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="F28" s="2">
-        <v>0.66</v>
+        <v>0.75</v>
       </c>
       <c r="G28" s="2">
         <v>1</v>
@@ -3129,10 +3129,10 @@
         <v>0.75</v>
       </c>
       <c r="E29" s="2">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="F29" s="2">
-        <v>0.66</v>
+        <v>0.75</v>
       </c>
       <c r="G29" s="2">
         <v>1</v>
@@ -3150,10 +3150,10 @@
         <v>0.75</v>
       </c>
       <c r="E30" s="2">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="F30" s="2">
-        <v>0.66</v>
+        <v>0.75</v>
       </c>
       <c r="G30" s="2">
         <v>1</v>
@@ -3171,10 +3171,10 @@
         <v>0.75</v>
       </c>
       <c r="E31" s="2">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="F31" s="2">
-        <v>0.66</v>
+        <v>0.75</v>
       </c>
       <c r="G31" s="2">
         <v>1</v>
@@ -3192,10 +3192,10 @@
         <v>0.75</v>
       </c>
       <c r="E32" s="2">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="F32" s="2">
-        <v>0.66</v>
+        <v>0.75</v>
       </c>
       <c r="G32" s="2">
         <v>1</v>
@@ -3311,6 +3311,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="D34:E34"/>
     <mergeCell ref="L34:M34"/>
     <mergeCell ref="A22:A26"/>
     <mergeCell ref="A27:A32"/>
@@ -3318,11 +3323,6 @@
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="A9:A11"/>
     <mergeCell ref="B33:H33"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="A12:A16"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="D34:E34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
added translocation_control exp and simulation
</commit_message>
<xml_diff>
--- a/Excel Files/life_table.xlsx
+++ b/Excel Files/life_table.xlsx
@@ -1,18 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20620" windowHeight="11640" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20610" windowHeight="11640" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="life table" sheetId="1" r:id="rId1"/>
     <sheet name="Dispersal" sheetId="3" r:id="rId2"/>
     <sheet name="Friendships" sheetId="4" r:id="rId3"/>
     <sheet name="Dominance" sheetId="2" r:id="rId4"/>
+    <sheet name="Translocation" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="140001" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="93">
   <si>
     <t>Year</t>
   </si>
@@ -394,6 +395,42 @@
   </si>
   <si>
     <t>NOTE: adult males are made to emigrate once every 5 years since their 1st emigration, so it does not matter that their probability of emigration according to this table is 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chance of being accepted </t>
+  </si>
+  <si>
+    <t>Female Acceptance (all ages)</t>
+  </si>
+  <si>
+    <t>Likelihood of Translocation: Control</t>
+  </si>
+  <si>
+    <t>Females</t>
+  </si>
+  <si>
+    <t>Males</t>
+  </si>
+  <si>
+    <t>Age in years</t>
+  </si>
+  <si>
+    <t>Likelihood of Translocation: Male-Biased</t>
+  </si>
+  <si>
+    <t>Biased towards</t>
+  </si>
+  <si>
+    <t>Sub-ad and young adult males</t>
+  </si>
+  <si>
+    <t>Likelihood of Translocation: Female-Biased</t>
+  </si>
+  <si>
+    <t>Biased Towards</t>
+  </si>
+  <si>
+    <t>Young adult females</t>
   </si>
 </sst>
 </file>
@@ -504,7 +541,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -541,6 +578,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -858,13 +899,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O55"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:15" s="2" customFormat="1" ht="108" customHeight="1">
+    <row r="1" spans="1:15" s="2" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>2</v>
       </c>
@@ -904,7 +945,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -923,7 +964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>40</v>
       </c>
@@ -961,7 +1002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>41</v>
       </c>
@@ -1001,7 +1042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="12"/>
       <c r="B5">
         <v>3</v>
@@ -1037,7 +1078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="12"/>
       <c r="B6">
         <v>4</v>
@@ -1073,7 +1114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="15" customHeight="1">
+    <row r="7" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>42</v>
       </c>
@@ -1114,7 +1155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="11"/>
       <c r="B8">
         <v>6</v>
@@ -1151,7 +1192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="11"/>
       <c r="B9">
         <v>7</v>
@@ -1190,7 +1231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="11"/>
       <c r="B10">
         <v>8</v>
@@ -1227,7 +1268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="11"/>
       <c r="B11">
         <v>9</v>
@@ -1264,7 +1305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>45</v>
       </c>
@@ -1305,7 +1346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="11"/>
       <c r="B13">
         <v>11</v>
@@ -1342,7 +1383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="11"/>
       <c r="B14">
         <v>12</v>
@@ -1379,7 +1420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="11"/>
       <c r="B15">
         <v>13</v>
@@ -1416,7 +1457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="11"/>
       <c r="B16">
         <v>14</v>
@@ -1453,7 +1494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>46</v>
       </c>
@@ -1494,7 +1535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="11"/>
       <c r="B18">
         <v>16</v>
@@ -1531,7 +1572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:15">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="11"/>
       <c r="B19">
         <v>17</v>
@@ -1568,7 +1609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="11"/>
       <c r="B20">
         <v>18</v>
@@ -1605,7 +1646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:15">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="11"/>
       <c r="B21">
         <v>19</v>
@@ -1642,7 +1683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:15">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>9</v>
       </c>
@@ -1683,7 +1724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="11"/>
       <c r="B23">
         <v>21</v>
@@ -1720,7 +1761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:15">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="11"/>
       <c r="B24">
         <v>22</v>
@@ -1757,7 +1798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:15">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="11"/>
       <c r="B25">
         <v>23</v>
@@ -1794,7 +1835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:15">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="11"/>
       <c r="B26">
         <v>24</v>
@@ -1831,7 +1872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:15">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
         <v>19</v>
       </c>
@@ -1872,7 +1913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:15">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="11"/>
       <c r="B28">
         <v>26</v>
@@ -1909,7 +1950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:15">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="11"/>
       <c r="B29">
         <v>27</v>
@@ -1946,7 +1987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:15">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="11"/>
       <c r="B30">
         <v>28</v>
@@ -1983,7 +2024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:15">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="11"/>
       <c r="B31">
         <v>29</v>
@@ -2020,7 +2061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:15">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="11"/>
       <c r="B32">
         <v>30</v>
@@ -2057,7 +2098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:15">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="10"/>
       <c r="B33">
         <v>31</v>
@@ -2091,7 +2132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:15">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="10"/>
       <c r="B34">
         <v>32</v>
@@ -2125,7 +2166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:15">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>63</v>
       </c>
@@ -2137,7 +2178,7 @@
         <v>2053.6022002246564</v>
       </c>
     </row>
-    <row r="37" spans="1:15">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>15</v>
       </c>
@@ -2145,7 +2186,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:15">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>16</v>
       </c>
@@ -2177,7 +2218,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="39" spans="1:15">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B39" s="1">
         <f xml:space="preserve"> SUM(F7:F11)</f>
         <v>939.27029048320014</v>
@@ -2227,7 +2268,7 @@
         <v>2422.0282388068249</v>
       </c>
     </row>
-    <row r="40" spans="1:15">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B40">
         <f t="shared" ref="B40:G40" si="6">(B39/$G$39)</f>
         <v>0.26514252166451985</v>
@@ -2277,7 +2318,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:15">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B41">
         <v>0.26514252166451985</v>
       </c>
@@ -2321,7 +2362,7 @@
         <v>0.99999975799230834</v>
       </c>
     </row>
-    <row r="43" spans="1:15" ht="43.5" customHeight="1">
+    <row r="43" spans="1:15" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="11" t="s">
         <v>60</v>
       </c>
@@ -2335,7 +2376,7 @@
       <c r="L43" s="11"/>
       <c r="M43" s="11"/>
     </row>
-    <row r="44" spans="1:15" ht="56">
+    <row r="44" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="B44" s="2" t="s">
         <v>57</v>
       </c>
@@ -2349,7 +2390,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="45" spans="1:15">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>54</v>
       </c>
@@ -2363,7 +2404,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="46" spans="1:15">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B46" s="8" t="s">
         <v>50</v>
       </c>
@@ -2377,7 +2418,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="47" spans="1:15">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B47" s="8" t="s">
         <v>51</v>
       </c>
@@ -2391,7 +2432,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:15">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B48" s="8" t="s">
         <v>52</v>
       </c>
@@ -2405,7 +2446,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="50" spans="2:5" ht="45" customHeight="1">
+    <row r="50" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="11" t="s">
         <v>61</v>
       </c>
@@ -2413,7 +2454,7 @@
       <c r="D50" s="11"/>
       <c r="E50" s="11"/>
     </row>
-    <row r="51" spans="2:5" ht="56">
+    <row r="51" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B51" s="2" t="s">
         <v>57</v>
       </c>
@@ -2421,7 +2462,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="52" spans="2:5">
+    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>54</v>
       </c>
@@ -2429,7 +2470,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="53" spans="2:5">
+    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B53" s="8" t="s">
         <v>50</v>
       </c>
@@ -2437,7 +2478,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="54" spans="2:5">
+    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B54" s="8" t="s">
         <v>51</v>
       </c>
@@ -2445,7 +2486,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="2:5">
+    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B55" s="8" t="s">
         <v>52</v>
       </c>
@@ -2455,6 +2496,13 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="I12:I16"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="A22:A26"/>
+    <mergeCell ref="A27:A32"/>
+    <mergeCell ref="I27:I32"/>
+    <mergeCell ref="I17:I21"/>
+    <mergeCell ref="I22:I26"/>
     <mergeCell ref="B43:E43"/>
     <mergeCell ref="J43:M43"/>
     <mergeCell ref="B50:E50"/>
@@ -2471,13 +2519,6 @@
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="I7:I8"/>
     <mergeCell ref="I9:I11"/>
-    <mergeCell ref="I12:I16"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="A22:A26"/>
-    <mergeCell ref="A27:A32"/>
-    <mergeCell ref="I27:I32"/>
-    <mergeCell ref="I17:I21"/>
-    <mergeCell ref="I22:I26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2493,21 +2534,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6:E32"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="8.83203125" style="2"/>
-    <col min="5" max="5" width="11.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="10.83203125" style="2" customWidth="1"/>
-    <col min="9" max="13" width="8.83203125" style="2"/>
-    <col min="14" max="14" width="14.33203125" style="2" customWidth="1"/>
-    <col min="15" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="4" width="8.85546875" style="2"/>
+    <col min="5" max="5" width="11.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="10.85546875" style="2" customWidth="1"/>
+    <col min="9" max="13" width="8.85546875" style="2"/>
+    <col min="14" max="14" width="14.28515625" style="2" customWidth="1"/>
+    <col min="15" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="27" customHeight="1">
+    <row r="1" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>27</v>
       </c>
@@ -2520,7 +2561,7 @@
       <c r="F1" s="11"/>
       <c r="G1" s="11"/>
     </row>
-    <row r="2" spans="1:18" ht="112">
+    <row r="2" spans="1:18" ht="150" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>23</v>
       </c>
@@ -2546,7 +2587,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>40</v>
       </c>
@@ -2572,7 +2613,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>41</v>
       </c>
@@ -2598,7 +2639,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="11"/>
       <c r="B5">
         <v>3</v>
@@ -2622,7 +2663,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
       <c r="B6">
         <v>4</v>
@@ -2643,7 +2684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="15" customHeight="1">
+    <row r="7" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>44</v>
       </c>
@@ -2666,7 +2707,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="11"/>
       <c r="B8">
         <v>6</v>
@@ -2687,7 +2728,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="15" customHeight="1">
+    <row r="9" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>43</v>
       </c>
@@ -2710,7 +2751,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="11"/>
       <c r="B10">
         <v>8</v>
@@ -2731,7 +2772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="11"/>
       <c r="B11">
         <v>9</v>
@@ -2752,7 +2793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="15" customHeight="1">
+    <row r="12" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>45</v>
       </c>
@@ -2775,7 +2816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="11"/>
       <c r="B13">
         <v>11</v>
@@ -2796,7 +2837,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="11"/>
       <c r="B14">
         <v>12</v>
@@ -2817,7 +2858,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="11"/>
       <c r="B15">
         <v>13</v>
@@ -2838,7 +2879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="11"/>
       <c r="B16">
         <v>14</v>
@@ -2859,7 +2900,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15" customHeight="1">
+    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>46</v>
       </c>
@@ -2882,7 +2923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="11"/>
       <c r="B18">
         <v>16</v>
@@ -2903,7 +2944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="11"/>
       <c r="B19">
         <v>17</v>
@@ -2924,7 +2965,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="11"/>
       <c r="B20">
         <v>18</v>
@@ -2945,7 +2986,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="11"/>
       <c r="B21">
         <v>19</v>
@@ -2966,7 +3007,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>9</v>
       </c>
@@ -2989,7 +3030,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="11"/>
       <c r="B23">
         <v>21</v>
@@ -3010,7 +3051,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="11"/>
       <c r="B24">
         <v>22</v>
@@ -3031,7 +3072,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="11"/>
       <c r="B25">
         <v>23</v>
@@ -3052,7 +3093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="11"/>
       <c r="B26">
         <v>24</v>
@@ -3073,7 +3114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
         <v>19</v>
       </c>
@@ -3096,7 +3137,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="11"/>
       <c r="B28">
         <v>26</v>
@@ -3117,7 +3158,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="11"/>
       <c r="B29">
         <v>27</v>
@@ -3138,7 +3179,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="11"/>
       <c r="B30">
         <v>28</v>
@@ -3159,7 +3200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="11"/>
       <c r="B31">
         <v>29</v>
@@ -3180,7 +3221,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="11"/>
       <c r="B32">
         <v>30</v>
@@ -3201,7 +3242,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="27" customHeight="1">
+    <row r="33" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>63</v>
       </c>
@@ -3215,7 +3256,7 @@
       <c r="G33" s="11"/>
       <c r="H33" s="11"/>
     </row>
-    <row r="34" spans="1:14" ht="56">
+    <row r="34" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="C34" s="2" t="s">
         <v>67</v>
       </c>
@@ -3234,7 +3275,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="35" spans="1:14">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C35" s="2" t="s">
         <v>68</v>
       </c>
@@ -3252,7 +3293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:14">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C36" s="2">
         <v>1</v>
       </c>
@@ -3269,7 +3310,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="37" spans="1:14">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C37" s="2">
         <v>2</v>
       </c>
@@ -3286,7 +3327,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:14">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C38" s="2">
         <v>3</v>
       </c>
@@ -3303,19 +3344,14 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="39" spans="1:14">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E39" s="6"/>
     </row>
-    <row r="40" spans="1:14">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E40" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="A12:A16"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="D34:E34"/>
     <mergeCell ref="L34:M34"/>
     <mergeCell ref="A22:A26"/>
     <mergeCell ref="A27:A32"/>
@@ -3323,6 +3359,11 @@
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="A9:A11"/>
     <mergeCell ref="B33:H33"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="D34:E34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -3342,17 +3383,17 @@
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="8.83203125" style="2"/>
-    <col min="3" max="3" width="16.83203125" style="2" customWidth="1"/>
-    <col min="4" max="5" width="8.83203125" style="2"/>
-    <col min="6" max="6" width="15.33203125" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="26.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" style="2"/>
+    <col min="3" max="3" width="16.85546875" style="2" customWidth="1"/>
+    <col min="4" max="5" width="8.85546875" style="2"/>
+    <col min="6" max="6" width="15.28515625" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="49.5" customHeight="1">
+    <row r="1" spans="1:7" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>36</v>
       </c>
@@ -3363,7 +3404,7 @@
       <c r="F1" s="11"/>
       <c r="G1" s="11"/>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>33</v>
       </c>
@@ -3371,7 +3412,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="78" customHeight="1">
+    <row r="3" spans="1:7" ht="78" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>69</v>
       </c>
@@ -3385,7 +3426,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="60" customHeight="1">
+    <row r="4" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>70</v>
       </c>
@@ -3399,7 +3440,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="42">
+    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>38</v>
       </c>
@@ -3411,7 +3452,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="28">
+    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>34</v>
       </c>
@@ -3422,7 +3463,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E7" s="2">
         <v>3</v>
       </c>
@@ -3430,42 +3471,42 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="28">
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="42">
+    <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="28">
+    <row r="11" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="28">
+    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="28">
+    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="28">
+    <row r="16" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>79</v>
       </c>
@@ -3492,12 +3533,12 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>14</v>
       </c>
@@ -3506,7 +3547,7 @@
       <c r="D1" s="14"/>
       <c r="E1" s="15"/>
     </row>
-    <row r="2" spans="1:5" ht="56">
+    <row r="2" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -3517,7 +3558,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="28">
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -3528,7 +3569,7 @@
         <v>1.1499999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="42">
+    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -3539,7 +3580,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="28">
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
@@ -3550,7 +3591,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>71</v>
       </c>
@@ -3566,4 +3607,929 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="S10" sqref="S10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="17" max="17" width="11.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="F1" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="J1" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+    </row>
+    <row r="2" spans="1:17" ht="75" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0.85</v>
+      </c>
+      <c r="B3">
+        <v>0.25</v>
+      </c>
+      <c r="C3">
+        <v>0.85</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>5</v>
+      </c>
+      <c r="H3">
+        <v>0.03</v>
+      </c>
+      <c r="I3">
+        <v>0.03</v>
+      </c>
+      <c r="J3" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="K3">
+        <v>5</v>
+      </c>
+      <c r="L3">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="M3">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="N3" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="O3">
+        <v>5</v>
+      </c>
+      <c r="P3">
+        <v>0.06</v>
+      </c>
+      <c r="Q3">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <v>6</v>
+      </c>
+      <c r="H4">
+        <v>0.03</v>
+      </c>
+      <c r="I4">
+        <v>0.03</v>
+      </c>
+      <c r="J4" s="11"/>
+      <c r="K4">
+        <v>6</v>
+      </c>
+      <c r="L4">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="M4">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="N4" s="11"/>
+      <c r="O4">
+        <v>6</v>
+      </c>
+      <c r="P4">
+        <v>0.06</v>
+      </c>
+      <c r="Q4">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <v>7</v>
+      </c>
+      <c r="H5">
+        <v>0.03</v>
+      </c>
+      <c r="I5">
+        <v>0.03</v>
+      </c>
+      <c r="J5" s="11"/>
+      <c r="K5">
+        <v>7</v>
+      </c>
+      <c r="L5">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="M5">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="N5" s="11"/>
+      <c r="O5">
+        <v>7</v>
+      </c>
+      <c r="P5">
+        <v>0.06</v>
+      </c>
+      <c r="Q5">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <v>8</v>
+      </c>
+      <c r="H6">
+        <v>0.03</v>
+      </c>
+      <c r="I6">
+        <v>0.03</v>
+      </c>
+      <c r="J6" s="11"/>
+      <c r="K6">
+        <v>8</v>
+      </c>
+      <c r="L6">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="M6">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="N6" s="11"/>
+      <c r="O6">
+        <v>8</v>
+      </c>
+      <c r="P6">
+        <v>0.06</v>
+      </c>
+      <c r="Q6">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="G7">
+        <v>9</v>
+      </c>
+      <c r="H7">
+        <v>0.03</v>
+      </c>
+      <c r="I7">
+        <v>0.03</v>
+      </c>
+      <c r="J7" s="11"/>
+      <c r="K7">
+        <v>9</v>
+      </c>
+      <c r="L7">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="M7">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="N7" s="11"/>
+      <c r="O7">
+        <v>9</v>
+      </c>
+      <c r="P7">
+        <v>0.06</v>
+      </c>
+      <c r="Q7">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="G8">
+        <v>10</v>
+      </c>
+      <c r="H8">
+        <v>0.03</v>
+      </c>
+      <c r="I8">
+        <v>0.03</v>
+      </c>
+      <c r="K8">
+        <v>10</v>
+      </c>
+      <c r="L8">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="M8">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="O8">
+        <v>10</v>
+      </c>
+      <c r="P8">
+        <v>0.03</v>
+      </c>
+      <c r="Q8">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="G9">
+        <v>11</v>
+      </c>
+      <c r="H9">
+        <v>0.03</v>
+      </c>
+      <c r="I9">
+        <v>0.03</v>
+      </c>
+      <c r="K9">
+        <v>11</v>
+      </c>
+      <c r="L9">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="M9">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="O9">
+        <v>11</v>
+      </c>
+      <c r="P9">
+        <v>0.03</v>
+      </c>
+      <c r="Q9">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="G10">
+        <v>12</v>
+      </c>
+      <c r="H10">
+        <v>0.03</v>
+      </c>
+      <c r="I10">
+        <v>0.03</v>
+      </c>
+      <c r="K10">
+        <v>12</v>
+      </c>
+      <c r="L10">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="M10">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="O10">
+        <v>12</v>
+      </c>
+      <c r="P10">
+        <v>0.03</v>
+      </c>
+      <c r="Q10">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="G11">
+        <v>13</v>
+      </c>
+      <c r="H11">
+        <v>0.03</v>
+      </c>
+      <c r="I11">
+        <v>0.03</v>
+      </c>
+      <c r="K11">
+        <v>13</v>
+      </c>
+      <c r="L11">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="M11">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="O11">
+        <v>13</v>
+      </c>
+      <c r="P11">
+        <v>0.03</v>
+      </c>
+      <c r="Q11">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="G12">
+        <v>14</v>
+      </c>
+      <c r="H12">
+        <v>0.03</v>
+      </c>
+      <c r="I12">
+        <v>0.03</v>
+      </c>
+      <c r="K12">
+        <v>14</v>
+      </c>
+      <c r="L12">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="M12">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="O12">
+        <v>14</v>
+      </c>
+      <c r="P12">
+        <v>0.03</v>
+      </c>
+      <c r="Q12">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="G13">
+        <v>15</v>
+      </c>
+      <c r="H13">
+        <v>0.03</v>
+      </c>
+      <c r="I13">
+        <v>0.03</v>
+      </c>
+      <c r="K13">
+        <v>15</v>
+      </c>
+      <c r="L13">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="M13">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="O13">
+        <v>15</v>
+      </c>
+      <c r="P13">
+        <v>0.03</v>
+      </c>
+      <c r="Q13">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="G14">
+        <v>16</v>
+      </c>
+      <c r="H14">
+        <v>0.03</v>
+      </c>
+      <c r="I14">
+        <v>0.03</v>
+      </c>
+      <c r="K14">
+        <v>16</v>
+      </c>
+      <c r="L14">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="M14">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="O14">
+        <v>16</v>
+      </c>
+      <c r="P14">
+        <v>0.03</v>
+      </c>
+      <c r="Q14">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="G15">
+        <v>17</v>
+      </c>
+      <c r="H15">
+        <v>0.03</v>
+      </c>
+      <c r="I15">
+        <v>0.03</v>
+      </c>
+      <c r="K15">
+        <v>17</v>
+      </c>
+      <c r="L15">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="M15">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="O15">
+        <v>17</v>
+      </c>
+      <c r="P15">
+        <v>0.03</v>
+      </c>
+      <c r="Q15">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="G16">
+        <v>18</v>
+      </c>
+      <c r="H16">
+        <v>0.03</v>
+      </c>
+      <c r="I16">
+        <v>0.03</v>
+      </c>
+      <c r="K16">
+        <v>18</v>
+      </c>
+      <c r="L16">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="M16">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="O16">
+        <v>18</v>
+      </c>
+      <c r="P16">
+        <v>0.03</v>
+      </c>
+      <c r="Q16">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="17" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="G17">
+        <v>19</v>
+      </c>
+      <c r="H17">
+        <v>0.03</v>
+      </c>
+      <c r="I17">
+        <v>0.03</v>
+      </c>
+      <c r="K17">
+        <v>19</v>
+      </c>
+      <c r="L17">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="M17">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="O17">
+        <v>19</v>
+      </c>
+      <c r="P17">
+        <v>0.03</v>
+      </c>
+      <c r="Q17">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="18" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="G18">
+        <v>20</v>
+      </c>
+      <c r="H18">
+        <v>0.03</v>
+      </c>
+      <c r="I18">
+        <v>0.03</v>
+      </c>
+      <c r="K18">
+        <v>20</v>
+      </c>
+      <c r="L18">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="M18">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="O18">
+        <v>20</v>
+      </c>
+      <c r="P18">
+        <v>0.03</v>
+      </c>
+      <c r="Q18">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="19" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="G19">
+        <v>21</v>
+      </c>
+      <c r="H19">
+        <v>0.03</v>
+      </c>
+      <c r="I19">
+        <v>0.03</v>
+      </c>
+      <c r="K19">
+        <v>21</v>
+      </c>
+      <c r="L19">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="M19">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="O19">
+        <v>21</v>
+      </c>
+      <c r="P19">
+        <v>0.03</v>
+      </c>
+      <c r="Q19">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="20" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="G20">
+        <v>22</v>
+      </c>
+      <c r="H20">
+        <v>0.03</v>
+      </c>
+      <c r="I20">
+        <v>0.03</v>
+      </c>
+      <c r="K20">
+        <v>22</v>
+      </c>
+      <c r="L20">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="M20">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="O20">
+        <v>22</v>
+      </c>
+      <c r="P20">
+        <v>0.03</v>
+      </c>
+      <c r="Q20">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="21" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="G21">
+        <v>23</v>
+      </c>
+      <c r="H21">
+        <v>0.03</v>
+      </c>
+      <c r="I21">
+        <v>0.03</v>
+      </c>
+      <c r="K21">
+        <v>23</v>
+      </c>
+      <c r="L21">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="M21">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="O21">
+        <v>23</v>
+      </c>
+      <c r="P21">
+        <v>0.03</v>
+      </c>
+      <c r="Q21">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="22" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="G22">
+        <v>24</v>
+      </c>
+      <c r="H22">
+        <v>0.03</v>
+      </c>
+      <c r="I22">
+        <v>0.03</v>
+      </c>
+      <c r="K22">
+        <v>24</v>
+      </c>
+      <c r="L22">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="M22">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="O22">
+        <v>24</v>
+      </c>
+      <c r="P22">
+        <v>0.03</v>
+      </c>
+      <c r="Q22">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="23" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="G23">
+        <v>25</v>
+      </c>
+      <c r="H23">
+        <v>0.03</v>
+      </c>
+      <c r="I23">
+        <v>0.03</v>
+      </c>
+      <c r="K23">
+        <v>25</v>
+      </c>
+      <c r="L23">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="M23">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="O23">
+        <v>25</v>
+      </c>
+      <c r="P23">
+        <v>0.03</v>
+      </c>
+      <c r="Q23">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="24" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="G24">
+        <v>26</v>
+      </c>
+      <c r="H24">
+        <v>0.03</v>
+      </c>
+      <c r="I24">
+        <v>0.03</v>
+      </c>
+      <c r="K24">
+        <v>26</v>
+      </c>
+      <c r="L24">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="M24">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="O24">
+        <v>26</v>
+      </c>
+      <c r="P24">
+        <v>0.03</v>
+      </c>
+      <c r="Q24">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="25" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="G25">
+        <v>27</v>
+      </c>
+      <c r="H25">
+        <v>0.03</v>
+      </c>
+      <c r="I25">
+        <v>0.03</v>
+      </c>
+      <c r="K25">
+        <v>27</v>
+      </c>
+      <c r="L25">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="M25">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="O25">
+        <v>27</v>
+      </c>
+      <c r="P25">
+        <v>0.03</v>
+      </c>
+      <c r="Q25">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="26" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="G26">
+        <v>28</v>
+      </c>
+      <c r="H26">
+        <v>0.03</v>
+      </c>
+      <c r="I26">
+        <v>0.03</v>
+      </c>
+      <c r="K26">
+        <v>28</v>
+      </c>
+      <c r="L26">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="M26">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="O26">
+        <v>28</v>
+      </c>
+      <c r="P26">
+        <v>0.03</v>
+      </c>
+      <c r="Q26">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="27" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="G27">
+        <v>29</v>
+      </c>
+      <c r="H27">
+        <v>0.03</v>
+      </c>
+      <c r="I27">
+        <v>0.03</v>
+      </c>
+      <c r="K27">
+        <v>29</v>
+      </c>
+      <c r="L27">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="M27">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="O27">
+        <v>29</v>
+      </c>
+      <c r="P27">
+        <v>0.03</v>
+      </c>
+      <c r="Q27">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="28" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="G28">
+        <v>30</v>
+      </c>
+      <c r="H28">
+        <v>0.03</v>
+      </c>
+      <c r="I28">
+        <v>0.03</v>
+      </c>
+      <c r="K28">
+        <v>30</v>
+      </c>
+      <c r="L28">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="M28">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="O28">
+        <v>30</v>
+      </c>
+      <c r="P28">
+        <v>0.03</v>
+      </c>
+      <c r="Q28">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="29" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="G29">
+        <v>31</v>
+      </c>
+      <c r="H29">
+        <f>SUM(H3:H28)</f>
+        <v>0.78000000000000047</v>
+      </c>
+      <c r="I29">
+        <f>SUM(I3:I28)</f>
+        <v>0.78000000000000047</v>
+      </c>
+      <c r="K29">
+        <v>31</v>
+      </c>
+      <c r="L29">
+        <f>SUM(L3:L28)</f>
+        <v>0.54600000000000015</v>
+      </c>
+      <c r="M29">
+        <f>SUM(M3:M28)</f>
+        <v>1.3020000000000007</v>
+      </c>
+      <c r="O29">
+        <v>31</v>
+      </c>
+      <c r="P29">
+        <f>SUM(P3:P28)</f>
+        <v>0.93000000000000049</v>
+      </c>
+      <c r="Q29">
+        <f>SUM(Q3:Q28)</f>
+        <v>0.26000000000000006</v>
+      </c>
+    </row>
+    <row r="30" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="H30">
+        <f>(H29*3) +I29</f>
+        <v>3.1200000000000019</v>
+      </c>
+      <c r="L30">
+        <f xml:space="preserve"> (3*L29)+ M29</f>
+        <v>2.9400000000000013</v>
+      </c>
+      <c r="P30">
+        <f xml:space="preserve"> (3*P29) +Q29</f>
+        <v>3.0500000000000016</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="J3:J7"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="N3:N7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added translocation table, and updated loader to include it
</commit_message>
<xml_diff>
--- a/Excel Files/life_table.xlsx
+++ b/Excel Files/life_table.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20610" windowHeight="11640" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23220" windowHeight="15320" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="life table" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="Dominance" sheetId="2" r:id="rId4"/>
     <sheet name="Translocation" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" calcOnSave="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="94">
   <si>
     <t>Year</t>
   </si>
@@ -431,6 +431,9 @@
   </si>
   <si>
     <t>Young adult females</t>
+  </si>
+  <si>
+    <t>This table is currently hardcoded</t>
   </si>
 </sst>
 </file>
@@ -563,6 +566,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -581,7 +585,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -903,32 +906,32 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:15" s="2" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:15" s="2" customFormat="1" ht="108" customHeight="1">
+      <c r="A1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11" t="s">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="11"/>
+      <c r="J1" s="12"/>
       <c r="K1" s="2" t="s">
         <v>3</v>
       </c>
@@ -945,18 +948,18 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
       <c r="I2" t="s">
         <v>1</v>
       </c>
@@ -964,7 +967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15">
       <c r="A3" t="s">
         <v>40</v>
       </c>
@@ -1002,8 +1005,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+    <row r="4" spans="1:15">
+      <c r="A4" s="13" t="s">
         <v>41</v>
       </c>
       <c r="B4">
@@ -1022,7 +1025,7 @@
       <c r="G4" s="1">
         <v>0</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="I4" s="12" t="s">
         <v>41</v>
       </c>
       <c r="J4">
@@ -1042,8 +1045,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="12"/>
+    <row r="5" spans="1:15">
+      <c r="A5" s="13"/>
       <c r="B5">
         <v>3</v>
       </c>
@@ -1060,7 +1063,7 @@
       <c r="G5" s="1">
         <v>0</v>
       </c>
-      <c r="I5" s="11"/>
+      <c r="I5" s="12"/>
       <c r="J5">
         <v>3</v>
       </c>
@@ -1078,8 +1081,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="12"/>
+    <row r="6" spans="1:15">
+      <c r="A6" s="13"/>
       <c r="B6">
         <v>4</v>
       </c>
@@ -1096,7 +1099,7 @@
       <c r="G6" s="1">
         <v>0</v>
       </c>
-      <c r="I6" s="11"/>
+      <c r="I6" s="12"/>
       <c r="J6">
         <v>4</v>
       </c>
@@ -1114,8 +1117,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+    <row r="7" spans="1:15" ht="15" customHeight="1">
+      <c r="A7" s="12" t="s">
         <v>42</v>
       </c>
       <c r="B7">
@@ -1135,7 +1138,7 @@
         <f xml:space="preserve"> E7*F7</f>
         <v>97.76</v>
       </c>
-      <c r="I7" s="11" t="s">
+      <c r="I7" s="12" t="s">
         <v>44</v>
       </c>
       <c r="J7">
@@ -1155,8 +1158,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
+    <row r="8" spans="1:15">
+      <c r="A8" s="12"/>
       <c r="B8">
         <v>6</v>
       </c>
@@ -1174,7 +1177,7 @@
         <f t="shared" ref="G8:G32" si="3" xml:space="preserve"> E8*F8</f>
         <v>95.8048</v>
       </c>
-      <c r="I8" s="11"/>
+      <c r="I8" s="12"/>
       <c r="J8">
         <v>6</v>
       </c>
@@ -1192,8 +1195,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
+    <row r="9" spans="1:15">
+      <c r="A9" s="12"/>
       <c r="B9">
         <v>7</v>
       </c>
@@ -1211,7 +1214,7 @@
         <f t="shared" si="3"/>
         <v>93.888704000000004</v>
       </c>
-      <c r="I9" s="11" t="s">
+      <c r="I9" s="12" t="s">
         <v>43</v>
       </c>
       <c r="J9">
@@ -1231,8 +1234,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
+    <row r="10" spans="1:15">
+      <c r="A10" s="12"/>
       <c r="B10">
         <v>8</v>
       </c>
@@ -1250,7 +1253,7 @@
         <f t="shared" si="3"/>
         <v>92.010929920000009</v>
       </c>
-      <c r="I10" s="11"/>
+      <c r="I10" s="12"/>
       <c r="J10">
         <v>8</v>
       </c>
@@ -1268,8 +1271,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
+    <row r="11" spans="1:15">
+      <c r="A11" s="12"/>
       <c r="B11">
         <v>9</v>
       </c>
@@ -1287,7 +1290,7 @@
         <f t="shared" si="3"/>
         <v>90.17071132160001</v>
       </c>
-      <c r="I11" s="11"/>
+      <c r="I11" s="12"/>
       <c r="J11">
         <v>9</v>
       </c>
@@ -1305,8 +1308,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
+    <row r="12" spans="1:15">
+      <c r="A12" s="12" t="s">
         <v>45</v>
       </c>
       <c r="B12">
@@ -1326,7 +1329,7 @@
         <f t="shared" si="3"/>
         <v>106.04075651420162</v>
       </c>
-      <c r="I12" s="11" t="s">
+      <c r="I12" s="12" t="s">
         <v>45</v>
       </c>
       <c r="J12">
@@ -1346,8 +1349,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
+    <row r="13" spans="1:15">
+      <c r="A13" s="12"/>
       <c r="B13">
         <v>11</v>
       </c>
@@ -1365,7 +1368,7 @@
         <f t="shared" si="3"/>
         <v>103.38973760134657</v>
       </c>
-      <c r="I13" s="11"/>
+      <c r="I13" s="12"/>
       <c r="J13">
         <v>11</v>
       </c>
@@ -1383,8 +1386,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="11"/>
+    <row r="14" spans="1:15">
+      <c r="A14" s="12"/>
       <c r="B14">
         <v>12</v>
       </c>
@@ -1402,7 +1405,7 @@
         <f t="shared" si="3"/>
         <v>100.80499416131291</v>
       </c>
-      <c r="I14" s="11"/>
+      <c r="I14" s="12"/>
       <c r="J14">
         <v>12</v>
       </c>
@@ -1420,8 +1423,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="11"/>
+    <row r="15" spans="1:15">
+      <c r="A15" s="12"/>
       <c r="B15">
         <v>13</v>
       </c>
@@ -1439,7 +1442,7 @@
         <f t="shared" si="3"/>
         <v>98.284869307280076</v>
       </c>
-      <c r="I15" s="11"/>
+      <c r="I15" s="12"/>
       <c r="J15">
         <v>13</v>
       </c>
@@ -1457,8 +1460,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
+    <row r="16" spans="1:15">
+      <c r="A16" s="12"/>
       <c r="B16">
         <v>14</v>
       </c>
@@ -1476,7 +1479,7 @@
         <f t="shared" si="3"/>
         <v>95.827747574598078</v>
       </c>
-      <c r="I16" s="11"/>
+      <c r="I16" s="12"/>
       <c r="J16">
         <v>14</v>
       </c>
@@ -1494,8 +1497,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
+    <row r="17" spans="1:15">
+      <c r="A17" s="12" t="s">
         <v>46</v>
       </c>
       <c r="B17">
@@ -1515,7 +1518,7 @@
         <f t="shared" si="3"/>
         <v>109.0040628661053</v>
       </c>
-      <c r="I17" s="11" t="s">
+      <c r="I17" s="12" t="s">
         <v>46</v>
       </c>
       <c r="J17">
@@ -1535,8 +1538,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="11"/>
+    <row r="18" spans="1:15">
+      <c r="A18" s="12"/>
       <c r="B18">
         <v>16</v>
       </c>
@@ -1554,7 +1557,7 @@
         <f t="shared" si="3"/>
         <v>105.73394098012214</v>
       </c>
-      <c r="I18" s="11"/>
+      <c r="I18" s="12"/>
       <c r="J18">
         <v>16</v>
       </c>
@@ -1572,8 +1575,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
+    <row r="19" spans="1:15">
+      <c r="A19" s="12"/>
       <c r="B19">
         <v>17</v>
       </c>
@@ -1591,7 +1594,7 @@
         <f t="shared" si="3"/>
         <v>102.56192275071849</v>
       </c>
-      <c r="I19" s="11"/>
+      <c r="I19" s="12"/>
       <c r="J19">
         <v>17</v>
       </c>
@@ -1609,8 +1612,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="11"/>
+    <row r="20" spans="1:15">
+      <c r="A20" s="12"/>
       <c r="B20">
         <v>18</v>
       </c>
@@ -1628,7 +1631,7 @@
         <f t="shared" si="3"/>
         <v>99.485065068196931</v>
       </c>
-      <c r="I20" s="11"/>
+      <c r="I20" s="12"/>
       <c r="J20">
         <v>18</v>
       </c>
@@ -1646,8 +1649,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="11"/>
+    <row r="21" spans="1:15">
+      <c r="A21" s="12"/>
       <c r="B21">
         <v>19</v>
       </c>
@@ -1665,7 +1668,7 @@
         <f t="shared" si="3"/>
         <v>96.500513116151041</v>
       </c>
-      <c r="I21" s="11"/>
+      <c r="I21" s="12"/>
       <c r="J21">
         <v>19</v>
       </c>
@@ -1683,8 +1686,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="11" t="s">
+    <row r="22" spans="1:15">
+      <c r="A22" s="12" t="s">
         <v>9</v>
       </c>
       <c r="B22">
@@ -1704,7 +1707,7 @@
         <f t="shared" si="3"/>
         <v>100.29160470285697</v>
       </c>
-      <c r="I22" s="11" t="s">
+      <c r="I22" s="12" t="s">
         <v>9</v>
       </c>
       <c r="J22">
@@ -1724,8 +1727,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="11"/>
+    <row r="23" spans="1:15">
+      <c r="A23" s="12"/>
       <c r="B23">
         <v>21</v>
       </c>
@@ -1743,7 +1746,7 @@
         <f t="shared" si="3"/>
         <v>99.288688655828395</v>
       </c>
-      <c r="I23" s="11"/>
+      <c r="I23" s="12"/>
       <c r="J23">
         <v>21</v>
       </c>
@@ -1761,8 +1764,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="11"/>
+    <row r="24" spans="1:15">
+      <c r="A24" s="12"/>
       <c r="B24">
         <v>22</v>
       </c>
@@ -1780,7 +1783,7 @@
         <f t="shared" si="3"/>
         <v>98.295801769270113</v>
       </c>
-      <c r="I24" s="11"/>
+      <c r="I24" s="12"/>
       <c r="J24">
         <v>22</v>
       </c>
@@ -1798,8 +1801,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="11"/>
+    <row r="25" spans="1:15">
+      <c r="A25" s="12"/>
       <c r="B25">
         <v>23</v>
       </c>
@@ -1817,7 +1820,7 @@
         <f t="shared" si="3"/>
         <v>97.312843751577418</v>
       </c>
-      <c r="I25" s="11"/>
+      <c r="I25" s="12"/>
       <c r="J25">
         <v>23</v>
       </c>
@@ -1835,8 +1838,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" s="11"/>
+    <row r="26" spans="1:15">
+      <c r="A26" s="12"/>
       <c r="B26">
         <v>24</v>
       </c>
@@ -1854,7 +1857,7 @@
         <f t="shared" si="3"/>
         <v>96.339715314061635</v>
       </c>
-      <c r="I26" s="11"/>
+      <c r="I26" s="12"/>
       <c r="J26">
         <v>24</v>
       </c>
@@ -1872,8 +1875,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" s="11" t="s">
+    <row r="27" spans="1:15">
+      <c r="A27" s="12" t="s">
         <v>19</v>
       </c>
       <c r="B27">
@@ -1893,7 +1896,7 @@
         <f t="shared" si="3"/>
         <v>25.433684842912271</v>
       </c>
-      <c r="I27" s="11" t="s">
+      <c r="I27" s="12" t="s">
         <v>19</v>
       </c>
       <c r="J27">
@@ -1913,8 +1916,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="11"/>
+    <row r="28" spans="1:15">
+      <c r="A28" s="12"/>
       <c r="B28">
         <v>26</v>
       </c>
@@ -1932,7 +1935,7 @@
         <f t="shared" si="3"/>
         <v>17.803579390038589</v>
       </c>
-      <c r="I28" s="11"/>
+      <c r="I28" s="12"/>
       <c r="J28">
         <v>26</v>
       </c>
@@ -1950,8 +1953,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="11"/>
+    <row r="29" spans="1:15">
+      <c r="A29" s="12"/>
       <c r="B29">
         <v>27</v>
       </c>
@@ -1969,7 +1972,7 @@
         <f t="shared" si="3"/>
         <v>12.462505573027014</v>
       </c>
-      <c r="I29" s="11"/>
+      <c r="I29" s="12"/>
       <c r="J29">
         <v>27</v>
       </c>
@@ -1987,8 +1990,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="11"/>
+    <row r="30" spans="1:15">
+      <c r="A30" s="12"/>
       <c r="B30">
         <v>28</v>
       </c>
@@ -2006,7 +2009,7 @@
         <f t="shared" si="3"/>
         <v>8.7237539011189096</v>
       </c>
-      <c r="I30" s="11"/>
+      <c r="I30" s="12"/>
       <c r="J30">
         <v>28</v>
       </c>
@@ -2024,8 +2027,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="11"/>
+    <row r="31" spans="1:15">
+      <c r="A31" s="12"/>
       <c r="B31">
         <v>29</v>
       </c>
@@ -2043,7 +2046,7 @@
         <f t="shared" si="3"/>
         <v>6.1066277307832371</v>
       </c>
-      <c r="I31" s="11"/>
+      <c r="I31" s="12"/>
       <c r="J31">
         <v>29</v>
       </c>
@@ -2061,8 +2064,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="11"/>
+    <row r="32" spans="1:15">
+      <c r="A32" s="12"/>
       <c r="B32">
         <v>30</v>
       </c>
@@ -2080,7 +2083,7 @@
         <f t="shared" si="3"/>
         <v>4.2746394115482662</v>
       </c>
-      <c r="I32" s="11"/>
+      <c r="I32" s="12"/>
       <c r="J32">
         <v>30</v>
       </c>
@@ -2098,7 +2101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15">
       <c r="A33" s="10"/>
       <c r="B33">
         <v>31</v>
@@ -2132,7 +2135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15">
       <c r="A34" s="10"/>
       <c r="B34">
         <v>32</v>
@@ -2166,7 +2169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15">
       <c r="A35" t="s">
         <v>63</v>
       </c>
@@ -2178,7 +2181,7 @@
         <v>2053.6022002246564</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15">
       <c r="B37" t="s">
         <v>15</v>
       </c>
@@ -2186,7 +2189,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15">
       <c r="B38" t="s">
         <v>16</v>
       </c>
@@ -2218,7 +2221,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15">
       <c r="B39" s="1">
         <f xml:space="preserve"> SUM(F7:F11)</f>
         <v>939.27029048320014</v>
@@ -2268,7 +2271,7 @@
         <v>2422.0282388068249</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15">
       <c r="B40">
         <f t="shared" ref="B40:G40" si="6">(B39/$G$39)</f>
         <v>0.26514252166451985</v>
@@ -2318,7 +2321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15">
       <c r="B41">
         <v>0.26514252166451985</v>
       </c>
@@ -2362,21 +2365,21 @@
         <v>0.99999975799230834</v>
       </c>
     </row>
-    <row r="43" spans="1:15" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="11" t="s">
+    <row r="43" spans="1:15" ht="43.5" customHeight="1">
+      <c r="B43" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="C43" s="11"/>
-      <c r="D43" s="11"/>
-      <c r="E43" s="11"/>
-      <c r="J43" s="11" t="s">
+      <c r="C43" s="12"/>
+      <c r="D43" s="12"/>
+      <c r="E43" s="12"/>
+      <c r="J43" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="K43" s="11"/>
-      <c r="L43" s="11"/>
-      <c r="M43" s="11"/>
-    </row>
-    <row r="44" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="K43" s="12"/>
+      <c r="L43" s="12"/>
+      <c r="M43" s="12"/>
+    </row>
+    <row r="44" spans="1:15" ht="56">
       <c r="B44" s="2" t="s">
         <v>57</v>
       </c>
@@ -2390,7 +2393,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15">
       <c r="B45" t="s">
         <v>54</v>
       </c>
@@ -2404,7 +2407,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15">
       <c r="B46" s="8" t="s">
         <v>50</v>
       </c>
@@ -2418,7 +2421,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15">
       <c r="B47" s="8" t="s">
         <v>51</v>
       </c>
@@ -2432,7 +2435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15">
       <c r="B48" s="8" t="s">
         <v>52</v>
       </c>
@@ -2446,15 +2449,15 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="50" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="11" t="s">
+    <row r="50" spans="2:5" ht="45" customHeight="1">
+      <c r="B50" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="C50" s="11"/>
-      <c r="D50" s="11"/>
-      <c r="E50" s="11"/>
-    </row>
-    <row r="51" spans="2:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="C50" s="12"/>
+      <c r="D50" s="12"/>
+      <c r="E50" s="12"/>
+    </row>
+    <row r="51" spans="2:5" ht="56">
       <c r="B51" s="2" t="s">
         <v>57</v>
       </c>
@@ -2462,7 +2465,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:5">
       <c r="B52" t="s">
         <v>54</v>
       </c>
@@ -2470,7 +2473,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:5">
       <c r="B53" s="8" t="s">
         <v>50</v>
       </c>
@@ -2478,7 +2481,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:5">
       <c r="B54" s="8" t="s">
         <v>51</v>
       </c>
@@ -2486,7 +2489,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:5">
       <c r="B55" s="8" t="s">
         <v>52</v>
       </c>
@@ -2496,13 +2499,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="I12:I16"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="A22:A26"/>
-    <mergeCell ref="A27:A32"/>
-    <mergeCell ref="I27:I32"/>
-    <mergeCell ref="I17:I21"/>
-    <mergeCell ref="I22:I26"/>
     <mergeCell ref="B43:E43"/>
     <mergeCell ref="J43:M43"/>
     <mergeCell ref="B50:E50"/>
@@ -2519,6 +2515,13 @@
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="I7:I8"/>
     <mergeCell ref="I9:I11"/>
+    <mergeCell ref="I12:I16"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="A22:A26"/>
+    <mergeCell ref="A27:A32"/>
+    <mergeCell ref="I27:I32"/>
+    <mergeCell ref="I17:I21"/>
+    <mergeCell ref="I22:I26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2538,30 +2541,30 @@
       <selection activeCell="D2" sqref="D2:G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="4" width="8.85546875" style="2"/>
-    <col min="5" max="5" width="11.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="10.85546875" style="2" customWidth="1"/>
-    <col min="9" max="13" width="8.85546875" style="2"/>
-    <col min="14" max="14" width="14.28515625" style="2" customWidth="1"/>
-    <col min="15" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="4" width="8.83203125" style="2"/>
+    <col min="5" max="5" width="11.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="10.83203125" style="2" customWidth="1"/>
+    <col min="9" max="13" width="8.83203125" style="2"/>
+    <col min="14" max="14" width="14.33203125" style="2" customWidth="1"/>
+    <col min="15" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:18" ht="27" customHeight="1">
+      <c r="A1" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11" t="s">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-    </row>
-    <row r="2" spans="1:18" ht="150" x14ac:dyDescent="0.25">
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+    </row>
+    <row r="2" spans="1:18" ht="112">
       <c r="A2" s="2" t="s">
         <v>23</v>
       </c>
@@ -2587,7 +2590,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18">
       <c r="A3" t="s">
         <v>40</v>
       </c>
@@ -2613,8 +2616,8 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+    <row r="4" spans="1:18">
+      <c r="A4" s="12" t="s">
         <v>41</v>
       </c>
       <c r="B4">
@@ -2639,8 +2642,8 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
+    <row r="5" spans="1:18">
+      <c r="A5" s="12"/>
       <c r="B5">
         <v>3</v>
       </c>
@@ -2663,8 +2666,8 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
+    <row r="6" spans="1:18">
+      <c r="A6" s="12"/>
       <c r="B6">
         <v>4</v>
       </c>
@@ -2684,8 +2687,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+    <row r="7" spans="1:18" ht="15" customHeight="1">
+      <c r="A7" s="12" t="s">
         <v>44</v>
       </c>
       <c r="B7">
@@ -2707,8 +2710,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
+    <row r="8" spans="1:18">
+      <c r="A8" s="12"/>
       <c r="B8">
         <v>6</v>
       </c>
@@ -2728,8 +2731,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+    <row r="9" spans="1:18" ht="15" customHeight="1">
+      <c r="A9" s="12" t="s">
         <v>43</v>
       </c>
       <c r="B9">
@@ -2751,8 +2754,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
+    <row r="10" spans="1:18">
+      <c r="A10" s="12"/>
       <c r="B10">
         <v>8</v>
       </c>
@@ -2772,8 +2775,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
+    <row r="11" spans="1:18">
+      <c r="A11" s="12"/>
       <c r="B11">
         <v>9</v>
       </c>
@@ -2793,8 +2796,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
+    <row r="12" spans="1:18" ht="15" customHeight="1">
+      <c r="A12" s="12" t="s">
         <v>45</v>
       </c>
       <c r="B12">
@@ -2816,8 +2819,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
+    <row r="13" spans="1:18">
+      <c r="A13" s="12"/>
       <c r="B13">
         <v>11</v>
       </c>
@@ -2837,8 +2840,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" s="11"/>
+    <row r="14" spans="1:18">
+      <c r="A14" s="12"/>
       <c r="B14">
         <v>12</v>
       </c>
@@ -2858,8 +2861,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="11"/>
+    <row r="15" spans="1:18">
+      <c r="A15" s="12"/>
       <c r="B15">
         <v>13</v>
       </c>
@@ -2879,8 +2882,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
+    <row r="16" spans="1:18">
+      <c r="A16" s="12"/>
       <c r="B16">
         <v>14</v>
       </c>
@@ -2900,8 +2903,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
+    <row r="17" spans="1:7" ht="15" customHeight="1">
+      <c r="A17" s="12" t="s">
         <v>46</v>
       </c>
       <c r="B17">
@@ -2923,8 +2926,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="11"/>
+    <row r="18" spans="1:7">
+      <c r="A18" s="12"/>
       <c r="B18">
         <v>16</v>
       </c>
@@ -2944,8 +2947,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
+    <row r="19" spans="1:7">
+      <c r="A19" s="12"/>
       <c r="B19">
         <v>17</v>
       </c>
@@ -2965,8 +2968,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="11"/>
+    <row r="20" spans="1:7">
+      <c r="A20" s="12"/>
       <c r="B20">
         <v>18</v>
       </c>
@@ -2986,8 +2989,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="11"/>
+    <row r="21" spans="1:7">
+      <c r="A21" s="12"/>
       <c r="B21">
         <v>19</v>
       </c>
@@ -3007,8 +3010,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="11" t="s">
+    <row r="22" spans="1:7">
+      <c r="A22" s="12" t="s">
         <v>9</v>
       </c>
       <c r="B22">
@@ -3030,8 +3033,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="11"/>
+    <row r="23" spans="1:7">
+      <c r="A23" s="12"/>
       <c r="B23">
         <v>21</v>
       </c>
@@ -3051,8 +3054,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="11"/>
+    <row r="24" spans="1:7">
+      <c r="A24" s="12"/>
       <c r="B24">
         <v>22</v>
       </c>
@@ -3072,8 +3075,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="11"/>
+    <row r="25" spans="1:7">
+      <c r="A25" s="12"/>
       <c r="B25">
         <v>23</v>
       </c>
@@ -3093,8 +3096,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="11"/>
+    <row r="26" spans="1:7">
+      <c r="A26" s="12"/>
       <c r="B26">
         <v>24</v>
       </c>
@@ -3114,8 +3117,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="11" t="s">
+    <row r="27" spans="1:7">
+      <c r="A27" s="12" t="s">
         <v>19</v>
       </c>
       <c r="B27">
@@ -3137,8 +3140,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="11"/>
+    <row r="28" spans="1:7">
+      <c r="A28" s="12"/>
       <c r="B28">
         <v>26</v>
       </c>
@@ -3158,8 +3161,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="11"/>
+    <row r="29" spans="1:7">
+      <c r="A29" s="12"/>
       <c r="B29">
         <v>27</v>
       </c>
@@ -3179,8 +3182,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="11"/>
+    <row r="30" spans="1:7">
+      <c r="A30" s="12"/>
       <c r="B30">
         <v>28</v>
       </c>
@@ -3200,8 +3203,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="11"/>
+    <row r="31" spans="1:7">
+      <c r="A31" s="12"/>
       <c r="B31">
         <v>29</v>
       </c>
@@ -3221,8 +3224,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="11"/>
+    <row r="32" spans="1:7">
+      <c r="A32" s="12"/>
       <c r="B32">
         <v>30</v>
       </c>
@@ -3242,40 +3245,40 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" ht="27" customHeight="1">
       <c r="A33" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B33" s="11" t="s">
+      <c r="B33" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="C33" s="11"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="11"/>
-      <c r="F33" s="11"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="11"/>
-    </row>
-    <row r="34" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+      <c r="C33" s="12"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="12"/>
+    </row>
+    <row r="34" spans="1:14" ht="56">
       <c r="C34" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D34" s="11" t="s">
+      <c r="D34" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="E34" s="11"/>
+      <c r="E34" s="12"/>
       <c r="F34" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="L34" s="11" t="s">
+      <c r="L34" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="M34" s="11"/>
+      <c r="M34" s="12"/>
       <c r="N34" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14">
       <c r="C35" s="2" t="s">
         <v>68</v>
       </c>
@@ -3293,7 +3296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14">
       <c r="C36" s="2">
         <v>1</v>
       </c>
@@ -3310,7 +3313,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14">
       <c r="C37" s="2">
         <v>2</v>
       </c>
@@ -3327,7 +3330,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14">
       <c r="C38" s="2">
         <v>3</v>
       </c>
@@ -3344,14 +3347,19 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14">
       <c r="E39" s="6"/>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14">
       <c r="E40" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="D34:E34"/>
     <mergeCell ref="L34:M34"/>
     <mergeCell ref="A22:A26"/>
     <mergeCell ref="A27:A32"/>
@@ -3359,11 +3367,6 @@
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="A9:A11"/>
     <mergeCell ref="B33:H33"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="A12:A16"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="D34:E34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -3383,28 +3386,28 @@
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" style="2"/>
-    <col min="3" max="3" width="16.85546875" style="2" customWidth="1"/>
-    <col min="4" max="5" width="8.85546875" style="2"/>
-    <col min="6" max="6" width="15.28515625" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="26.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" style="2"/>
+    <col min="3" max="3" width="16.83203125" style="2" customWidth="1"/>
+    <col min="4" max="5" width="8.83203125" style="2"/>
+    <col min="6" max="6" width="15.33203125" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:7" ht="49.5" customHeight="1">
+      <c r="A1" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="2" t="s">
         <v>33</v>
       </c>
@@ -3412,7 +3415,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="78" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="78" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>69</v>
       </c>
@@ -3426,7 +3429,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="60" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>70</v>
       </c>
@@ -3440,7 +3443,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="42">
       <c r="A5" s="2" t="s">
         <v>38</v>
       </c>
@@ -3452,7 +3455,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="28">
       <c r="A6" s="2" t="s">
         <v>34</v>
       </c>
@@ -3463,7 +3466,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="E7" s="2">
         <v>3</v>
       </c>
@@ -3471,42 +3474,42 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="28">
       <c r="A9" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="42">
       <c r="A10" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="28">
       <c r="A11" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="28">
       <c r="A14" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="28">
       <c r="A15" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="28">
       <c r="A16" s="2" t="s">
         <v>79</v>
       </c>
@@ -3533,21 +3536,21 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:5">
+      <c r="A1" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="15"/>
-    </row>
-    <row r="2" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="16"/>
+    </row>
+    <row r="2" spans="1:5" ht="56">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -3558,7 +3561,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="28">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -3569,7 +3572,7 @@
         <v>1.1499999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="42">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -3580,7 +3583,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="28">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
@@ -3591,7 +3594,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="9" t="s">
         <v>71</v>
       </c>
@@ -3613,39 +3616,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="S10" sqref="S10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="17" max="17" width="11.7109375" customWidth="1"/>
+    <col min="17" max="17" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:17">
+      <c r="A1" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="F1" s="17" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="F1" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="J1" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16" t="s">
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="O1" s="16"/>
-      <c r="P1" s="16"/>
-      <c r="Q1" s="16"/>
-    </row>
-    <row r="2" spans="1:17" ht="75" x14ac:dyDescent="0.25">
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+    </row>
+    <row r="2" spans="1:17" ht="70">
       <c r="A2" s="2" t="s">
         <v>81</v>
       </c>
@@ -3692,7 +3695,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17">
       <c r="A3">
         <v>0.85</v>
       </c>
@@ -3714,7 +3717,7 @@
       <c r="I3">
         <v>0.03</v>
       </c>
-      <c r="J3" s="11" t="s">
+      <c r="J3" s="12" t="s">
         <v>89</v>
       </c>
       <c r="K3">
@@ -3726,7 +3729,7 @@
       <c r="M3">
         <v>8.4000000000000005E-2</v>
       </c>
-      <c r="N3" s="11" t="s">
+      <c r="N3" s="12" t="s">
         <v>92</v>
       </c>
       <c r="O3">
@@ -3739,7 +3742,10 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17">
+      <c r="A4" t="s">
+        <v>93</v>
+      </c>
       <c r="G4">
         <v>6</v>
       </c>
@@ -3749,7 +3755,7 @@
       <c r="I4">
         <v>0.03</v>
       </c>
-      <c r="J4" s="11"/>
+      <c r="J4" s="12"/>
       <c r="K4">
         <v>6</v>
       </c>
@@ -3759,7 +3765,7 @@
       <c r="M4">
         <v>8.4000000000000005E-2</v>
       </c>
-      <c r="N4" s="11"/>
+      <c r="N4" s="12"/>
       <c r="O4">
         <v>6</v>
       </c>
@@ -3770,7 +3776,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17">
       <c r="G5">
         <v>7</v>
       </c>
@@ -3780,7 +3786,7 @@
       <c r="I5">
         <v>0.03</v>
       </c>
-      <c r="J5" s="11"/>
+      <c r="J5" s="12"/>
       <c r="K5">
         <v>7</v>
       </c>
@@ -3790,7 +3796,7 @@
       <c r="M5">
         <v>8.4000000000000005E-2</v>
       </c>
-      <c r="N5" s="11"/>
+      <c r="N5" s="12"/>
       <c r="O5">
         <v>7</v>
       </c>
@@ -3801,7 +3807,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17">
       <c r="G6">
         <v>8</v>
       </c>
@@ -3811,7 +3817,7 @@
       <c r="I6">
         <v>0.03</v>
       </c>
-      <c r="J6" s="11"/>
+      <c r="J6" s="12"/>
       <c r="K6">
         <v>8</v>
       </c>
@@ -3821,7 +3827,7 @@
       <c r="M6">
         <v>8.4000000000000005E-2</v>
       </c>
-      <c r="N6" s="11"/>
+      <c r="N6" s="12"/>
       <c r="O6">
         <v>8</v>
       </c>
@@ -3832,7 +3838,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17">
       <c r="G7">
         <v>9</v>
       </c>
@@ -3842,7 +3848,7 @@
       <c r="I7">
         <v>0.03</v>
       </c>
-      <c r="J7" s="11"/>
+      <c r="J7" s="12"/>
       <c r="K7">
         <v>9</v>
       </c>
@@ -3852,7 +3858,7 @@
       <c r="M7">
         <v>8.4000000000000005E-2</v>
       </c>
-      <c r="N7" s="11"/>
+      <c r="N7" s="12"/>
       <c r="O7">
         <v>9</v>
       </c>
@@ -3863,7 +3869,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17">
       <c r="G8">
         <v>10</v>
       </c>
@@ -3892,7 +3898,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17">
       <c r="G9">
         <v>11</v>
       </c>
@@ -3921,7 +3927,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17">
       <c r="G10">
         <v>12</v>
       </c>
@@ -3950,7 +3956,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17">
       <c r="G11">
         <v>13</v>
       </c>
@@ -3979,7 +3985,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17">
       <c r="G12">
         <v>14</v>
       </c>
@@ -4008,7 +4014,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17">
       <c r="G13">
         <v>15</v>
       </c>
@@ -4037,7 +4043,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17">
       <c r="G14">
         <v>16</v>
       </c>
@@ -4066,7 +4072,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17">
       <c r="G15">
         <v>17</v>
       </c>
@@ -4095,7 +4101,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17">
       <c r="G16">
         <v>18</v>
       </c>
@@ -4124,7 +4130,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="17" spans="7:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="7:17">
       <c r="G17">
         <v>19</v>
       </c>
@@ -4153,7 +4159,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="18" spans="7:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="7:17">
       <c r="G18">
         <v>20</v>
       </c>
@@ -4182,7 +4188,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="19" spans="7:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="7:17">
       <c r="G19">
         <v>21</v>
       </c>
@@ -4211,7 +4217,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="20" spans="7:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="7:17">
       <c r="G20">
         <v>22</v>
       </c>
@@ -4240,7 +4246,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="21" spans="7:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="7:17">
       <c r="G21">
         <v>23</v>
       </c>
@@ -4269,7 +4275,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="22" spans="7:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="7:17">
       <c r="G22">
         <v>24</v>
       </c>
@@ -4298,7 +4304,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="23" spans="7:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="7:17">
       <c r="G23">
         <v>25</v>
       </c>
@@ -4327,7 +4333,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="24" spans="7:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="7:17">
       <c r="G24">
         <v>26</v>
       </c>
@@ -4356,7 +4362,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="25" spans="7:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="7:17">
       <c r="G25">
         <v>27</v>
       </c>
@@ -4385,7 +4391,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="26" spans="7:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="7:17">
       <c r="G26">
         <v>28</v>
       </c>
@@ -4414,7 +4420,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="27" spans="7:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="7:17">
       <c r="G27">
         <v>29</v>
       </c>
@@ -4443,7 +4449,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="28" spans="7:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="7:17">
       <c r="G28">
         <v>30</v>
       </c>
@@ -4472,7 +4478,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="29" spans="7:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="7:17">
       <c r="G29">
         <v>31</v>
       </c>
@@ -4507,7 +4513,10 @@
         <v>0.26000000000000006</v>
       </c>
     </row>
-    <row r="30" spans="7:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="7:17">
+      <c r="G30" t="s">
+        <v>63</v>
+      </c>
       <c r="H30">
         <f>(H29*3) +I29</f>
         <v>3.1200000000000019</v>
@@ -4530,6 +4539,11 @@
     <mergeCell ref="N3:N7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>